<commit_message>
Day 9 | Final
</commit_message>
<xml_diff>
--- a/Batch/15/In_Class/Day_8.xlsx
+++ b/Batch/15/In_Class/Day_8.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Acciojob\Modules\Excel\Batch\15\In_Class\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FFD6DD-595F-43E9-911C-D67157A4664F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B49EAC90-EED0-4B3A-86F0-7F5F36F03027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="30" windowWidth="29040" windowHeight="15720" tabRatio="741" activeTab="9" xr2:uid="{E4FAC7A2-194B-4DBE-ACA1-546198A701A9}"/>
+    <workbookView xWindow="-28920" yWindow="30" windowWidth="29040" windowHeight="15720" tabRatio="741" activeTab="1" xr2:uid="{E4FAC7A2-194B-4DBE-ACA1-546198A701A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Errors" sheetId="7" r:id="rId1"/>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4422" uniqueCount="903">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4456" uniqueCount="933">
   <si>
     <t>Intro To excel</t>
   </si>
@@ -15561,6 +15561,96 @@
   </si>
   <si>
     <t>12-31-2025</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Srinath</t>
+  </si>
+  <si>
+    <t>Bhatia</t>
+  </si>
+  <si>
+    <t>Abdul</t>
+  </si>
+  <si>
+    <t>Priyanshu</t>
+  </si>
+  <si>
+    <t>Ahmad</t>
+  </si>
+  <si>
+    <t>Vaidwan</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Anuj</t>
+  </si>
+  <si>
+    <t>Rahman</t>
+  </si>
+  <si>
+    <t>Verma</t>
+  </si>
+  <si>
+    <t>Vishnoi</t>
+  </si>
+  <si>
+    <t>Ak.95</t>
+  </si>
+  <si>
+    <t>Soabhagya</t>
+  </si>
+  <si>
+    <t>Kumar</t>
+  </si>
+  <si>
+    <t>Afsar4</t>
+  </si>
+  <si>
+    <t>Tcs</t>
+  </si>
+  <si>
+    <t>Nestle</t>
+  </si>
+  <si>
+    <t>Google</t>
+  </si>
+  <si>
+    <t>Aramco</t>
+  </si>
+  <si>
+    <t>Genpact</t>
+  </si>
+  <si>
+    <t>Pg</t>
+  </si>
+  <si>
+    <t>Ahead</t>
+  </si>
+  <si>
+    <t>Ecl</t>
+  </si>
+  <si>
+    <t>Gmail</t>
+  </si>
+  <si>
+    <t>Vishu</t>
+  </si>
+  <si>
+    <t>Arpit</t>
+  </si>
+  <si>
+    <t>Tanya</t>
+  </si>
+  <si>
+    <t>Babblu</t>
+  </si>
+  <si>
+    <t>Arzoo</t>
   </si>
 </sst>
 </file>
@@ -15730,15 +15820,6 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -15750,6 +15831,15 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -15789,8 +15879,8 @@
       <xdr:row>15</xdr:row>
       <xdr:rowOff>10181</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="4" name="Ink 3">
@@ -15809,7 +15899,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="4" name="Ink 3">
@@ -15854,8 +15944,8 @@
       <xdr:row>14</xdr:row>
       <xdr:rowOff>178894</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="5" name="Ink 4">
@@ -15874,7 +15964,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="5" name="Ink 4">
@@ -15919,8 +16009,8 @@
       <xdr:row>14</xdr:row>
       <xdr:rowOff>179974</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="6" name="Ink 5">
@@ -15939,7 +16029,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="6" name="Ink 5">
@@ -15973,19 +16063,19 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>601423</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>56854</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>94835</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>107103</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="22" name="Ink 21">
@@ -16004,7 +16094,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="22" name="Ink 21">
@@ -16038,19 +16128,19 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>277993</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>53892</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>373393</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>30701</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="23" name="Ink 22">
@@ -16069,7 +16159,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="23" name="Ink 22">
@@ -16114,8 +16204,8 @@
       <xdr:row>17</xdr:row>
       <xdr:rowOff>9632</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="36" name="Ink 35">
@@ -16134,7 +16224,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="36" name="Ink 35">
@@ -16179,8 +16269,8 @@
       <xdr:row>17</xdr:row>
       <xdr:rowOff>95394</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="44" name="Ink 43">
@@ -16199,7 +16289,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="44" name="Ink 43">
@@ -16244,8 +16334,8 @@
       <xdr:row>17</xdr:row>
       <xdr:rowOff>28794</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="48" name="Ink 47">
@@ -16264,7 +16354,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="48" name="Ink 47">
@@ -16309,8 +16399,8 @@
       <xdr:row>17</xdr:row>
       <xdr:rowOff>18714</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId17">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="50" name="Ink 49">
@@ -16329,7 +16419,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="50" name="Ink 49">
@@ -16374,8 +16464,8 @@
       <xdr:row>18</xdr:row>
       <xdr:rowOff>112800</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId19">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="71" name="Ink 70">
@@ -16394,7 +16484,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="71" name="Ink 70">
@@ -16439,8 +16529,8 @@
       <xdr:row>18</xdr:row>
       <xdr:rowOff>84360</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId21">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="80" name="Ink 79">
@@ -16459,7 +16549,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="80" name="Ink 79">
@@ -16504,8 +16594,8 @@
       <xdr:row>13</xdr:row>
       <xdr:rowOff>163926</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId23">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="81" name="Ink 80">
@@ -16524,7 +16614,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="81" name="Ink 80">
@@ -16569,8 +16659,8 @@
       <xdr:row>14</xdr:row>
       <xdr:rowOff>252</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId25">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="82" name="Ink 81">
@@ -16589,7 +16679,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="82" name="Ink 81">
@@ -16634,8 +16724,8 @@
       <xdr:row>13</xdr:row>
       <xdr:rowOff>173646</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId27">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="83" name="Ink 82">
@@ -16654,7 +16744,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="83" name="Ink 82">
@@ -16699,8 +16789,8 @@
       <xdr:row>15</xdr:row>
       <xdr:rowOff>66341</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId29">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="92" name="Ink 91">
@@ -16719,7 +16809,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="92" name="Ink 91">
@@ -16764,8 +16854,8 @@
       <xdr:row>15</xdr:row>
       <xdr:rowOff>78221</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId31">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="93" name="Ink 92">
@@ -16784,7 +16874,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="93" name="Ink 92">
@@ -16829,8 +16919,8 @@
       <xdr:row>15</xdr:row>
       <xdr:rowOff>87859</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId33">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="94" name="Ink 93">
@@ -16849,7 +16939,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="94" name="Ink 93">
@@ -16894,8 +16984,8 @@
       <xdr:row>15</xdr:row>
       <xdr:rowOff>66619</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId35">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="100" name="Ink 99">
@@ -16914,7 +17004,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="100" name="Ink 99">
@@ -16959,8 +17049,8 @@
       <xdr:row>15</xdr:row>
       <xdr:rowOff>93783</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId37">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="102" name="Ink 101">
@@ -16979,7 +17069,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="102" name="Ink 101">
@@ -17024,8 +17114,8 @@
       <xdr:row>19</xdr:row>
       <xdr:rowOff>178724</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId39">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="113" name="Ink 112">
@@ -17044,7 +17134,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="113" name="Ink 112">
@@ -17089,8 +17179,8 @@
       <xdr:row>20</xdr:row>
       <xdr:rowOff>17375</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId41">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="118" name="Ink 117">
@@ -17109,7 +17199,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="118" name="Ink 117">
@@ -17154,8 +17244,8 @@
       <xdr:row>20</xdr:row>
       <xdr:rowOff>17293</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId43">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="123" name="Ink 122">
@@ -17174,7 +17264,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="123" name="Ink 122">
@@ -17219,8 +17309,8 @@
       <xdr:row>19</xdr:row>
       <xdr:rowOff>162246</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId45">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="129" name="Ink 128">
@@ -17239,7 +17329,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="129" name="Ink 128">
@@ -17284,8 +17374,8 @@
       <xdr:row>21</xdr:row>
       <xdr:rowOff>86457</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId47">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="138" name="Ink 137">
@@ -17304,7 +17394,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="138" name="Ink 137">
@@ -17338,19 +17428,19 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>383113</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>152634</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>380291</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>54859</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId49">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="160" name="Ink 159">
@@ -17369,7 +17459,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="160" name="Ink 159">
@@ -17414,8 +17504,8 @@
       <xdr:row>28</xdr:row>
       <xdr:rowOff>64605</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId51">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="199" name="Ink 198">
@@ -17434,7 +17524,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="199" name="Ink 198">
@@ -17880,8 +17970,8 @@
       <xdr:row>70</xdr:row>
       <xdr:rowOff>69672</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="14" name="Ink 13">
@@ -17900,7 +17990,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="14" name="Ink 13">
@@ -17945,8 +18035,8 @@
       <xdr:row>76</xdr:row>
       <xdr:rowOff>21915</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="32" name="Ink 31">
@@ -17965,7 +18055,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="32" name="Ink 31">
@@ -18010,8 +18100,8 @@
       <xdr:row>72</xdr:row>
       <xdr:rowOff>179327</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="35" name="Ink 34">
@@ -18030,7 +18120,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="35" name="Ink 34">
@@ -18075,8 +18165,8 @@
       <xdr:row>76</xdr:row>
       <xdr:rowOff>49913</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId16">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="48" name="Ink 47">
@@ -18095,7 +18185,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="48" name="Ink 47">
@@ -18140,8 +18230,8 @@
       <xdr:row>79</xdr:row>
       <xdr:rowOff>171794</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId18">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="82" name="Ink 81">
@@ -18160,7 +18250,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="82" name="Ink 81">
@@ -18205,8 +18295,8 @@
       <xdr:row>72</xdr:row>
       <xdr:rowOff>55564</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId20">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="83" name="Ink 82">
@@ -18225,7 +18315,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="83" name="Ink 82">
@@ -18270,8 +18360,8 @@
       <xdr:row>83</xdr:row>
       <xdr:rowOff>106382</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId22">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="95" name="Ink 94">
@@ -18290,7 +18380,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="95" name="Ink 94">
@@ -18335,8 +18425,8 @@
       <xdr:row>85</xdr:row>
       <xdr:rowOff>64673</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId24">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="115" name="Ink 114">
@@ -18355,7 +18445,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="115" name="Ink 114">
@@ -18405,8 +18495,8 @@
       <xdr:row>2</xdr:row>
       <xdr:rowOff>102528</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="2" name="Ink 1">
@@ -18425,7 +18515,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="2" name="Ink 1">
@@ -18470,8 +18560,8 @@
       <xdr:row>2</xdr:row>
       <xdr:rowOff>17208</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="9" name="Ink 8">
@@ -18490,7 +18580,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="9" name="Ink 8">
@@ -18535,8 +18625,8 @@
       <xdr:row>2</xdr:row>
       <xdr:rowOff>169210</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="16" name="Ink 15">
@@ -18555,7 +18645,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="16" name="Ink 15">
@@ -18600,8 +18690,8 @@
       <xdr:row>4</xdr:row>
       <xdr:rowOff>21374</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="20" name="Ink 19">
@@ -18620,7 +18710,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="20" name="Ink 19">
@@ -18665,8 +18755,8 @@
       <xdr:row>6</xdr:row>
       <xdr:rowOff>153258</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="39" name="Ink 38">
@@ -18685,7 +18775,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="39" name="Ink 38">
@@ -18730,8 +18820,8 @@
       <xdr:row>5</xdr:row>
       <xdr:rowOff>143337</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="40" name="Ink 39">
@@ -18750,7 +18840,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="40" name="Ink 39">
@@ -18795,8 +18885,8 @@
       <xdr:row>4</xdr:row>
       <xdr:rowOff>161496</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="41" name="Ink 40">
@@ -18815,7 +18905,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="41" name="Ink 40">
@@ -18860,8 +18950,8 @@
       <xdr:row>5</xdr:row>
       <xdr:rowOff>124535</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="42" name="Ink 41">
@@ -18880,7 +18970,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="42" name="Ink 41">
@@ -18925,8 +19015,8 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>38192</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId17">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="50" name="Ink 49">
@@ -18945,7 +19035,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="50" name="Ink 49">
@@ -18990,8 +19080,8 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>114465</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId19">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="51" name="Ink 50">
@@ -19010,7 +19100,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="51" name="Ink 50">
@@ -19055,8 +19145,8 @@
       <xdr:row>5</xdr:row>
       <xdr:rowOff>161697</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId21">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="61" name="Ink 60">
@@ -19075,7 +19165,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="61" name="Ink 60">
@@ -19120,8 +19210,8 @@
       <xdr:row>5</xdr:row>
       <xdr:rowOff>113457</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId23">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="62" name="Ink 61">
@@ -19140,7 +19230,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="62" name="Ink 61">
@@ -19185,8 +19275,8 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>26312</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId25">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="73" name="Ink 72">
@@ -19205,7 +19295,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="73" name="Ink 72">
@@ -19250,8 +19340,8 @@
       <xdr:row>9</xdr:row>
       <xdr:rowOff>172189</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId27">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="74" name="Ink 73">
@@ -19270,7 +19360,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="74" name="Ink 73">
@@ -19315,8 +19405,8 @@
       <xdr:row>9</xdr:row>
       <xdr:rowOff>65547</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId29">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="75" name="Ink 74">
@@ -19335,7 +19425,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="75" name="Ink 74">
@@ -19380,8 +19470,8 @@
       <xdr:row>13</xdr:row>
       <xdr:rowOff>48761</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId31">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="84" name="Ink 83">
@@ -19400,7 +19490,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="84" name="Ink 83">
@@ -19445,8 +19535,8 @@
       <xdr:row>11</xdr:row>
       <xdr:rowOff>164033</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId33">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="85" name="Ink 84">
@@ -19465,7 +19555,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="85" name="Ink 84">
@@ -19510,8 +19600,8 @@
       <xdr:row>10</xdr:row>
       <xdr:rowOff>163750</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
+      <mc:Choice Requires="xdr14">
         <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId35">
           <xdr14:nvContentPartPr>
             <xdr14:cNvPr id="86" name="Ink 85">
@@ -19530,7 +19620,7 @@
           </xdr14:xfrm>
         </xdr:contentPart>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:pic>
           <xdr:nvPicPr>
             <xdr:cNvPr id="86" name="Ink 85">
@@ -19590,7 +19680,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">110 54 7331,'0'0'10805,"0"-28"-5370,-4 55-5411,0-1 0,-2 0 1,0 0-1,-2 0 0,-16 36 0,9-22-4,9-25-33,4-6 34,-1 0 0,-1 0 1,0 0-1,0 0 1,-1-1-1,-9 14 0,13-21 105,1-14-68,1-7-82,1-1-1,1 1 0,1 0 0,1 1 0,9-26 1,43-96-129,-55 136 140,1 1-1,-1-1 1,0 0 0,1 1-1,0 0 1,0-1-1,1 1 1,6-6 0,-9 9 9,-1 1 1,1 0 0,0-1-1,-1 1 1,1-1-1,0 1 1,-1 0-1,1 0 1,0-1-1,0 1 1,-1 0 0,1 0-1,0 0 1,0 0-1,0 0 1,-1 0-1,1 0 1,0 0-1,0 0 1,-1 0 0,1 1-1,0-1 1,1 0-1,-1 2 1,1-1 1,0 0-1,-1 1 0,1-1 0,-1 1 0,1-1 0,-1 1 0,0-1 0,0 1 0,1 0 1,-1 0-1,1 3 0,14 32 30,-1 0 0,-3 1 0,10 45 0,13 119 86,-35-200-642,3 15 1451,-5-11-7643,-6-7 1302</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="276.43">0 293 9604,'0'0'7796,"63"0"-7252,-33 0 113,0-2-273,-3-2 16,-7 3-64,-10-1-160,-4 2-96,-3-2 32,-3 0-368,0-2-1473,0 0-1696</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="276.41">0 293 9604,'0'0'7796,"63"0"-7252,-33 0 113,0-2-273,-3-2 16,-7 3-64,-10-1-160,-4 2-96,-3-2 32,-3 0-368,0-2-1473,0 0-1696</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -19634,7 +19724,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7323.48">2730 154 6563,'0'0'12870,"-10"-21"-13799,10 25-1216,0 9-768,0 3-3618</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8332.77">2760 257 10645,'0'0'5509,"-13"0"-4946,-42 5-144,52-4-392,0 0 0,0 1 0,1-1 1,-1 0-1,0 1 0,1 0 0,-1 0 0,1 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0 1 1,0-1-1,0 1 0,1-1 0,-1 1 0,1 0 1,0-1-1,0 1 0,0 0 0,0 0 0,0 0 1,1 0-1,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 1,0 4-1,1-6-55,0-1-1,-1 1 1,1 0 0,0-1 0,-1 1-1,1-1 1,0 1 0,0-1 0,-1 1-1,1-1 1,0 0 0,0 1 0,0-1 0,0 0-1,0 0 1,0 0 0,-1 1 0,1-1-1,0 0 1,0 0 0,0 0 0,0-1-1,0 1 1,0 0 0,0 0 0,0 0-1,-1-1 1,1 1 0,0 0 0,0-1-1,1 0 1,30-9-752,-29 8 798,-1 0 0,1 0-1,-1 1 1,1-1-1,0 1 1,0 0-1,0-1 1,0 2 0,0-1-1,0 0 1,0 0-1,0 1 1,0 0-1,4-1 1,-5 2-5,0 0 0,-1 0 0,1-1-1,-1 1 1,0 0 0,1 0 0,-1 1 0,0-1 0,0 0 0,1 0-1,-1 1 1,0-1 0,0 0 0,0 1 0,-1-1 0,1 1 0,0-1 0,0 1-1,-1 0 1,1-1 0,-1 1 0,0 0 0,1-1 0,-1 1 0,0 0 0,0 2-1,1 7 24,0-1-1,-1 0 0,0 1 1,0-1-1,-1 1 0,-1-1 0,0 0 1,-5 16-1,6-23 26,0 1 1,0-1 0,0 1-1,-1-1 1,1 0-1,-1 0 1,0 0-1,0 0 1,-1 0-1,1 0 1,0 0 0,-1-1-1,0 1 1,1-1-1,-1 0 1,0 1-1,0-2 1,-1 1-1,1 0 1,0 0-1,-1-1 1,1 0 0,0 0-1,-1 0 1,0 0-1,1 0 1,-8 0-1,10-4 37,0 1 0,1 0 0,-1-1-1,1 1 1,0-1 0,0 1-1,0-1 1,0 1 0,0-1 0,1-3-1,-1 5-88,3-11-129,1 0 0,0 1 0,1-1 0,0 1 0,1 0 0,0 0 0,0 1 0,1-1 0,13-12 0,0-5-353,4-7 9,3-2-437,32-61 1,-53 85 1299,0-1 1,0 0-1,-1 0 1,-1 0 0,-1-1-1,0 1 1,0-1-1,0-26 1,-3 41-374,0 1-1,0-1 1,0 0 0,0 0 0,-1 0-1,1 1 1,0-1 0,0 0-1,0 0 1,0 0 0,0 1-1,0-1 1,0 0 0,0 0-1,-1 0 1,1 0 0,0 0 0,0 1-1,0-1 1,0 0 0,-1 0-1,1 0 1,0 0 0,0 0-1,0 0 1,-1 0 0,1 0 0,0 0-1,0 0 1,0 0 0,-1 1-1,1-1 1,0 0 0,0 0-1,0 0 1,-1-1 0,1 1 0,0 0-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 0 0,0 0-1,0 0 1,-1 0 0,1 0 0,0 0-1,0-1 1,0 1 0,0 0-1,0 0 1,-1 0 0,1 0-1,0 0 1,0-1 0,0 1 0,0 0-1,0 0 1,0 0 0,0-1-1,0 1 1,-1 0 0,1 0-1,0 0 1,0-1 0,-10 15-57,1 8 29,1 1 0,2 0 0,0 0 0,1 1 0,1 0 0,2 0 0,0 0-1,2 0 1,3 34 0,-4-57-42,1 1 1,0-1-1,0 1 0,0-1 0,0 1 0,1-1 1,-1 0-1,0 1 0,1-1 0,-1 0 0,1 1 1,-1-1-1,1 0 0,-1 1 0,1-1 1,0 0-1,0 0 0,0 0 0,-1 0 0,1 0 1,0 0-1,0 0 0,1 0 0,-1 0 1,0 0-1,0 0 0,0-1 0,1 1 0,-1 0 1,0-1-1,0 1 0,1-1 0,-1 0 0,1 1 1,-1-1-1,0 0 0,1 0 0,-1 0 1,1 0-1,-1 0 0,0 0 0,1 0 0,-1 0 1,1-1-1,-1 1 0,2-1 0,3-1-108,-1-1-1,1 1 1,-1-1-1,0 1 1,0-2-1,0 1 1,-1 0-1,1-1 1,6-7-1,-10 11 160,0 0-1,0 0 0,0 0 1,0 0-1,0 0 1,0 0-1,0 0 0,-1 1 1,1-1-1,0 0 1,0 0-1,0 1 1,0-1-1,0 0 0,0 1 1,0-1-1,-1 1 1,1 0-1,0-1 0,0 1 1,-1-1-1,1 1 1,0 0-1,-1 0 1,1-1-1,0 1 0,-1 0 1,1 1-1,1 1 15,1-1-1,0 1 0,-1-1 0,1 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0-1 0,1 1 0,4 0 1,-5-1-95,1 0 0,-1-1 0,1 0-1,-1 1 1,0-1 0,1-1 0,-1 1 0,1 0 0,-1-1 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,1-1 0,-1 1 0,0-1 0,-1 0 0,1 0 0,0 0 0,0 0 0,2-3 0,-2 0 23,-1 0 1,1 0-1,-1 0 1,0 0-1,0 0 1,0-1 0,-1 1-1,0-1 1,0 1-1,0-1 1,-1 1-1,1-1 1,-2-6 0,2-16 57,0 17 19,-1 0 0,0 0 0,0 0 0,-1 0 0,0 1 0,-1-1 0,0 0 0,-1 1 0,0-1 0,-6-13 0,9 24 29,0 0 1,0 0-1,0 0 0,-1 0 0,1-1 1,0 1-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,0 0 0,0 0 0,0 0 1,0-1-1,0 1 0,-1 0 1,1 0-1,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,-1 0 1,1 1-1,0-1 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,-1 0-1,1 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 1 0,0-1 0,-1 0 1,1 0-1,0 0 0,0 0 1,0 0-1,0 0 0,0 1 0,0-1 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 1 1,0-1-1,0 0 0,0 0 1,-5 18 596,-1 20-837,3-18 80,-2 20-180,2 0-1,2 1 1,3 44 0,-2-85 88,0 1 1,0-1-1,0 1 1,0 0-1,1-1 0,-1 1 1,0-1-1,0 1 1,0-1-1,0 1 1,1-1-1,-1 1 1,0-1-1,1 1 1,-1-1-1,0 1 1,1-1-1,-1 1 0,0-1 1,1 1-1,-1-1 1,1 0-1,-1 1 1,1-1-1,-1 0 1,1 1-1,-1-1 1,1 0-1,0 0 1,9 1-6474</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8503.73">3095 196 13654,'0'0'5123,"53"-6"-5331,-23 6-1089,3 0-704,1 2-2161,-1 0-6387</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8785.96">3404 263 8772,'0'0'11173,"-3"0"-10997,16 0-160,4 0 144,6 0-160,0 0-64,-3 0-656,0 0-833,-7 0-976,-3 0-2945</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8785.94">3404 263 8772,'0'0'11173,"-3"0"-10997,16 0-160,4 0 144,6 0-160,0 0-64,-3 0-656,0 0-833,-7 0-976,-3 0-2945</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8996.27">3427 352 10533,'0'0'8372,"-10"11"-7940,30-11-432,3 0-16,7-2-480,0-7-449,-3-1-976,-4-1-592,-3-1-2705</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9267.66">3490 190 9989,'0'0'10039,"-6"-1"-9770,6 0-268,-1 1 1,0 0-1,0-1 0,1 1 0,-1 0 0,0-1 0,0 1 1,0 0-1,0 0 0,1 0 0,-1 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0 0 0,1 0 1,-1 0-1,0 1 0,0-1 0,0 0 0,-1 1 0,20 12 10,48 18-15,-53-25-8,56 27-177,-64-31 174,1 1-1,-2 1 1,1-1 0,0 1 0,-1 0 0,1 0 0,-1 0-1,0 1 1,-1-1 0,5 7 0,-7-9 30,0 0 0,-1 0 0,1 0 0,0 1 0,-1-1 1,1 0-1,-1 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 1,-1 1-1,1-1 0,-1 0 0,0 0 0,1 1 0,-1-1 0,0 0 0,0 0 1,-1 0-1,1 0 0,0 0 0,-1 0 0,-2 3 0,-5 4 5,-1 1-1,0-1 0,-18 12 1,7-5-589,-1 1-1928,1-2-1953</inkml:trace>
 </inkml:ink>
@@ -19871,7 +19961,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="426.76">24 736 3810,'0'0'11717,"0"38"-11301,17-36-128,3-2-176,6 0-112,1 0-1744,-1-10-6356</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1007.89">887 451 14231,'0'0'7758,"-6"-5"-7313,-20-15-154,26 20-282,-1-1 0,0 1 0,1-1 0,-1 1 0,0 0 1,0 0-1,1-1 0,-1 1 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 1 1,1-1-1,-1 0 0,0 0 0,1 1 0,-1-1 0,0 1 0,1-1 0,-1 0 0,0 1 0,1-1 0,-1 1 0,1-1 0,-1 1 0,1 0 1,-1-1-1,1 1 0,-1 1 0,-14 25-5,13-24 19,-2 9 0,-1 0 1,2 0-1,0 0 1,0 0-1,1 1 1,0-1-1,1 1 1,1-1-1,0 1 1,1 0-1,0-1 1,4 18-1,-4-25-64,0 0-1,0 0 1,0 0 0,1 0-1,0-1 1,0 1 0,0-1-1,1 1 1,-1-1-1,1 0 1,0 0 0,0 0-1,0 0 1,1 0-1,0-1 1,-1 0 0,1 1-1,0-1 1,0-1 0,1 1-1,-1-1 1,1 1-1,-1-1 1,1-1 0,0 1-1,0-1 1,-1 1-1,1-1 1,0-1 0,0 1-1,0-1 1,0 0-1,7 0 1,-7-2 2,1 1 0,-1-1 0,0 0 0,1 0 0,-1-1 0,0 1 1,0-1-1,-1 0 0,1-1 0,-1 1 0,1-1 0,-1 0 0,0 0 0,0 0 0,-1 0 0,1-1 0,-1 0 0,4-7 0,0 1 57,-1-1 0,0 1 0,-1-1-1,-1 0 1,1 0 0,-2-1 0,3-16-1,-4 15-12,0 1 0,-2-1-1,1 0 1,-2 0 0,0 0-1,-1 0 1,-3-15-1,4 25 13,0 1 0,-1-1 0,1 1 0,0 0 0,-1-1 0,0 1 1,0 0-1,0 0 0,0 0 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 1 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 1 0,0-1 0,-1 1 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 1 0,1-1 0,-1 1 0,0 0 0,-6 1 0,7-1-312,0 1 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,1 1 0,-1-1 0,0 1-1,1 0 1,-1 0 0,1 0 0,-1 0 0,1 0 0,-3 4 0,1-2-944,-12 11-6263</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="83020.92">24 85 9124,'0'0'10370,"0"-11"-7881,-1 29-2612,2 23 307,-1-40-215,0 0 0,0 1 0,1-1 0,-1 0 0,1 0 0,-1 0 0,1-1 0,-1 1 0,1 0 0,-1 0 1,1 0-1,0 0 0,0 0 0,-1-1 0,1 1 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 0 0,0 1 0,0-1 0,0 1 0,0-1 1,0 0-1,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,2 0 0,-1 0-31,0 0 1,0 0-1,0 0 1,0 0-1,0-1 1,0 1-1,0 0 1,0-1-1,0 1 0,0-1 1,0 0-1,0 0 1,0 0-1,0 0 1,-1 0-1,1 0 1,0 0-1,-1 0 0,1-1 1,0 1-1,-1-1 1,0 1-1,1-1 1,-1 0-1,0 1 0,0-1 1,0 0-1,0 0 1,0 0-1,-1 0 1,1 0-1,0 0 1,-1 0-1,1 0 0,-1 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0-3-1,-6 109 2186,5-86-1983,1-13-4039</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="83570.71">854 49 9268,'0'0'9498,"-7"0"-9127,4-1-318,1 0-35,0 0 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,-4 1 0,5 1-6,0-1 1,-1 1-1,1-1 1,0 1 0,0-1-1,0 1 1,1-1-1,-1 1 1,0 0-1,0 0 1,1-1 0,-1 1-1,1 0 1,0 0-1,0 0 1,-1-1 0,1 1-1,0 0 1,0 0-1,1 0 1,-1 0 0,0 0-1,1-1 1,0 4-1,0 1 2,1 0 0,-1 1 0,2-1-1,-1 0 1,0 0 0,4 5-1,-2-6 61,-1-1-1,0 0 1,-1 1-1,1 0 1,-1-1-1,0 1 1,0 0-1,-1 0 1,1 1-1,-1-1 1,0 0-1,0 7 1,-21-9-27,7-5-6060</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="83570.7">854 49 9268,'0'0'9498,"-7"0"-9127,4-1-318,1 0-35,0 0 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,-4 1 0,5 1-6,0-1 1,-1 1-1,1-1 1,0 1 0,0-1-1,0 1 1,1-1-1,-1 1 1,0 0-1,0 0 1,1-1 0,-1 1-1,1 0 1,0 0-1,0 0 1,-1-1 0,1 1-1,0 0 1,0 0-1,1 0 1,-1 0 0,0 0-1,1-1 1,0 4-1,0 1 2,1 0 0,-1 1 0,2-1-1,-1 0 1,0 0 0,4 5-1,-2-6 61,-1-1-1,0 0 1,-1 1-1,1 0 1,-1-1-1,0 1 1,0 0-1,-1 0 1,1 1-1,-1-1 1,0 0-1,0 7 1,-21-9-27,7-5-6060</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="83755.07">821 48 13478,'0'0'4898,"89"-33"-4417,-75 28 207,-4 1-288,-4 2-144,-3-2-256</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="91077.6">1192 872 9764,'0'0'6137,"-10"0"-5177,-44 4 552,-65 11 1,31-2-2209,11-7-5576,87-6 909</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="91538.89">406 905 13142,'0'0'4728,"-15"0"-3867,-229 13 1639,172-2-2118,71-11-673,14 0-14868</inkml:trace>
@@ -19904,8 +19994,8 @@
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">0 343 9236,'0'0'7142,"6"-3"-5080,41-3-558,91-1 0,-8 2-1417,-125 5-983,6-1 1610,-26 0-18465</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="323.2">219 352 3794,'0'0'13950,"-6"21"-13408,15 102-386,-4-92-153,-2-1 0,-1 1 0,-2 0-1,-4 37 1,4-66 11,-1 1 0,1-1 0,-1 1-1,1-1 1,-1 1 0,0-1-1,0 1 1,0-1 0,-1 0-1,1 0 1,0 1 0,-1-1-1,0 0 1,1 0 0,-1 0 0,0-1-1,0 1 1,0 0 0,0-1-1,0 1 1,0-1 0,-1 0-1,1 0 1,0 0 0,-1 0-1,1 0 1,-1 0 0,1-1 0,-1 1-1,1-1 1,-1 1 0,1-1-1,-1 0 1,0 0 0,1 0-1,-1-1 1,1 1 0,-1-1-1,-2 0 1,-3-1 30,1 1 1,-1-2-1,1 1 0,0-1 0,0 0 1,0 0-1,0-1 0,1 0 1,0 0-1,-1-1 0,1 0 0,-5-5 1,7 2-2014,6 3-3111,6 0-3017</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="825.85">660 411 8468,'0'0'6952,"-4"5"-6602,-2 6-133,-1-1-1,2 2 1,-1-1-1,1 1 1,1-1 0,0 1-1,1 1 1,0-1 0,1 0-1,1 1 1,-1-1-1,2 1 1,0-1 0,3 25-1,-3-34-209,1 0-1,-1-1 0,1 1 1,0 0-1,0-1 1,0 1-1,0-1 0,0 1 1,0-1-1,1 0 0,-1 1 1,1-1-1,-1 0 0,1 0 1,0 0-1,0 0 0,0 0 1,0 0-1,1-1 0,-1 1 1,0-1-1,1 1 1,-1-1-1,1 0 0,-1 0 1,1 0-1,-1-1 0,1 1 1,0 0-1,-1-1 0,1 0 1,0 1-1,0-1 0,-1 0 1,1-1-1,0 1 1,0 0-1,-1-1 0,1 1 1,0-1-1,-1 0 0,1 0 1,-1 0-1,1 0 0,-1-1 1,1 1-1,-1-1 0,0 1 1,0-1-1,0 0 0,0 0 1,0 0-1,0 0 1,3-4-1,1-5 107,-1 1 0,1-1 0,-2 0 0,0-1 0,0 1 0,-1-1 0,0 0-1,-1 0 1,0 0 0,0-21 0,-2 25-56,0-1-1,0 1 1,-1 0-1,0 0 1,-1 0 0,0 0-1,0 1 1,0-1-1,-1 0 1,0 1-1,-1-1 1,1 1-1,-1 0 1,-1 0-1,0 1 1,-9-12 0,12 17-34,1-1 1,-1 0 0,0 1-1,1-1 1,-1 1 0,0 0 0,0-1-1,0 1 1,0 0 0,0 0 0,0 1-1,0-1 1,0 0 0,-1 1-1,1-1 1,0 1 0,0-1 0,0 1-1,-1 0 1,1 0 0,0 0-1,0 0 1,-1 1 0,1-1 0,0 1-1,0-1 1,0 1 0,-1 0 0,1 0-1,0 0 1,0 0 0,-2 1-1,1 1-171,1-1-1,-1 1 0,1 0 0,-1-1 0,1 1 0,0 0 0,0 1 0,1-1 0,-1 0 0,0 1 0,1-1 1,0 0-1,0 1 0,0 0 0,0-1 0,1 1 0,-1 0 0,1 5 0,0 12-2849,0-1-1541</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1175.09">1099 351 5138,'0'0'11742,"0"7"-11222,3 34 667,-3 0 0,-5 59 0,1-75-1643,0 0 0,-16 48 0,18-65-885,0 1-5415</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="825.83">660 411 8468,'0'0'6952,"-4"5"-6602,-2 6-133,-1-1-1,2 2 1,-1-1-1,1 1 1,1-1 0,0 1-1,1 1 1,0-1 0,1 0-1,1 1 1,-1-1-1,2 1 1,0-1 0,3 25-1,-3-34-209,1 0-1,-1-1 0,1 1 1,0 0-1,0-1 1,0 1-1,0-1 0,0 1 1,0-1-1,1 0 0,-1 1 1,1-1-1,-1 0 0,1 0 1,0 0-1,0 0 0,0 0 1,0 0-1,1-1 0,-1 1 1,0-1-1,1 1 1,-1-1-1,1 0 0,-1 0 1,1 0-1,-1-1 0,1 1 1,0 0-1,-1-1 0,1 0 1,0 1-1,0-1 0,-1 0 1,1-1-1,0 1 1,0 0-1,-1-1 0,1 1 1,0-1-1,-1 0 0,1 0 1,-1 0-1,1 0 0,-1-1 1,1 1-1,-1-1 0,0 1 1,0-1-1,0 0 0,0 0 1,0 0-1,0 0 1,3-4-1,1-5 107,-1 1 0,1-1 0,-2 0 0,0-1 0,0 1 0,-1-1 0,0 0-1,-1 0 1,0 0 0,0-21 0,-2 25-56,0-1-1,0 1 1,-1 0-1,0 0 1,-1 0 0,0 0-1,0 1 1,0-1-1,-1 0 1,0 1-1,-1-1 1,1 1-1,-1 0 1,-1 0-1,0 1 1,-9-12 0,12 17-34,1-1 1,-1 0 0,0 1-1,1-1 1,-1 1 0,0 0 0,0-1-1,0 1 1,0 0 0,0 0 0,0 1-1,0-1 1,0 0 0,-1 1-1,1-1 1,0 1 0,0-1 0,0 1-1,-1 0 1,1 0 0,0 0-1,0 0 1,-1 1 0,1-1 0,0 1-1,0-1 1,0 1 0,-1 0 0,1 0-1,0 0 1,0 0 0,-2 1-1,1 1-171,1-1-1,-1 1 0,1 0 0,-1-1 0,1 1 0,0 0 0,0 1 0,1-1 0,-1 0 0,0 1 0,1-1 1,0 0-1,0 1 0,0 0 0,0-1 0,1 1 0,-1 0 0,1 5 0,0 12-2849,0-1-1541</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1175.08">1099 351 5138,'0'0'11742,"0"7"-11222,3 34 667,-3 0 0,-5 59 0,1-75-1643,0 0 0,-16 48 0,18-65-885,0 1-5415</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1716.38">1095 385 3826,'0'0'11920,"13"-11"-11229,43-35-171,-50 42-428,1 0 0,0 1 0,0 0 1,0 0-1,0 1 0,0 0 0,1 0 0,-1 0 0,1 1 0,-1 0 0,1 1 0,-1 0 0,1 0 1,0 0-1,8 2 0,-15-2-80,1 1 9,-1 0 1,1-1-1,0 1 0,-1 0 1,1 0-1,-1 0 0,0 0 1,1 0-1,-1 0 0,0 0 1,0 0-1,1 1 0,-1-1 1,0 0-1,0 1 0,-1-1 1,1 1-1,0-1 0,0 1 1,-1 0-1,1-1 0,-1 1 1,1-1-1,-1 1 0,0 0 1,1 0-1,-1-1 0,0 1 1,0 0-1,0-1 0,-1 1 1,1 0-1,-1 3 0,1 1 12,-1 0 0,0 0-1,0 0 1,0 0 0,-1 0-1,1 0 1,-2-1 0,-3 10-1,-106 115 240,111-128-281,0-1-1,1 0 0,-1 1 1,0-1-1,0 0 0,0 1 0,1-1 1,-1 1-1,1-1 0,-1 1 1,1-1-1,0 1 0,0 0 1,0-1-1,-1 1 0,1-1 0,1 1 1,-1-1-1,0 1 0,0 0 1,1-1-1,-1 1 0,0-1 1,1 1-1,0-1 0,-1 1 0,1-1 1,0 0-1,0 1 0,0-1 1,0 0-1,0 1 0,0-1 1,0 0-1,0 0 0,0 0 0,0 0 1,3 1-1,7 6-242,-1-2-1,1 0 1,0 0-1,12 4 1,-7-2-223,-1-2 186,21 11 69,-35-17 225,1 1 0,-1 0 0,0 0 0,0-1 0,0 1 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,-1 0 1,1 1-1,0-1 0,0 0 0,-1 0 0,1 1 0,0-1 0,-1 0 0,1 1 0,-1 1 0,0-1 81,0-1-1,-1 0 1,0 1-1,1-1 1,-1 0 0,0 0-1,1 1 1,-1-1 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,0 0 0,0-1-1,-1 1 1,1 0-1,0-1 1,0 1 0,-2 0-1,-34 15 1116,28-12-812,-19 7-101,-70 25 1391,87-33-2735,0-1 0,0 0 0,-22 0 0,23-2-3653</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="83068.39">272 49 12038,'0'0'8086,"0"-1"-8013,0 0 0,0 1 0,0-1 1,0 0-1,0 0 0,0 1 0,0-1 0,-1 0 0,1 0 0,0 1 1,-1-1-1,1 0 0,0 0 0,-1 1 0,1-1 0,-1 1 1,1-1-1,-1 0 0,1 1 0,-1-1 0,0 1 0,1-1 1,-1 1-1,0-1 0,0 1 0,-3 1-63,1 1 1,0 0-1,-1 1 0,1-1 1,0 0-1,0 1 0,1 0 0,-1 0 1,0 0-1,1 0 0,0 0 1,0 0-1,0 0 0,0 1 0,0-1 1,-1 5-1,0-1-16,1 1-1,0 0 1,0 0 0,0 0-1,1 0 1,0 13 0,1-19-70,1 0 1,0 0-1,0-1 1,0 1-1,0-1 0,0 1 1,0-1-1,0 1 1,0-1-1,1 0 1,-1 0-1,0 1 0,1-1 1,-1 0-1,1 0 1,0 0-1,-1-1 1,1 1-1,0 0 1,-1 0-1,1-1 0,0 1 1,0-1-1,0 0 1,-1 0-1,1 1 1,0-1-1,0 0 0,0-1 1,0 1-1,-1 0 1,1 0-1,2-1 1,-3 0 95,-1 1 0,1 0 1,-1-1-1,1 1 0,0-1 1,-1 1-1,0-1 0,1 1 1,-1-1-1,1 0 0,-1 1 1,0-1-1,1 1 1,-1-1-1,0 0 0,1 1 1,-1-1-1,0 0 0,0 1 1,0-1-1,0 0 0,0 1 1,0-1-1,0 0 0,0 1 1,0-1-1,0 0 0,0 0 1,0 1-1,0-1 1,0 0-1,-1 1 0,1-1 1,0 1-1,-1-1 0,1 0 1,0 1-1,-1-1 0,1 1 1,-1-1-1,1 1 0,-1-2 1,-1 1 51,1-1 0,-1 0 0,1 1 1,-1-1-1,1 1 0,-1 0 0,0-1 1,0 1-1,0 0 0,0 0 0,0 0 1,-3-1-1,-26 2-1340,30 0 1187,1 0 1,-1 1-1,0-1 1,0 0-1,0 1 1,1-1-1,-1 1 1,0-1-1,0 1 1,1-1-1,-1 1 1,0 0-1,1-1 1,-1 1-1,1 0 1,-1 0-1,1-1 1,-1 1-1,1 0 1,0 0-1,-1 0 1,1-1-1,0 1 0,-1 0 1,1 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0-1 1,0 2-1,3 5-3131,11-1-1577</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="83537.03">574 77 8964,'0'0'10482,"-18"0"-9535,42 0-1115,-13-1 162,-1 1 1,0 0-1,0 0 0,1 1 0,-1 0 0,0 1 0,0 1 0,11 3 0,-20-6 11,0 1 1,0 0-1,0 0 1,0-1-1,0 1 0,0 0 1,0 0-1,0 0 1,-1 0-1,1 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,-1 0 1,1 0-1,-1 1 0,0-1 1,1 0-1,-1 0 1,0 0-1,0 1 1,0-1-1,0 0 0,0 0 1,0 1-1,0-1 1,0 0-1,0 0 0,-1 0 1,1 1-1,0-1 1,-1 0-1,1 0 1,-1 0-1,1 0 0,-1 0 1,0 0-1,0 2 1,-3 3 32,0 0 0,0 0 0,0 0 0,-1 0 0,-6 5 0,-19 25-4733,27-30-582</inkml:trace>
@@ -20066,8 +20156,8 @@
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">101 91 7716,'0'0'7856,"2"-5"-6652,4-16-46,0 3 2672,-4 44-2968,-2 197-566,0-223-258,-92 6-350,91-6 365,7 0-274,144 4-4663,-104-4 3122,-39-1-2381</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="367.56">34 8 7652,'0'0'10404,"-33"-8"-9667,36 8-721,17 8 128,3-3 16,11 3-16,5-6-48,1 0-96,3-2-1057,-9 0-1216,-8 0-1793,-6 0-3121</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1112.88">492 144 3506,'0'0'10895,"0"-6"-9942,-1 4-1216,-6-33 3837,7 34-3521,0 1 1,-1-1 0,1 0 0,0 0-1,-1 1 1,1-1 0,-1 1-1,1-1 1,-1 0 0,1 1 0,-1-1-1,1 1 1,-1-1 0,1 1-1,-1-1 1,0 1 0,1 0 0,-1-1-1,0 1 1,1 0 0,-1 0-1,0-1 1,0 1 0,1 0 0,-1 0-1,0 0 1,0 0 0,1 0-1,-1 0 1,0 0 0,0 0 0,1 0-1,-1 0 1,0 0 0,0 0-1,1 1 1,-1-1 0,0 0 0,0 1-1,1-1 1,-1 0 0,1 1-1,-1-1 1,0 1 0,1-1 0,-1 1-1,1-1 1,-1 1 0,1-1-1,-1 1 1,0 1 0,-2 1-40,0 0 0,0 1 1,0 0-1,1 0 0,-1-1 0,1 2 0,0-1 1,0 0-1,1 0 0,-1 1 0,1-1 1,0 1-1,0-1 0,0 6 0,-2 70 69,3-58-19,0-19-61,0 0 1,1 1-1,-1-1 1,1 0-1,0 0 1,0 1-1,0-1 1,0 0-1,0 0 1,1 0-1,-1 0 0,1 0 1,0-1-1,0 1 1,0 0-1,0-1 1,0 1-1,1-1 1,-1 0-1,1 0 1,0 0-1,-1 0 0,1 0 1,0-1-1,0 1 1,0-1-1,0 0 1,0 0-1,1 0 1,-1 0-1,0 0 0,0-1 1,6 1-1,-2 0-13,-1-1-1,0 0 1,1 0-1,-1 0 1,0-1-1,0 0 1,1 0-1,-1 0 1,0-1-1,0 0 1,0 0-1,-1-1 1,1 0-1,0 0 1,-1 0-1,0 0 0,7-6 1,-8 4 9,-1 1-1,0 0 1,0-1-1,-1 0 1,1 0 0,-1 0-1,0 0 1,0 0-1,-1 0 1,1 0 0,-1-1-1,0 1 1,-1 0-1,1-1 1,-1 1 0,0-1-1,0 1 1,-1 0 0,0-1-1,0 1 1,0 0-1,0-1 1,-1 1 0,0 0-1,0 0 1,-4-6-1,4 6 12,-1-1 0,0 1 0,0-1 0,0 1 0,-1 0 0,0 1 0,0-1 0,0 0 0,-1 1-1,1 0 1,-1 0 0,0 0 0,0 1 0,0 0 0,-1 0 0,1 0 0,-1 0 0,0 1 0,0 0-1,1 0 1,-1 1 0,-1 0 0,-6-1 0,9 2 14,0-1 0,0 2-1,0-1 1,0 0 0,0 1 0,0 0-1,0-1 1,0 2 0,-4 0 0,7-1-204,-1 1 1,1-1 0,0 0 0,0 0 0,0 1-1,0-1 1,0 0 0,0 1 0,0-1 0,0 1-1,0-1 1,1 1 0,-1 0 0,0-1 0,1 1-1,0 0 1,-1-1 0,1 1 0,0 0 0,0-1-1,0 1 1,0 0 0,0 2 0,3 6-2799,8-3-1474</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1582.18">847 61 6787,'0'0'12891,"-3"-1"-11848,-11-6-336,11 6 0,28 1-432,17-2 135,53-10-1,-26 3-1340,1 5-5170</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1112.86">492 144 3506,'0'0'10895,"0"-6"-9942,-1 4-1216,-6-33 3837,7 34-3521,0 1 1,-1-1 0,1 0 0,0 0-1,-1 1 1,1-1 0,-1 1-1,1-1 1,-1 0 0,1 1 0,-1-1-1,1 1 1,-1-1 0,1 1-1,-1-1 1,0 1 0,1 0 0,-1-1-1,0 1 1,1 0 0,-1 0-1,0-1 1,0 1 0,1 0 0,-1 0-1,0 0 1,0 0 0,1 0-1,-1 0 1,0 0 0,0 0 0,1 0-1,-1 0 1,0 0 0,0 0-1,1 1 1,-1-1 0,0 0 0,0 1-1,1-1 1,-1 0 0,1 1-1,-1-1 1,0 1 0,1-1 0,-1 1-1,1-1 1,-1 1 0,1-1-1,-1 1 1,0 1 0,-2 1-40,0 0 0,0 1 1,0 0-1,1 0 0,-1-1 0,1 2 0,0-1 1,0 0-1,1 0 0,-1 1 0,1-1 1,0 1-1,0-1 0,0 6 0,-2 70 69,3-58-19,0-19-61,0 0 1,1 1-1,-1-1 1,1 0-1,0 0 1,0 1-1,0-1 1,0 0-1,0 0 1,1 0-1,-1 0 0,1 0 1,0-1-1,0 1 1,0 0-1,0-1 1,0 1-1,1-1 1,-1 0-1,1 0 1,0 0-1,-1 0 0,1 0 1,0-1-1,0 1 1,0-1-1,0 0 1,0 0-1,1 0 1,-1 0-1,0 0 0,0-1 1,6 1-1,-2 0-13,-1-1-1,0 0 1,1 0-1,-1 0 1,0-1-1,0 0 1,1 0-1,-1 0 1,0-1-1,0 0 1,0 0-1,-1-1 1,1 0-1,0 0 1,-1 0-1,0 0 0,7-6 1,-8 4 9,-1 1-1,0 0 1,0-1-1,-1 0 1,1 0 0,-1 0-1,0 0 1,0 0-1,-1 0 1,1 0 0,-1-1-1,0 1 1,-1 0-1,1-1 1,-1 1 0,0-1-1,0 1 1,-1 0 0,0-1-1,0 1 1,0 0-1,0-1 1,-1 1 0,0 0-1,0 0 1,-4-6-1,4 6 12,-1-1 0,0 1 0,0-1 0,0 1 0,-1 0 0,0 1 0,0-1 0,0 0 0,-1 1-1,1 0 1,-1 0 0,0 0 0,0 1 0,0 0 0,-1 0 0,1 0 0,-1 0 0,0 1 0,0 0-1,1 0 1,-1 1 0,-1 0 0,-6-1 0,9 2 14,0-1 0,0 2-1,0-1 1,0 0 0,0 1 0,0 0-1,0-1 1,0 2 0,-4 0 0,7-1-204,-1 1 1,1-1 0,0 0 0,0 0 0,0 1-1,0-1 1,0 0 0,0 1 0,0-1 0,0 1-1,0-1 1,1 1 0,-1 0 0,0-1 0,1 1-1,0 0 1,-1-1 0,1 1 0,0 0 0,0-1-1,0 1 1,0 0 0,0 2 0,3 6-2799,8-3-1474</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1582.16">847 61 6787,'0'0'12891,"-3"-1"-11848,-11-6-336,11 6 0,28 1-432,17-2 135,53-10-1,-26 3-1340,1 5-5170</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1955.78">983 61 6963,'0'0'12006,"-20"-6"-9309,21 27-2585,2 1-1,0-1 1,1 0 0,2 0-1,9 27 1,2 8 24,-16-54-128,0 0 1,-1 1-1,1-1 1,-1 0 0,1 0-1,-1 1 1,0-1 0,0 0-1,0 1 1,0-1-1,0 0 1,-1 1 0,1-1-1,-1 0 1,1 1 0,-1-1-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,-1 0 1,1 0 0,-1 0-1,1 0 1,-1-1-1,1 1 1,-1-1 0,0 1-1,0-1 1,0 0 0,0 1-1,0-1 1,0 0-1,0 0 1,0 0 0,-1-1-1,1 1 1,0-1 0,0 1-1,-5 0 1,-8 1 44,1-1 1,-1 0-1,0-1 1,0-1-1,-18-2 1,29 2-72,0 1 1,1-1-1,-1 0 1,1 0 0,-1-1-1,1 1 1,-1-1-1,1 0 1,0 0-1,-4-2 1,6 3-391,0 0 0,-1 0 0,1-1 1,0 1-1,0 0 0,0-1 0,0 1 0,0 0 0,0-1 0,0 0 1,0 1-1,1-1 0,-1 1 0,0-4 0,0-4-5040</inkml:trace>
 </inkml:ink>
 </file>
@@ -20098,7 +20188,7 @@
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">31 148 10405,'0'0'9839,"-3"-4"-9063,-7-7-102,4 12 252,0 30 204,4-15-1421,-1 90 395,3-73-91,0-32-13,0 0 0,0 0 0,0 0 0,1 0-1,-1 0 1,0 1 0,1-1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0-1,1 0 1,0 0 0,-1 0 0,1 0 0,0-1 0,0 1 0,0 0 0,-1 0-1,1-1 1,0 1 0,0 0 0,0-1 0,0 1 0,0-1 0,1 1 0,-1-1-1,0 0 1,0 1 0,0-1 0,0 0 0,0 0 0,1 0 0,-1 0 0,2 0-1,-1 0-7,1 0-1,0 0 0,-1 0 0,1-1 0,-1 1 0,1-1 0,-1 0 0,1 1 1,-1-1-1,1 0 0,-1-1 0,0 1 0,1 0 0,-1-1 0,3-2 0,2-4-30,-1 0 0,-1-1 0,1 1 0,-2-1 0,1 0 0,-1-1 0,0 1 0,-1-1 0,0 0 0,-1 1 0,0-1 0,-1 0 0,1-17-1,-2 26 70,0 24 50,-8 77 234,0-2-3088,10-94-697,9-1-1312</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="263.04">217 313 11829,'0'0'7972,"33"4"-7492,-13-4-208,3 0-256,1 0-16,-1 0-64,-7-4-1312,-2 4-1874,-8-4-1040</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="443.43">250 396 9748,'0'0'10005,"-7"31"-9813,24-29 176,13-2-304,0 0-64,6-8-256,1-5-1633,-4 1-1024,-10-1-2241,-6 0-3106</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="443.41">250 396 9748,'0'0'10005,"-7"31"-9813,24-29 176,13-2-304,0 0-64,6-8-256,1-5-1633,-4 1-1024,-10-1-2241,-6 0-3106</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="702.52">369 216 13510,'0'0'5875,"11"3"-5787,15 7-45,-1 0 0,0 1 0,0 2 0,-1 1 0,-1 0 0,27 22 0,-48-34 5,0-1-1,-1 1 1,1 0-1,0-1 1,-1 1-1,1 0 1,-1 0-1,0 0 1,0 0-1,1 0 1,-1 0-1,0 0 0,-1 1 1,1-1-1,0 0 1,-1 1-1,1-1 1,-1 0-1,0 1 1,0-1-1,0 0 1,0 1-1,0-1 1,0 0-1,-1 1 0,1-1 1,-1 0-1,1 1 1,-1-1-1,0 0 1,0 0-1,0 0 1,0 0-1,-1 0 1,1 0-1,0 0 1,-1 0-1,-1 2 1,-9 7 215,0 1 0,-1-2 1,0 0-1,-25 15 0,-5 5-821,26-17-1782,0-4-2625</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2362.85">881 402 8932,'0'0'8868,"-7"-2"-8548,7 10 209,-10 1-273,0 3 16,0-1-128,-3 2-96,0 1-48,-4-3-288,4 2-1969,-1-5-1713,8 0-5026</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3228.95">1083 248 6707,'0'0'10760,"-13"-11"-6348,13 9-4378,1 0 0,0-1 0,-1 1 0,1 0 0,0 0 0,0 0-1,0 1 1,1-1 0,-1 0 0,0 0 0,1 1 0,-1-1 0,1 0-1,-1 1 1,1 0 0,0-1 0,0 1 0,-1 0 0,1 0 0,0 0 0,0 0-1,0 0 1,0 0 0,1 1 0,-1-1 0,4 0 0,4-1-28,1-1 0,0 1 0,-1 1 0,13 0 0,-22 1-7,0 1 0,0-1 1,0 1-1,0-1 0,0 1 0,0 0 0,0-1 1,0 1-1,0 0 0,-1 0 0,1-1 1,0 1-1,0 0 0,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 0 0,1 0 1,-1 0-1,0 0 0,1 0 0,-1 0 1,0 1-1,0-1 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 1,0 0-1,-1 1 0,1-1 0,0 0 0,-1 1 1,0 4 9,0-1-1,0 0 1,0 1 0,-1-1 0,0 0 0,0 0 0,-3 7-1,-24 23 30,21-27-66,1 1 0,0 0 1,0 1-1,-7 13 0,17-21-92,0 0 0,0 0 0,1 0 0,-1 0 0,1-1-1,-1 1 1,1-1 0,0 0 0,-1 0 0,1 0 0,4 0 0,11 4-90,-17-5 201,0 1 1,0 0 0,0 0 0,0 0 0,0 1 0,0-1-1,0 0 1,0 1 0,0-1 0,0 1 0,-1 0-1,1-1 1,-1 1 0,1 0 0,-1 0 0,0 0 0,0 0-1,0 0 1,0 0 0,1 4 0,-2-4 26,0-1-1,0 1 1,0-1 0,0 1-1,-1-1 1,1 0 0,-1 1 0,1-1-1,-1 1 1,1-1 0,-1 0-1,0 0 1,0 1 0,0-1-1,0 0 1,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,-1 0 0,1-1 0,0 1-1,-1 0 1,1-1 0,0 1-1,-1-1 1,1 1 0,-4-1 0,-3 3-239,-1-1 0,0 0 1,0-1-1,-1 0 1,-14-1-1,24 0 109,-1 0 0,1 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 1,0 0-1,-1-1 0,1 1 0,0 0 0,0 0 0,0 0 0,0 0 0,-1-1 0,1 1 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,-1 0 0,1-1 0,0 1 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0-1 0,1 1 1,-1 0-1,0-3-1002,0-11-3891</inkml:trace>
@@ -20135,7 +20225,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1461.04">1039 700 6243,'0'0'11960,"-4"-5"-10853,3 2-1061,-1 1 0,1 0-1,-1 1 1,1-1 0,-1 0 0,0 0 0,0 1-1,0-1 1,0 1 0,0-1 0,0 1-1,0 0 1,0 0 0,0 0 0,-1 0-1,1 0 1,0 0 0,-1 1 0,1-1-1,-1 1 1,1 0 0,0-1 0,-1 1 0,1 0-1,-1 1 1,1-1 0,-1 0 0,1 1-1,0-1 1,-1 1 0,1 0 0,0 0-1,-1 0 1,1 0 0,0 0 0,0 0-1,0 0 1,-3 4 0,-9 6 5,1 1 0,0 0-1,1 1 1,1 0 0,0 1 0,-11 18-1,17-24-26,1 0 0,0 0 0,0 0 0,1 1 0,0-1 0,0 1 0,1 0 0,0 0 0,1 0 0,-1 0 0,2 0 0,0 0 0,1 16 0,-1-23-22,1 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0-1 0,0 1 0,1 0 0,-1-1 0,1 0 0,0 1 0,-1-1 0,1 0 0,3 2 0,-1-1 8,1 0 0,0 0 0,0 0 0,0-1 0,0 1 0,0-1 0,0-1-1,6 1 1,-3 0 4,1-1 0,0 0 0,-1-1-1,1 0 1,-1 0 0,1-1 0,-1 0-1,0 0 1,14-7 0,-14 4-8,0 0 0,0-1 0,-1 0-1,1-1 1,-1 1 0,-1-2 0,1 1 0,-1 0 0,-1-1 0,1 0 0,-1-1 0,-1 1 0,0-1 0,7-18 0,-10 23-2,0-1 1,0 1 0,0-1-1,-1 1 1,1-1 0,-1 0-1,0 1 1,0-1 0,-1 1-1,1-1 1,-1 1 0,0-1-1,0 1 1,-1-1 0,1 1 0,-1 0-1,0-1 1,0 1 0,-1 0-1,1 1 1,-1-1 0,0 0-1,0 1 1,0-1 0,0 1-1,0 0 1,-1 0 0,0 0-1,1 1 1,-1-1 0,0 1 0,0 0-1,-5-2 1,4 2-129,0 0 0,0 0 0,-1 1 0,1-1-1,0 1 1,-1 1 0,-9-1 0,-19 6-8762,24-2 1202</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1786.03">976 590 4482,'0'0'9031,"-4"6"-8476,1 16-177,2 0-1,0 0 1,2 26 0,0-3-387,-1-44-128,0-1 0,0 0-1,-1 1 1,1-1 0,0 0 0,0 1 0,-1-1 0,1 0 0,0 1 0,0-1-1,-1 0 1,1 1 0,0-1 0,-1 0 0,1 0 0,0 0 0,-1 1 0,1-1-1,-1 0 1,1 0 0,0 0 0,-1 0 0,1 0 0,0 1 0,-1-1 0,1 0 0,-1 0-1,1 0 1,-1 0 0,1 0 0,0 0 0,-1-1 0,1 1 0,-1 0 0,1 0-1,-2 0-621,-7 0-4297</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2079.03">564 474 5955,'0'0'6915,"-13"8"-6771,13 7 80,-3 2-128,3 2-16,0 2 0,0 2-80,0-1-16,10-1-1168,3-2-3074</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2586.22">1387 738 7892,'0'0'9932,"-2"-3"-8753,2 2-1120,0 0 0,0 0 0,-1 1 0,1-1 0,0 0 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 1 0,0-1 0,1 0 0,-1 1 0,1-1 0,-1 1 0,0-1 0,0 1 0,1-1 0,-1 1 0,0 0 0,0-1 0,1 1 0,-1 0 0,0 0 0,0-1 0,0 1 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 1 0,0 0-21,-1 1 0,1-1 0,0 1 0,-1 0 0,1 0-1,0-1 1,0 2 0,0-1 0,1 0 0,-1 0 0,-1 3 0,-3 5-22,0 0 1,1 0 0,0 1 0,1-1-1,-4 14 1,7-18-13,0 0-1,0 1 0,0-1 1,1 0-1,-1 0 1,2 0-1,-1 1 0,1-1 1,2 11-1,-2-15 2,0 1 0,0-1 1,0 0-1,0 0 0,1 0 0,-1 0 0,1 0 1,-1-1-1,1 1 0,0 0 0,0-1 0,0 1 0,0-1 1,0 0-1,0 1 0,0-1 0,0 0 0,0 0 0,1-1 1,-1 1-1,0 0 0,0-1 0,1 1 0,-1-1 0,1 0 1,-1 0-1,4 0 0,0 0 9,0-1-1,-1 1 1,1-1 0,-1-1-1,1 1 1,-1-1 0,1 0-1,-1 0 1,0-1-1,0 1 1,0-1 0,0 0-1,0 0 1,-1-1 0,0 0-1,1 1 1,-1-1 0,-1-1-1,1 1 1,0-1 0,-1 1-1,0-1 1,0 0 0,-1 0-1,1 0 1,-1-1 0,0 1-1,-1 0 1,1-1-1,-1 1 1,0-1 0,0 0-1,-1 1 1,1-1 0,-1 0-1,-1 1 1,1-1 0,-1 0-1,0 1 1,0-1 0,-1 1-1,-2-7 1,3 9-29,-1 0 1,0 0-1,1 0 0,-1 0 1,0 0-1,-1 1 1,1-1-1,0 1 0,-1 0 1,1 0-1,-1 0 0,0 0 1,0 0-1,0 0 1,0 1-1,0-1 0,0 1 1,0 0-1,-3-1 0,-30-5-2639,1 6-5642,24 1 560</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2586.21">1387 738 7892,'0'0'9932,"-2"-3"-8753,2 2-1120,0 0 0,0 0 0,-1 1 0,1-1 0,0 0 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 1 0,0-1 0,1 0 0,-1 1 0,1-1 0,-1 1 0,0-1 0,0 1 0,1-1 0,-1 1 0,0 0 0,0-1 0,1 1 0,-1 0 0,0 0 0,0-1 0,0 1 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 1 0,0 0-21,-1 1 0,1-1 0,0 1 0,-1 0 0,1 0-1,0-1 1,0 2 0,0-1 0,1 0 0,-1 0 0,-1 3 0,-3 5-22,0 0 1,1 0 0,0 1 0,1-1-1,-4 14 1,7-18-13,0 0-1,0 1 0,0-1 1,1 0-1,-1 0 1,2 0-1,-1 1 0,1-1 1,2 11-1,-2-15 2,0 1 0,0-1 1,0 0-1,0 0 0,1 0 0,-1 0 0,1 0 1,-1-1-1,1 1 0,0 0 0,0-1 0,0 1 0,0-1 1,0 0-1,0 1 0,0-1 0,0 0 0,0 0 0,1-1 1,-1 1-1,0 0 0,0-1 0,1 1 0,-1-1 0,1 0 1,-1 0-1,4 0 0,0 0 9,0-1-1,-1 1 1,1-1 0,-1-1-1,1 1 1,-1-1 0,1 0-1,-1 0 1,0-1-1,0 1 1,0-1 0,0 0-1,0 0 1,-1-1 0,0 0-1,1 1 1,-1-1 0,-1-1-1,1 1 1,0-1 0,-1 1-1,0-1 1,0 0 0,-1 0-1,1 0 1,-1-1 0,0 1-1,-1 0 1,1-1-1,-1 1 1,0-1 0,0 0-1,-1 1 1,1-1 0,-1 0-1,-1 1 1,1-1 0,-1 0-1,0 1 1,0-1 0,-1 1-1,-2-7 1,3 9-29,-1 0 1,0 0-1,1 0 0,-1 0 1,0 0-1,-1 1 1,1-1-1,0 1 0,-1 0 1,1 0-1,-1 0 0,0 0 1,0 0-1,0 0 1,0 1-1,0-1 0,0 1 1,0 0-1,-3-1 0,-30-5-2639,1 6-5642,24 1 560</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2863.97">1334 594 9732,'0'0'8124,"-1"-4"-7700,-2 4-291,1 14 12,-1 40 163,2 69 254,1-111-901,1 14 849,5-17-2737,7-6-3822,-6-3-1320</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3405.01">2310 364 9076,'0'0'9682,"-1"-11"-8268,-4-38-342,5 44-1013,1 0-1,-1-1 0,1 1 1,0 0-1,0 0 1,0 0-1,1 0 0,0 0 1,0 0-1,0 1 0,1-1 1,-1 1-1,1-1 1,0 1-1,1 0 0,-1 0 1,0 0-1,1 0 0,0 1 1,0 0-1,5-4 0,7-4-38,1 0-1,0 1 0,33-13 0,-37 17-149,0 1 1,0 0-1,1 0 0,0 2 0,0 0 1,0 0-1,20 0 0,-33 3-73,-1 0-1,1 1 0,0-1 1,-1 0-1,1 1 0,0-1 1,-1 0-1,1 1 0,-1-1 1,1 0-1,-1 1 0,1-1 1,-1 1-1,1-1 0,-1 1 1,1 0-1,-1-1 0,0 1 1,1-1-1,-1 1 0,0 0 1,0-1-1,1 1 0,-1 0 1,0-1-1,0 1 0,0 0 1,0-1-1,0 1 0,0 0 1,0-1-1,0 1 0,0 0 1,0-1-1,0 1 0,0 0 1,0-1-1,-1 1 0,1 0 1,0-1-1,0 1 0,-1 0 1,1-1-1,0 1 0,-1-1 0,0 2 1,-13 17-6462</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3590.97">2373 376 8036,'0'0'6098,"69"-21"-5953,-26 2-145,4 2-753,-7-2-687,-10 2-1906,-11 2-1616</inkml:trace>
@@ -20192,12 +20282,12 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6223.9">1056 1129 5955,'0'0'8892,"10"-8"-8369,-7 5-495,4-2 96,0 0 0,0 0 0,0 0-1,0 1 1,1 0 0,0 0 0,0 1 0,0 0-1,0 0 1,0 1 0,0 0 0,17-1 0,-24 3-118,-1 0 0,1 0-1,-1 0 1,0 0 0,1 0 0,-1 0 0,0 0 0,1 1 0,-1-1 0,0 0 0,1 0 0,-1 0 0,0 0-1,1 1 1,-1-1 0,0 0 0,0 0 0,1 1 0,-1-1 0,0 0 0,0 0 0,0 1 0,1-1-1,-1 0 1,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,1 0 0,-1 1 0,0-1 0,0 0-1,0 1 1,0 0 0,-3 19 266,-12 17 260,0-19-392,12-16-142,0 1-1,1-1 1,-1 1-1,1 0 0,0 0 1,0 0-1,0 0 1,0 1-1,0-1 1,1 1-1,0-1 0,-1 1 1,0 3-1,4-6-26,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 1,-1 0-1,1 0 0,0-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,3 0 0,27 9-174,-31-9 198,-1 0 1,0 1 0,0-1 0,1 0-1,-1 1 1,0-1 0,0 0 0,0 1-1,0-1 1,0 0 0,0 1 0,1-1-1,-1 0 1,0 1 0,0-1 0,0 1-1,0-1 1,0 0 0,0 1 0,-1-1-1,1 0 1,0 1 0,0-1-1,0 0 1,0 1 0,0-1 0,0 0-1,-1 1 1,1-1 0,0 0 0,0 1-1,0-1 1,-1 0 0,1 1 0,-18 11 64,-25 5 189,39-15-247,-5 1-224,-17 5 572,17-4-4856</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6786.28">1524 1161 7475,'0'0'9021,"-7"-6"-6023,5 11-2937,1 0-1,-1 0 1,1 0-1,0 1 1,0-1 0,1 1-1,0-1 1,0 0-1,1 7 1,-1-11-110,1 0 1,0 1 0,-1-1 0,1 1-1,0-1 1,0 0 0,0 0 0,0 1 0,0-1-1,0 0 1,1 0 0,-1 0 0,0 0-1,0 0 1,1-1 0,-1 1 0,1 0-1,-1 0 1,1-1 0,-1 1 0,1-1-1,-1 0 1,1 1 0,-1-1 0,1 0-1,0 0 1,-1 0 0,1 0 0,-1 0-1,1 0 1,-1 0 0,1-1 0,0 1-1,2-2 1,-1 2-47,-1-1-1,1 1 1,-1-1-1,1 0 1,-1 0-1,1 0 1,-1-1-1,0 1 1,1 0-1,-1-1 1,0 1-1,0-1 1,0 0-1,0 0 1,0 0-1,-1 0 1,3-4-1,21-42 194,-19 33 405,-10 65 1549,1-42-2264,-11 38 1095,11-13-5457</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7168.2">2155 1010 11493,'0'0'4858,"-10"6"-4415,-28 21-56,36-25-336,1 0 0,-1 1 0,0-1 0,1 0 0,0 1 0,0 0 0,-1-1 0,1 1 0,1 0 0,-1-1 0,0 1 0,1 0 0,0 0 1,-1 0-1,1 0 0,0-1 0,0 1 0,1 3 0,0 0 10,-1 0 1,1-1-1,0 1 1,1-1-1,0 0 1,0 1 0,2 5-1,6 2-397,9 19 1989,-21-21-2689,-18-6-3220</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7318.97">2118 1083 6451,'0'0'9220,"56"-68"-8195,-36 55-49,-3 3-224,-1 1-127,-6 1-81,0 5-272,0-1-272,-3 4-384,-4 0-1793</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7318.96">2118 1083 6451,'0'0'9220,"56"-68"-8195,-36 55-49,-3 3-224,-1 1-127,-6 1-81,0 5-272,0-1-272,-3 4-384,-4 0-1793</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8023.66">2842 1203 7764,'0'0'7966,"-12"-1"-7200,-37-1-107,47 3-599,-1 0 0,0-1 1,1 1-1,-1 0 1,1 1-1,0-1 1,-1 0-1,1 1 0,0-1 1,0 1-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 0,1 0 1,-1 0-1,1 1 1,-1-1-1,1 1 1,0-1-1,0 1 1,-1 3-1,1-4-59,0 0 0,1 0 0,-1 0-1,0 0 1,1-1 0,-1 1 0,1 0 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0-1,1 0 1,0-1 0,0 1 0,-1 0 0,1 0 0,0-1 0,0 1-1,0 0 1,1-1 0,-1 1 0,2 1 0,2-1-33,0 0 0,0-1 0,1 1 1,-1-1-1,0-1 0,0 1 0,1 0 0,-1-1 1,0 0-1,1-1 0,-1 1 0,6-2 0,-10 2 47,-1 0 0,0-1 0,1 1 0,-1 0 0,1 0 1,-1 0-1,0-1 0,1 1 0,-1 0 0,0 0 0,1-1 0,-1 1 0,0 0 0,0-1 0,1 1 0,-1 0 0,0-1 0,0 1 0,1-1 0,-1 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0-1 0,0 1 1,0-1-1,-1 1 0,1 0 0,0-1 0,0 1 0,0 0 0,-1-1 0,1 1 0,0 0 0,-1-1 0,1 1 0,0 0 0,-1-1 0,1 1 0,0 0 0,-1 0 0,1-1 0,0 1 0,-2 0 0,-20-14 534,15 12-528,-1 0-1,1 1 0,0 0 0,0 0 1,-1 0-1,1 1 0,0 0 1,-1 0-1,-12 3 0,12 12-1529,8-14 1239,0 0-1,0-1 0,0 1 1,0 0-1,0 0 0,0 0 1,0 0-1,0-1 0,0 1 1,0 0-1,0 0 0,1 0 1,-1 0-1,0-1 0,1 1 1,-1 0-1,0 0 0,1-1 1,-1 1-1,1 1 0,16 4-6166</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8353.39">3011 1192 11221,'0'0'5918,"-4"-3"-5377,4 3-542,0 0 1,0 0-1,0 0 1,-1 0-1,1 0 0,0 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,0 0 0,-1 0 1,1 0-1,0-1 1,0 1-1,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 1,0-1-1,0 1 0,0 0 1,-1 0-1,1 0 1,0-1-1,0 1 0,0 0 1,0 0-1,0 0 0,0-1 1,0 1-1,0 0 1,0 0-1,0-1 0,0 1 1,0 0-1,0 0 0,0-1 1,0 1-1,0 0 0,0 0 1,0-1-1,0 1 1,0 0-1,0 0 0,0 0 1,0-1-1,0 1 0,0 0 1,1 0-1,-1 0 0,0-1 1,0 1-1,0 0 1,0 0-1,1 0 0,-1 0 1,0-1-1,24-2 107,44 5 435,-61-1-435,-5-1-62,-1 0 0,0 0 0,1 0-1,-1 1 1,0-1 0,1 1 0,-1-1 0,0 1 0,1-1 0,-1 1-1,0 0 1,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0-1,0 0 1,0 1 0,0-1 0,0 0 0,-1 0 0,1 0-1,0 1 1,-1-1 0,1 0 0,-1 1 0,1-1 0,-1 0 0,0 1-1,0-1 1,0 1 0,1-1 0,-1 0 0,0 1 0,-1-1-1,1 1 1,0-1 0,0 0 0,-1 1 0,0 1 0,-1 9 163,-1 0 0,-1 0 1,-8 18-1,9-21-234,2-7-130,-9 31-228,13-14-6175,5-15-862</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8869.48">3389 1242 9989,'0'0'10039,"-7"5"-9615,4-4-399,0 0 1,0 1-1,1-1 1,-1 1-1,1 0 0,-1 0 1,1 0-1,-1 0 1,1 0-1,0 1 0,0-1 1,0 1-1,1-1 0,-1 1 1,0 0-1,1-1 1,0 1-1,0 0 0,0 0 1,0 0-1,0 0 1,0 0-1,1 0 0,-1 0 1,1 1-1,0-1 0,0 0 1,0 0-1,1 0 1,-1 0-1,1 0 0,0 4 1,0-6-29,0 0-1,0 1 1,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0 0-1,1 0 1,-1 0 0,0 0 0,1-1 0,-1 1 0,0 0 0,1-1 0,-1 1-1,1-1 1,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 0 0,1 0 0,-1 0 0,1-1 0,2 0-1,-2 1 19,0-1 0,-1 1 0,1 0 0,0-1 0,0 0-1,0 1 1,-1-1 0,1 0 0,0 0 0,0 0-1,-1 0 1,1 0 0,-1-1 0,1 1 0,-1 0 0,0-1-1,0 1 1,1-1 0,-1 1 0,0-1 0,0 0 0,0 1-1,-1-1 1,1 0 0,1-2 0,-2-3-16,1 0 0,-1 0 0,-1 0 0,1 1 0,-1-1 0,0 0 0,-1 1 0,1-1 0,-1 1 0,-4-10 0,-3 0 53,0 0 0,-17-22 0,4 5 27,22 33-92,0 0 0,0 0 1,-1 0-1,1-1 0,0 1 0,0 0 0,0-1 0,0 1 1,0 0-1,-1 0 0,1-1 0,0 1 0,0 0 0,0-1 1,0 1-1,0 0 0,0-1 0,0 1 0,0 0 0,0-1 1,0 1-1,0 0 0,0 0 0,1-1 0,-1 1 0,0 0 1,0-1-1,0 1 0,0 0 0,0 0 0,1-1 1,-1 1-1,0 0 0,0 0 0,0-1 0,1 1 0,-1 0 1,0 0-1,0 0 0,1-1 0,-1 1 0,0 0 0,0 0 1,1 0-1,0 0 0,21-4-365,-17 4 316,0 0-1,-1 1 0,1-1 0,0 1 0,-1 0 1,1 0-1,7 3 0,-10-3 65,-1 0 0,1 1-1,-1-1 1,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0 0-1,0-1 1,-1 1 0,1 0 0,-1 0 0,1-1 0,-1 1-1,1 0 1,-1 0 0,0 0 0,0 0 0,0 0 0,0-1 0,0 1-1,-1 0 1,1 0 0,0 0 0,-1 0 0,1-1 0,-1 1-1,-1 2 1,0 0 39,0 1 1,0-1-1,0 0 0,-1 1 0,0-1 0,0 0 0,0 0 1,-1-1-1,-5 6 0,-3 1 3,-10 7-2187,3-9-3807,-1-4-6352</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9643.26">3475 97 1761,'0'0'14468,"-10"-13"-10701,-10 189-3020,20-164-861</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10149.05">3044 164 2481,'0'0'11035,"9"-5"-10294,30-15-149,-39 19-575,1 1 0,-1 0 0,0 0-1,1-1 1,-1 1 0,1 0 0,-1 0-1,1 0 1,-1 0 0,1-1 0,-1 1-1,1 0 1,-1 0 0,1 0 0,-1 0-1,0 0 1,1 0 0,-1 0 0,1 1-1,-1-1 1,1 0 0,-1 0 0,1 0-1,-1 0 1,1 1 0,-1-1 0,0 0-1,1 0 1,-1 1 0,1-1 0,-1 0-1,0 1 1,1-1 0,3 19 211,-10 20-4,-19-1-51,21-34-154,1 0 0,0 0 1,0 0-1,0 0 0,0 1 1,1-1-1,0 1 1,-1 0-1,2 0 0,-1 0 1,1 0-1,-2 9 0,4-14-16,0 1 1,0 0-1,0 0 0,0-1 0,0 1 0,0-1 0,1 1 0,-1-1 0,0 1 0,0-1 0,1 0 0,-1 1 0,0-1 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,2-1 0,35 1 147,-35 0-110,7-1-136,0 0 0,-1-1-1,1 0 1,-1 0 0,0-1-1,1 0 1,-1 0 0,0-1-1,14-9 1,-18 3-3983,-5 5-1582</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10149.04">3044 164 2481,'0'0'11035,"9"-5"-10294,30-15-149,-39 19-575,1 1 0,-1 0 0,0 0-1,1-1 1,-1 1 0,1 0 0,-1 0-1,1 0 1,-1 0 0,1-1 0,-1 1-1,1 0 1,-1 0 0,1 0 0,-1 0-1,0 0 1,1 0 0,-1 0 0,1 1-1,-1-1 1,1 0 0,-1 0 0,1 0-1,-1 0 1,1 1 0,-1-1 0,0 0-1,1 0 1,-1 1 0,1-1 0,-1 0-1,0 1 1,1-1 0,3 19 211,-10 20-4,-19-1-51,21-34-154,1 0 0,0 0 1,0 0-1,0 0 0,0 1 1,1-1-1,0 1 1,-1 0-1,2 0 0,-1 0 1,1 0-1,-2 9 0,4-14-16,0 1 1,0 0-1,0 0 0,0-1 0,0 1 0,0-1 0,1 1 0,-1-1 0,0 1 0,0-1 0,1 0 0,-1 1 0,0-1 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,2-1 0,35 1 147,-35 0-110,7-1-136,0 0 0,-1-1-1,1 0 1,-1 0 0,0-1-1,1 0 1,-1 0 0,0-1-1,14-9 1,-18 3-3983,-5 5-1582</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10720.15">2652 103 8788,'0'0'6619,"4"-17"-5949,-3 17-668,-1 0 0,1 1 1,0-1-1,0 0 0,0 0 1,0 1-1,0-1 1,-1 0-1,1 1 0,0-1 1,0 1-1,-1-1 0,1 1 1,0-1-1,-1 1 0,1-1 1,0 1-1,-1 0 0,1-1 1,-1 1-1,1 0 1,-1 0-1,1-1 0,-1 1 1,0 0-1,1 0 0,-1 0 1,0 0-1,0-1 0,0 1 1,1 0-1,-1 0 0,0 0 1,0 0-1,0 0 1,-1 0-1,1 0 0,0-1 1,0 1-1,-1 2 0,-11 52 291,3-19-205,10-34-85,0-1-1,-1 1 0,1-1 0,0 1 1,0-1-1,0 0 0,0 1 0,0-1 1,0 0-1,0 0 0,0 0 0,0 1 1,1-1-1,-1 0 0,0-1 0,1 1 1,-1 0-1,1 0 0,-1 0 0,1-1 1,-1 1-1,1-1 0,0 0 0,-1 1 1,1-1-1,-1 0 0,4 0 0,16 7 239,-21-7-235,1 0-1,-1 1 0,0-1 1,1 0-1,-1 0 0,0 1 1,0-1-1,0 0 0,1 1 1,-1-1-1,0 0 0,0 1 1,0-1-1,1 0 0,-1 1 1,0-1-1,0 0 0,0 1 1,0-1-1,0 0 0,0 1 1,0-1-1,0 1 0,0-1 0,0 0 1,0 1-1,0-1 0,0 1 1,0-1-1,-1 0 0,1 1 1,0-1-1,0 0 0,0 1 1,0-1-1,-1 0 0,1 1 1,0-1-1,0 0 0,-1 0 1,1 1-1,0-1 0,0 0 1,-1 0-1,1 1 0,0-1 1,-1 0-1,1 0 0,-1 1 1,-17 9 21,-12-1-1116,-2-5-3478,6-3-2031</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11304.96">2035 188 9076,'0'0'5736,"-9"23"-5269,8-20-426,0-1 0,1 1 1,0-1-1,-1 1 0,1-1 0,0 1 0,0-1 1,0 1-1,1-1 0,-1 1 0,1-1 0,-1 1 0,1-1 1,0 0-1,0 1 0,0-1 0,0 0 0,0 1 1,1-1-1,-1 0 0,1 0 0,-1 0 0,3 2 1,0-3-61,-1 1 0,1-1 0,0 0 0,0 1 0,-1-2 0,1 1 0,0 0 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 0,5 0 0,-7 1-28,-1-1-1,0 1 0,1 0 1,-1 0-1,1-1 1,-1 1-1,0-1 0,1 1 1,-1-1-1,0 0 1,1 0-1,-1 1 0,0-1 1,0 0-1,0 0 1,0 0-1,0 0 0,0 0 1,0-1-1,0 1 0,0 0 1,0 0-1,-1-1 1,1 1-1,0-3 0,-1 4 142,-1 29 149,-1-12-473,-14 56 1181,15-69-1258,-1 0 0,1-1 0,-1 1 0,1 0 0,-1-1 1,0 0-1,0 1 0,-1-1 0,1 0 0,0 0 0,-1 0 0,0 0 1,0-1-1,0 1 0,-5 3 0,-6 0-4423</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="11750.39">1667 177 9012,'0'0'5451,"-8"-3"-4747,1 0-537,4 2-121,1-1-1,0 1 1,-1 0-1,1 0 0,-1 0 1,1 1-1,-1-1 1,0 1-1,1-1 0,-5 1 1,12 30 362,31 2 169,-33-30-549,1 0 0,-1 0-1,0 0 1,0 0 0,0 1 0,0 0 0,0-1-1,0 1 1,-1 0 0,0 0 0,1 1 0,-1-1-1,0 0 1,0 1 0,-1-1 0,1 1-1,-1-1 1,0 1 0,0 0 0,1 4 0,-15-4-2305,3-5-3530,3-2 474</inkml:trace>
@@ -20408,7 +20498,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="48120.47">21 63 11621,'0'0'8559,"1"0"-8489,0-1 0,0 1 1,0 0-1,0 0 0,0 1 0,0-1 1,0 0-1,0 0 0,0 0 0,0 1 1,0-1-1,0 0 0,0 1 0,-1-1 1,1 1-1,0-1 0,1 2 0,0 13 184,0-1-1,1 1 1,0 0-1,8 20 1,5 25 77,16 214 515,-17-105-588,-9-52-125,-6-90-2798,1-74 166,-7-143-4848,4 163 6910,-2-1 0,-1 0-1,-2 1 1,-18-49 0,-6 7 1057,-13-33 3026,44 100-3497,-1 0 1,0 1-1,0-1 1,1 0-1,-1 0 1,1 1-1,0-1 1,-1 0-1,1 0 1,0 0-1,0 1 1,0-1-1,0 0 1,0 0-1,1 0 1,-1 0-1,1 1 1,-1-1-1,2-3 1,-1 5-32,0-1 0,-1 1 0,1-1 0,0 1 0,0 0 1,0-1-1,0 1 0,0 0 0,0 0 0,0 0 1,0-1-1,0 1 0,0 0 0,0 0 0,0 1 0,0-1 1,0 0-1,0 0 0,0 0 0,0 1 0,0-1 1,0 0-1,0 1 0,1 0 0,8 4 265,0 0-1,-1 0 1,0 1-1,16 14 1,24 24 164,-3-4-312,-1 2 1,54 67 0,-92-100-336,-4-4-53,0 1 1,1-1-1,0 0 1,0 0 0,0-1-1,1 1 1,0-1-1,0 0 1,0 0-1,6 3 1,-4-21-2679,-2-12 1981,-2 0-1,-1 0 0,-1 0 1,-4-36-1,1-1 590,2 32 444,-2 1-1,-6-38 1,4 52 1069,0 0 1,0 0-1,-9-17 1,12 30 1345,2 34-2160,26 152 803,-8-63-1090,-17-107-247,0 8 74,1 0-1,1-1 0,1 1 1,11 28-1,-14-45-174,-1-1-1,0 0 0,1 1 0,0-1 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,1 0 1,0-1-1,-1 1 0,1-1 0,0 0 0,0 0 1,0 0-1,1 0 0,-1 0 0,0-1 0,1 1 0,-1-1 1,1 0-1,-1 0 0,1 0 0,0-1 0,-1 1 1,1-1-1,0 0 0,-1 0 0,1 0 0,0-1 1,5 0-1,-6-1-35,1 0-1,-1 0 1,0 0 0,-1 0 0,1 0 0,0-1-1,-1 1 1,1-1 0,-1 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,-1 0-1,1 0 1,-1-1 0,0 1 0,0-1-1,0 1 1,-1-1 0,1 1 0,-1-5 0,4-14 216,-2 0 0,0-30 0,-1 33 712,0 14-126,0 0 0,-1 1 0,0-1 0,0 1 0,-1-1 0,1 0 1,-3-8-1,3 13-456,0-1 0,0 1 0,0-1 0,0 1 0,-1 0 0,1-1 0,0 1 1,0-1-1,-1 1 0,1 0 0,0-1 0,-1 1 0,1 0 0,0-1 0,-1 1 0,1 0 1,0 0-1,-1 0 0,1-1 0,0 1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1-1 0,1 1 1,0 0-1,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 1 1,0-1-1,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1 1 0,1-1 0,-1 0 1,1 0-1,0 1 0,-1-1 0,1 1 0,-2 0-49,1 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,0 0 0,0 0-1,1 1 1,-1-1-1,1 0 1,-1 1 0,1-1-1,-1 0 1,1 1 0,0-1-1,-1 2 1,1-1-53,0 0-1,0 1 1,0-1 0,0 0-1,0 1 1,0-1 0,1 0-1,-1 0 1,1 1 0,0-1-1,-1 0 1,1 0 0,0 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,1 0 0,-1 0-1,1-1 1,-1 1 0,1 0-1,0-1 1,0 0 0,-1 1-1,1-1 1,0 0 0,0 0-1,1 0 1,-1 0 0,0 0-1,0 0 1,0-1 0,1 1 0,-1-1-1,0 0 1,0 0 0,1 1-1,-1-1 1,0-1 0,1 1-1,-1 0 1,0-1 0,1 1-1,-1-1 1,0 1 0,0-1-1,4-2 1,-3 1-8,-1 0-1,1 1 1,-1-1 0,0-1 0,0 1-1,0 0 1,0 0 0,0-1 0,0 1 0,0-1-1,-1 0 1,0 0 0,1 1 0,-1-1-1,0 0 1,0 0 0,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 0 0,0 0-1,0 0 1,0 0 0,0-1 0,-1 1-1,1 0 1,-3-5 0,2 7-1,1 0 1,-1-1-1,0 1 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,-1 0 0,1 0 1,0 0-1,0 0 0,-1 1 1,1-1-1,0 0 0,-1 1 1,1-1-1,-1 1 0,1-1 1,-1 1-1,1 0 1,-1 0-1,1 0 0,-3 0 1,-48 0 62,36 0-56,16 0-9,-1 0-40,-1 0 1,1-1-1,0 1 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 1,-1 0-1,1 0 0,0 0 1,0 0-1,0 0 1,0 1-1,0-1 0,0 0 1,0 1-1,0-1 1,0 1-1,0-1 0,0 1 1,0 0-1,0-1 1,0 1-1,0 0 0,0 0 1,0 0-1,1-1 1,-1 1-1,0 0 0,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,-1 2 1,22-5-4542,-12-2 3412,-1 0 0,0-1 0,0 0 0,0-1 0,-1 0 0,1 0 0,-1 0 0,-1-1 0,1 0 0,-1-1 0,5-8 0,19-24-2150</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="48323.86">716 121 144,'0'0'15559,"0"-20"-12987,0-60-664,0 60-590,0 32 111,0-9-1405,-1 69 146,3 0 1,3 0-1,19 95 0,-20-148-1813,1-1 1,14 34-1,-17-47-847</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="48483.57">752 409 2945,'0'0'10453,"-42"-127"-8308,42 96-544,0-3-273,6 3-671,24-3-401,6 6-48,0 4 224,0 4-256,-12 16-176,-6 4-304,-12 7-752,-6 34-1714,0 14-3873</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="49454.26">656 1156 11989,'0'0'8562,"9"20"-7540,-9-19-1016,10 18 175,-2 1 0,-1 0 0,0 1 0,-1-1 0,-2 1 0,0 0 0,1 27 0,-5 95 227,0-143-407,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 1 0,0-1 1,0 0-1,-1 0 0,1 0 0,0 0 1,0 0-1,0 0 0,0 1 0,0-1 0,0 0 1,-1 0-1,1 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 0,0 0 1,0 0-1,-1 0 0,1 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 0,0 0 1,0-1-1,0 1 0,-1 0 0,1 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0 0 1,0-1-1,0 1 0,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 0,0-1 1,0 1-1,0 0 0,0 0 0,0 0 0,0 0 1,0 0-1,0-1 0,0 1 0,-3-7 16,-1 0 0,1-1 0,1 1 0,-1-1 0,1 0 0,0 0 0,1 1 0,-1-15 0,1-76-54,1 66 36,0 12-4,0-19 5,1-1 0,9-54 1,-8 82-15,0 1 0,1 0 1,1 0-1,0 0 1,0 0-1,1 1 0,1 0 1,-1-1-1,2 2 1,-1-1-1,1 1 0,15-15 1,-1 9-44,-20 14 55,-1 1 1,0 0-1,0-1 0,1 1 0,-1 0 0,0 0 1,0-1-1,1 1 0,-1 0 0,0 0 1,1-1-1,-1 1 0,0 0 0,1 0 1,-1 0-1,1 0 0,-1 0 0,0-1 1,1 1-1,-1 0 0,0 0 0,1 0 0,-1 0 1,1 0-1,-1 0 0,0 0 0,1 0 1,-1 0-1,1 1 0,-1-1 0,0 0 1,1 0-1,-1 0 0,0 0 0,1 0 0,-1 1 1,0-1-1,1 0 0,-1 0 0,0 1 1,1-1-1,-1 0 0,0 0 0,0 1 1,1-1-1,-1 0 0,0 1 0,0-1 0,0 0 1,1 1-1,-1-1 0,0 1 0,0-1 1,0 0-1,0 1 0,0 0 0,-2 18-15,-1 1 0,-1-1 0,0 0 0,-2-1-1,0 1 1,-1-1 0,-1 0 0,0-1 0,-14 21 0,7-11-133,1 2 0,-18 50 0,32-78 152,0 0 1,0-1 0,0 1-1,0 0 1,0 0 0,0 0-1,1 0 1,-1 0 0,0 0-1,0-1 1,1 1 0,-1 0-1,0 0 1,1 0 0,-1-1-1,1 1 1,-1 0 0,1 0-1,0-1 1,-1 1 0,1 0-1,-1-1 1,1 1 0,0-1-1,0 1 1,-1-1 0,1 1-1,0-1 1,0 0 0,0 1-1,0-1 1,-1 0 0,1 1-1,0-1 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,-1 0 0,2-1-1,56 1 176,-38-1-113,238-10 680,-225 9-679,2 2 22,-33 0-266,-2 3-524,-3 12-1448,-12 8-3013</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="49454.25">656 1156 11989,'0'0'8562,"9"20"-7540,-9-19-1016,10 18 175,-2 1 0,-1 0 0,0 1 0,-1-1 0,-2 1 0,0 0 0,1 27 0,-5 95 227,0-143-407,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 1 0,0-1 1,0 0-1,-1 0 0,1 0 0,0 0 1,0 0-1,0 0 0,0 1 0,0-1 0,0 0 1,-1 0-1,1 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 0,0 0 1,0 0-1,-1 0 0,1 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 0,0 0 1,0-1-1,0 1 0,-1 0 0,1 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0 0 1,0-1-1,0 1 0,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 0,0-1 1,0 1-1,0 0 0,0 0 0,0 0 0,0 0 1,0 0-1,0-1 0,0 1 0,-3-7 16,-1 0 0,1-1 0,1 1 0,-1-1 0,1 0 0,0 0 0,1 1 0,-1-15 0,1-76-54,1 66 36,0 12-4,0-19 5,1-1 0,9-54 1,-8 82-15,0 1 0,1 0 1,1 0-1,0 0 1,0 0-1,1 1 0,1 0 1,-1-1-1,2 2 1,-1-1-1,1 1 0,15-15 1,-1 9-44,-20 14 55,-1 1 1,0 0-1,0-1 0,1 1 0,-1 0 0,0 0 1,0-1-1,1 1 0,-1 0 0,0 0 1,1-1-1,-1 1 0,0 0 0,1 0 1,-1 0-1,1 0 0,-1 0 0,0-1 1,1 1-1,-1 0 0,0 0 0,1 0 0,-1 0 1,1 0-1,-1 0 0,0 0 0,1 0 1,-1 0-1,1 1 0,-1-1 0,0 0 1,1 0-1,-1 0 0,0 0 0,1 0 0,-1 1 1,0-1-1,1 0 0,-1 0 0,0 1 1,1-1-1,-1 0 0,0 0 0,0 1 1,1-1-1,-1 0 0,0 1 0,0-1 0,0 0 1,1 1-1,-1-1 0,0 1 0,0-1 1,0 0-1,0 1 0,0 0 0,-2 18-15,-1 1 0,-1-1 0,0 0 0,-2-1-1,0 1 1,-1-1 0,-1 0 0,0-1 0,-14 21 0,7-11-133,1 2 0,-18 50 0,32-78 152,0 0 1,0-1 0,0 1-1,0 0 1,0 0 0,0 0-1,1 0 1,-1 0 0,0 0-1,0-1 1,1 1 0,-1 0-1,0 0 1,1 0 0,-1-1-1,1 1 1,-1 0 0,1 0-1,0-1 1,-1 1 0,1 0-1,-1-1 1,1 1 0,0-1-1,0 1 1,-1-1 0,1 1-1,0-1 1,0 0 0,0 1-1,0-1 1,-1 0 0,1 1-1,0-1 1,0 0 0,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,-1 0 0,2-1-1,56 1 176,-38-1-113,238-10 680,-225 9-679,2 2 22,-33 0-266,-2 3-524,-3 12-1448,-12 8-3013</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="50501">110 2094 9044,'0'0'15815,"0"5"-15809,5 58 109,2 1 0,24 99 1,-13-75 69,72 272 15,-90-360-246,0 1 0,1-1 0,-1 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,1-1 0,-1 0 0,0 1 0,0-1 0,1 0 0,-1 0 0,0 1 0,0-1 0,1 0 0,-1 0 0,0 1 0,1-1-1,-1 0 1,0 0 0,1 0 0,-1 0 0,0 0 0,1 1 0,-1-1 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0-1 0,1 1 0,-1 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,1-1 0,-1 1 0,0 0 0,1 0 0,-1-1 0,0 1 0,0 0 0,1 0 0,-1-1 0,0 0 0,1-64-6698,-1 19 39</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="51424.94">117 2310 8308,'0'0'3804,"-7"-21"-1251,-21-71-197,27 86-2028,-1 0 0,1 0 0,0 0 0,0 0 0,1-1 0,0 1-1,0 0 1,1-10 0,0 14-245,-1 0-1,1 0 0,0 0 1,0 0-1,-1 0 1,1 0-1,0 0 0,1 0 1,-1 1-1,0-1 1,0 0-1,1 1 0,-1-1 1,1 1-1,-1-1 1,1 1-1,3-2 0,2 0 11,1 1 0,0 0-1,0 0 1,0 1 0,0-1-1,0 2 1,1-1 0,-1 1-1,13 2 1,-18-2-67,8 1 16,0 1 1,0 0-1,-1 1 1,1 0-1,-1 1 1,0 0-1,0 0 1,0 1-1,-1 1 1,0-1 0,0 2-1,0-1 1,-1 1-1,0 0 1,0 1-1,0 0 1,-1 0-1,8 13 1,1 1 19,-2 0 0,0 2 0,-2-1 0,0 2 1,-2 0-1,11 37 0,-12-29-393,-2 1 1,-1-1-1,-1 1 1,-3 1-1,0-1 1,-2 0-1,-6 40 1,6-71 152,0 0 0,0-1 0,-1 1 0,1 0 0,-1-1-1,0 1 1,1 0 0,-1-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,-1 0 0,1 0 0,-1 1 0,0-1 0,0 0 0,0 0-1,0-1 1,0 1 0,0 0 0,0-1 0,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1-1-1,0 1 1,0-1 0,1 0 0,-1 0 0,0 0 0,-3 0 0,-1-1 179,0-1 0,0 0 0,0 0 0,1 0 0,-1-1-1,1 0 1,-1 0 0,1 0 0,0-1 0,0 0 0,0 0 0,-10-10 0,11 8 345,0 0 0,0 1 1,1-2-1,0 1 0,0 0 0,0-1 0,1 0 1,-1 0-1,2 0 0,-1 0 0,1 0 1,0 0-1,1-1 0,0 1 0,-1-11 1,2 11-276,0 0 1,1-1 0,0 1-1,0 0 1,1 0 0,0 0-1,0 0 1,0 0 0,1 1-1,4-9 1,9-12 111,32-43 0,-40 60-81,0 1 0,0 0 0,1 0 0,0 1 0,1 0 0,0 1 0,13-9 0,-19 14-44,-1 0 0,1 1 0,-1-1 0,1 1 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,-1 1 0,1 0 0,0 0 0,0 0 0,0 0-1,0 1 1,0-1 0,-1 1 0,1 0 0,0 0 0,0 0 0,-1 1 0,1-1 0,-1 1 0,1 0 0,-1 0 0,0 0 0,0 1 0,0-1 0,5 5 0,3 7 61,0 0-1,0 1 1,-1 0-1,-1 0 1,9 22-1,14 21 14,-28-50-115,-3-6-15,0 0 1,0 0-1,-1 0 0,1 0 0,1-1 0,-1 1 1,0 0-1,0-1 0,0 1 0,1-1 0,-1 1 1,1-1-1,0 0 0,-1 1 0,1-1 1,0 0-1,-1 0 0,3 1 0,-3-3-5,0 0-1,0 0 1,0 1 0,0-1-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 0-1,-1 0 1,1 0 0,-1-1-1,1 1 1,-1 0 0,1 0-1,-1 0 1,0 0 0,0-1-1,1 1 1,-1 0-1,0 0 1,0-3 0,4-31 11,-2 11 8,1 0 1,1 0 0,12-42 0,-16 66-17,1-1 0,-1 0 0,0 0 0,0 0 0,1 1 1,-1-1-1,0 0 0,1 0 0,-1 1 0,1-1 0,-1 0 1,1 1-1,-1-1 0,1 1 0,-1-1 0,1 1 0,0-1 1,-1 1-1,1-1 0,0 1 0,0-1 0,-1 1 0,1 0 1,0-1-1,0 1 0,-1 0 0,1 0 0,0 0 0,0-1 1,0 1-1,0 0 0,-1 0 0,1 0 0,0 0 1,0 1-1,0-1 0,-1 0 0,1 0 0,0 0 0,0 1 1,0-1-1,-1 0 0,1 1 0,0-1 0,-1 1 0,1-1 1,0 1-1,38 33-3,-23-19 24,-10-11-67,0 0 0,0-1 1,0 0-1,0 0 0,1 0 0,-1-1 0,1 0 0,-1 0 0,1-1 0,0 0 0,0 0 1,0 0-1,0-1 0,0 0 0,-1-1 0,1 1 0,0-1 0,0-1 0,10-2 1,-12 2-23,0 0-1,-1 0 1,1 0 0,-1 0 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 0,-1-1 0,0 1 0,1-1 0,-1 0 0,0 0 0,-1 0 0,1 0 0,-1-1 0,0 1 0,0-1 0,0 1 0,-1-1 0,1 0 0,-1 0 0,0 1 0,-1-1 0,1 0 0,-1-8 0,0 12 66,0-1 1,-1 1 0,1 0 0,0 0 0,-1-1 0,1 1-1,-1 0 1,0 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,0 0-1,0 1 1,0-1 0,-1 1 0,1-1 0,0 1 0,0-1-1,0 1 1,-1-1 0,1 1 0,0 0 0,-1 0 0,1 0 0,0 0-1,0 0 1,-1 0 0,1 0 0,-2 0 0,-2 0 54,1 1 1,-1-1 0,0 1-1,1 0 1,-1 0-1,1 0 1,0 0 0,-1 1-1,1 0 1,-6 3-1,3 1 25,-1 1 0,1 0 0,1 1 0,-1-1 0,1 1 0,1 0 0,0 1 0,0-1 0,0 1 0,1 0 0,0 1 0,1-1 0,0 0 0,1 1 0,0 0 0,0-1 0,1 1 0,0 0 0,1 0 0,0 0 0,1 10 0,0-18-80,-1-1 0,1 0 0,-1 0 1,1 0-1,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0-1 1,0 1-1,0-1 0,1 1 0,-1-1 0,0 0 0,0 1 1,1-1-1,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 1,1 0-1,-1 0 0,0-1 0,0 1 0,1 0 0,-1-1 0,0 1 1,0-1-1,2 0 0,2 0-38,-1-1 1,1 0-1,0 0 1,0 0-1,-1 0 1,1-1-1,-1 0 0,0 0 1,6-5-1,-1-3-11,-1-1 0,0 0 1,0-1-1,-2 0 0,1 0 0,-2 0 0,0-1 0,0 1 0,-1-1 0,1-15 0,0 3 60,-2-1 1,-2 1 0,0 0-1,-5-47 1,2 62 48,0 0 0,-1 0 0,-1 0 0,0 1 0,0 0 0,-1-1 0,0 2 0,-1-1 0,0 0-1,0 1 1,-1 0 0,0 1 0,-12-11 0,1 9 518,18 10-561,-1 0 0,1 0 0,-1 0 0,1 0-1,0 1 1,-1-1 0,1 0 0,-1 0 0,1 1 0,0-1 0,-1 0 0,1 0-1,0 1 1,-1-1 0,1 0 0,0 1 0,0-1 0,-1 1 0,1-1-1,0 0 1,0 1 0,0-1 0,-1 1 0,1-1 0,0 0 0,0 1 0,0 0-1,-1 43 340,2-29-395,0 7 83,0 1 0,2-1 1,0 0-1,2 0 0,0-1 1,2 1-1,0-1 0,1-1 1,20 37-1,-19-42-346,1 0 0,1 0 0,0-1 0,1-1 0,18 17 0,-20-21-570,2 0-1,-1-1 0,1 0 0,1-1 1,-1 0-1,1-1 0,16 5 0,20 0-4970</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="51714.55">1502 2105 9300,'0'0'13292,"7"3"-12559,1-1-655,0 0-1,0 0 0,0-1 0,1 0 1,-1-1-1,0 1 0,0-1 0,1-1 0,-1 0 1,0 0-1,0-1 0,0 0 0,0 0 1,0 0-1,0-1 0,0-1 0,-1 1 1,0-1-1,8-6 0,18-9-38,-1-1 0,-1-2 0,-1-1 1,-1-2-1,36-38 0,-63 60-184,1-1 0,-1 1 0,0-1 0,0 1 1,0-1-1,0 0 0,-1 1 0,0-1 0,0 0 0,0 0 1,0 0-1,0 0 0,-1-1 0,0 1 0,0 0 0,0 0 1,0 0-1,0 0 0,-1 0 0,-1-5 0,0 3-1039,0 0-1,0 1 1,-1-1-1,1 1 1,-1-1-1,0 1 1,-7-8-1,-9-14-9833</inkml:trace>
@@ -20478,7 +20568,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">186 233 12998,'0'0'8572,"-6"13"-8068,-1 2-332,1 1 0,1 0-1,0 1 1,1-1 0,1 1 0,0-1-1,0 26 1,2-31-111,1 1 1,1-1-1,0 0 1,0 0-1,1 0 0,0 0 1,1-1-1,5 14 0,24 65 310,-35-103-15,-9-14-301,-17-18-37,3 0-1,2-2 1,2 0-1,1-2 1,4 0-1,-15-63 1,30 103-22,0 1 0,1-1 0,0 0 1,1 1-1,0-1 0,0 0 0,1 1 0,2-12 0,-2 18-3,0 0-1,0 0 1,1 0-1,-1 0 0,1 0 1,-1 0-1,1 0 0,0 1 1,0-1-1,0 1 1,1-1-1,-1 1 0,0 0 1,1 0-1,0 0 0,-1 0 1,1 0-1,0 1 1,0-1-1,0 1 0,0 0 1,0 0-1,0 0 1,0 0-1,1 0 0,3 0 1,2 0-71,1-1 1,-1 1-1,1 1 1,0 0-1,-1 0 1,1 1-1,-1 0 0,1 1 1,-1 0-1,0 0 1,1 1-1,11 5 1,-15-4-235,0-1 0,-1 1 0,1 0 0,-1 0 0,0 0 0,-1 1 0,1 0 0,-1 0 0,0 0-1,0 1 1,0-1 0,-1 1 0,1 0 0,-2 0 0,1 0 0,-1 0 0,1 0 0,1 12 0,3 34-4594,-6-3-2377</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="644.34">43 541 12694,'0'0'5485,"12"-20"-4669,-1-2-596,-7 13-145,0 0 0,1 1 0,0-1 1,1 1-1,0 0 0,0 1 1,0-1-1,1 1 0,0 1 0,1-1 1,-1 1-1,13-7 0,-3 2 66,1 1 0,0 1 0,1 1 0,33-11 1,-40 17-596,0-1 1,0 1 0,-1 1-1,1 0 1,19 2 0,-30-1 250,1 1 0,-1-1 0,1 1 0,-1 0 0,1-1-1,-1 1 1,1 0 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 1 0,0-1 0,0 0 0,0 1-1,0-1 1,-1 1 0,1-1 0,0 0 0,-1 1 0,1 0 0,-1-1 0,1 1 0,-1-1 0,0 1 0,1 0-1,-1-1 1,0 1 0,0 2 0,0 2-359,0 0 1,0-1-1,0 1 0,-1 0 0,0 0 0,0-1 1,0 1-1,-3 8 0,-5 2 315,-1-1 0,0 0 0,-1 0 0,-1-1 0,-23 22 0,17-17 2432,0 0-1,-21 32 1,28-38-702,10-11-1277,0-1 1,0 0-1,0 1 0,-1-1 0,1 0 1,1 1-1,-1 0 0,0-1 0,0 1 1,0-1-1,1 1 0,-1 0 1,1 0-1,-1-1 0,1 4 0,15-4 141,0-3-593,1 0-1,-1 0 1,0-1 0,0-1-1,-1-1 1,1 0-1,-1-1 1,0-1 0,0 0-1,18-13 1,22-16-2845,54-50 1,-88 69 2414,-13 11 603,7-5 163,1 0 1,-2-2-1,0 0 1,0 0-1,-1-1 1,13-20-1,-25 33 98,1 0 0,0 0 0,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 0-1,0 0 1,1 0 0,-1 0 0,0 0 0,0 0 0,1 1 0,-1-1 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0-1,-1 0 1,1 0 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,0 1 0,1-1-1,-1 0 1,0 1 0,0-1 0,0 0 0,1 1 0,-1-1 0,0 1 0,0 0 0,0-1 0,0 1-1,0 0 1,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,-1 0 0,-3-1 163,-1 1 0,1 0 0,0 0 0,0 0 0,-1 1 0,1 0 0,0 0 0,-9 3 0,7-1-248,0 1-1,1 0 1,-1 0-1,1 0 1,0 1-1,0 0 1,1 0 0,-1 1-1,1 0 1,1 0-1,-9 12 1,-2 8-45,-21 47 0,22-42-33,14-30-194,-1 0 1,1 0 0,-1 0-1,1 1 1,-1-1 0,1 0-1,-1 0 1,1 0-1,-1 0 1,0 0 0,0 0-1,1 0 1,-1 0 0,0-1-1,0 1 1,0 0 0,0 0-1,-2 0 1,2-2-62,0 0 0,0 0 0,0 0 0,0 0-1,0-1 1,1 1 0,-1 0 0,0-1 0,1 1 0,-1 0 0,0-1 0,1 1 0,0-1-1,-1 1 1,1-3 0,-10-29-1206,-9-31 584,17 57 1347,-1 0 1,0 0-1,-1 0 0,1 1 1,-2-1-1,-5-7 2369,20 15-2226,5 3-572,-1 1 1,1 1-1,-1 1 0,0 0 0,-1 0 0,16 12 1,39 20-643,-50-31-261,1 0-1,0-2 1,0 0 0,29 5 0,39-5-5817,-39-6 1103</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="644.32">43 541 12694,'0'0'5485,"12"-20"-4669,-1-2-596,-7 13-145,0 0 0,1 1 0,0-1 1,1 1-1,0 0 0,0 1 1,0-1-1,1 1 0,0 1 0,1-1 1,-1 1-1,13-7 0,-3 2 66,1 1 0,0 1 0,1 1 0,33-11 1,-40 17-596,0-1 1,0 1 0,-1 1-1,1 0 1,19 2 0,-30-1 250,1 1 0,-1-1 0,1 1 0,-1 0 0,1-1-1,-1 1 1,1 0 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 1 0,0-1 0,0 0 0,0 1-1,0-1 1,-1 1 0,1-1 0,0 0 0,-1 1 0,1 0 0,-1-1 0,1 1 0,-1-1 0,0 1 0,1 0-1,-1-1 1,0 1 0,0 2 0,0 2-359,0 0 1,0-1-1,0 1 0,-1 0 0,0 0 0,0-1 1,0 1-1,-3 8 0,-5 2 315,-1-1 0,0 0 0,-1 0 0,-1-1 0,-23 22 0,17-17 2432,0 0-1,-21 32 1,28-38-702,10-11-1277,0-1 1,0 0-1,0 1 0,-1-1 0,1 0 1,1 1-1,-1 0 0,0-1 0,0 1 1,0-1-1,1 1 0,-1 0 1,1 0-1,-1-1 0,1 4 0,15-4 141,0-3-593,1 0-1,-1 0 1,0-1 0,0-1-1,-1-1 1,1 0-1,-1-1 1,0-1 0,0 0-1,18-13 1,22-16-2845,54-50 1,-88 69 2414,-13 11 603,7-5 163,1 0 1,-2-2-1,0 0 1,0 0-1,-1-1 1,13-20-1,-25 33 98,1 0 0,0 0 0,-1 1 0,1-1 0,-1 0 0,1 0 0,-1 0-1,0 0 1,1 0 0,-1 0 0,0 0 0,0 0 0,1 1 0,-1-1 0,0 0 0,0 0 0,0 0-1,0 0 1,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0-1,-1 0 1,1 0 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,0 1 0,1-1-1,-1 0 1,0 1 0,0-1 0,0 0 0,1 1 0,-1-1 0,0 1 0,0 0 0,0-1 0,0 1-1,0 0 1,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,-1 0 0,-3-1 163,-1 1 0,1 0 0,0 0 0,0 0 0,-1 1 0,1 0 0,0 0 0,-9 3 0,7-1-248,0 1-1,1 0 1,-1 0-1,1 0 1,0 1-1,0 0 1,1 0 0,-1 1-1,1 0 1,1 0-1,-9 12 1,-2 8-45,-21 47 0,22-42-33,14-30-194,-1 0 1,1 0 0,-1 0-1,1 1 1,-1-1 0,1 0-1,-1 0 1,1 0-1,-1 0 1,0 0 0,0 0-1,1 0 1,-1 0 0,0-1-1,0 1 1,0 0 0,0 0-1,-2 0 1,2-2-62,0 0 0,0 0 0,0 0 0,0 0-1,0-1 1,1 1 0,-1 0 0,0-1 0,1 1 0,-1 0 0,0-1 0,1 1 0,0-1-1,-1 1 1,1-3 0,-10-29-1206,-9-31 584,17 57 1347,-1 0 1,0 0-1,-1 0 0,1 1 1,-2-1-1,-5-7 2369,20 15-2226,5 3-572,-1 1 1,1 1-1,-1 1 0,0 0 0,-1 0 0,16 12 1,39 20-643,-50-31-261,1 0-1,0-2 1,0 0 0,29 5 0,39-5-5817,-39-6 1103</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1441.72">991 346 6355,'0'0'6600,"-6"-22"-4786,-22-66-109,27 86-1605,0 0 1,0 1-1,1-1 0,-1 0 0,0 0 0,-1 1 1,1-1-1,0 0 0,0 1 0,-1-1 0,1 1 0,-1 0 1,1-1-1,-1 1 0,0 0 0,1 0 0,-1 0 1,0 0-1,0 0 0,0 1 0,0-1 0,1 0 1,-1 1-1,0 0 0,0-1 0,0 1 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 1 0,0-1 1,-3 1-1,2 0-28,0 0 1,0 0 0,0 0-1,1 1 1,-1-1-1,0 1 1,1-1 0,-1 1-1,1 0 1,-1 0-1,1 0 1,0 0 0,0 0-1,0 1 1,0-1-1,-2 5 1,0 3 0,2-1-1,-1 1 1,1-1-1,1 1 1,0 0-1,0 0 1,1 0-1,0 0 1,0-1-1,1 1 1,1 0 0,2 10-1,-3-17-75,1 1 0,-1-1 0,1 1 0,-1-1 0,1 0 0,0 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,1-1 0,0 1 0,-1-1 0,1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,1-1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1-1 0,0 1 0,-1-1 0,1 0 0,0 0 0,-1-1 0,1 1 0,0-1 0,-1 0 0,5-1 0,-4 0-17,1 0 1,0 0-1,-1 0 0,1-1 0,-1 0 0,0 0 1,0 0-1,0 0 0,0-1 0,-1 1 0,1-1 1,-1 0-1,0 0 0,0-1 0,0 1 0,2-6 1,18-22 6,-23 32 16,1 0 0,0 0 0,-1 0 0,1 0 1,0 0-1,0 0 0,-1 0 0,1 0 0,0 1 1,-1-1-1,1 0 0,0 0 0,-1 1 0,1-1 1,0 0-1,-1 1 0,1-1 0,-1 0 0,1 1 1,-1-1-1,1 1 0,-1-1 0,1 1 0,-1-1 1,1 1-1,-1 0 0,1-1 0,-1 1 0,0-1 1,0 1-1,1 0 0,-1-1 0,0 1 0,0 1 1,15 25 185,-14-27-176,13 35 191,-12-27-168,0-1 1,1 0-1,0 1 0,0-1 0,0-1 1,1 1-1,0 0 0,1-1 0,-1 0 1,1 0-1,0 0 0,10 7 0,-15-13-32,1 0-1,-1 1 0,1-1 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1 0 1,0 0-1,-1 0 0,1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1 0 1,0 0-1,-1-1 0,1 1 0,-1 0 0,1 0 0,0-1 0,-1 1 0,1 0 1,-1-1-1,1 1 0,-1-1 0,0 1 0,1-1 0,-1 1 0,1-1 1,-1 0-1,14-21 8,-8 13-19,-4 5-1,0 1-1,1 0 1,0 0-1,0 0 1,0 1-1,0-1 1,0 1-1,1-1 1,-1 1-1,0 0 1,1 0-1,5-1 1,-8 2 6,1 1 0,-1 0 0,1-1 0,0 1 0,-1 0 0,1 0 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1 1 0,-1-1 0,1 1 0,-1-1 0,1 1 1,-1 0-1,1 0 0,-1-1 0,0 1 0,0 0 0,1 0 0,-1 0 0,0 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 1 0,-1-1 0,1 1 0,0-1 0,-1 0 0,2 4 0,20 74 70,-17-70 23,0-16-66,4-22-57,-8 25 29,6-23-200,1 0 0,2 0 0,18-35 0,-28 61 200,1-1 0,0 1 0,0-1-1,0 1 1,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,1 0-1,-1 0 1,0 0 0,1 0 0,-1 0 0,1 1 0,-1-1 0,3 0-1,-4 1 10,1 0 0,0 0 0,0 0-1,0 0 1,-1 0 0,1 1 0,0-1-1,-1 0 1,1 1 0,0-1 0,-1 0-1,1 1 1,0-1 0,-1 1-1,1-1 1,-1 1 0,1-1 0,0 1-1,-1-1 1,0 1 0,1 0 0,-1-1-1,1 1 1,-1 0 0,0-1 0,1 1-1,-1 0 1,0 0 0,0-1 0,1 1-1,-1 0 1,0 0 0,0-1-1,0 1 1,0 0 0,0 0 0,0 1-1,2 23 244,12 71 142,-13-88-374,1 0 0,1 0-1,0 0 1,0 0 0,1 0 0,-1-1-1,2 1 1,-1-1 0,6 7-1,-9-13-15,-1 0 0,1 0-1,0 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,0 0 0,0-1-1,0 1 1,-1 0-1,1-1 1,0 1-1,0 0 1,0-1 0,0 1-1,0-1 1,0 0-1,0 1 1,0-1-1,0 0 1,0 1 0,0-1-1,1 0 1,-1 0-1,0 0 1,0 0-1,0 0 1,0 0 0,0 0-1,0-1 1,0 1-1,0 0 1,0 0-1,0-1 1,0 1 0,0-1-1,0 1 1,0-1-1,0 1 1,0-1-1,0 0 1,0 0 0,0 1-1,-1-1 1,1 0-1,0 0 1,-1 0-1,1 0 1,0 0 0,-1 1-1,1-1 1,-1 0-1,0 0 1,1-1-1,-1 1 1,1-1 0,4-11-1,-1 0 0,0 0 1,3-24-1,-5 21 26,-2 16-20,0-1 1,1 1 0,-1-1-1,0 1 1,0-1-1,0 1 1,0-1 0,0 0-1,0 1 1,1-1-1,-1 1 1,0 0 0,0-1-1,1 1 1,-1-1-1,0 1 1,1-1 0,-1 1-1,1 0 1,-1-1-1,0 1 1,1 0 0,-1-1-1,1 1 1,-1 0-1,1-1 1,-1 1 0,1 0-1,-1 0 1,1 0-1,0-1 1,16 11 71,17 32-44,-28-33-5,0-3-162,-1 1 0,1-1 0,0-1 0,0 1 0,1-1-1,0 0 1,-1 0 0,2-1 0,-1 0 0,0 0 0,1 0 0,14 3-1,-8-4-1257,-1 0-1,1-1 0,0-1 0,16 0 0,29-1-9791</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1912.94">2075 386 15063,'0'0'7972,"22"-4"-7514,114-14-119,143-25-1366,-261 39 452,45-13-2658,-26-2-2315,-31 10-2478,-17 5 5916,-21 2 3581,29 2-1826,-27-1 3538,-1-2 0,-45-10 0,6 0 3099,136 13-4209,-31-2-2147,43 5 1,-60-2 66,0 2-1,-1 0 1,0 1 0,1 1-1,-1 0 1,16 9 0,-29-12 12,0 0 0,0 0 0,0 0 0,-1 1 0,1-1 0,-1 1 0,0 0 0,0 0 1,0 0-1,0 1 0,-1-1 0,1 1 0,-1-1 0,0 1 0,0 0 0,0 0 0,0 0 0,-1 0 1,0 0-1,1 0 0,-2 1 0,1-1 0,0 0 0,-1 0 0,0 1 0,0-1 0,0 0 1,0 1-1,-1-1 0,-1 5 0,-3 7 18,-1-1 0,0 0 1,-1 0-1,0-1 0,-2 0 1,0 0-1,0-1 0,-1 0 1,-1 0-1,-13 12 0,-25 32-196,13-10-1407,5-10-3161</inkml:trace>
 </inkml:ink>
@@ -20521,10 +20611,10 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6343.96">3846 671 9316,'0'0'7284,"27"1"-6100,-6 0-922,-10-2-165,0 1 0,-1 1 0,1 0 0,-1 0-1,1 1 1,-1 0 0,1 1 0,-1 0 0,0 0 0,0 1 0,0 1 0,-1 0 0,0 0 0,15 11 0,-7-2 193,-1 0 0,0 2 0,14 18 0,-25-27-205,0 0 1,-1 0-1,0 0 0,0 0 1,0 0-1,-1 1 1,-1 0-1,1-1 0,-1 1 1,0 0-1,1 14 1,-3-13-31,1 1 0,-2-1 0,1 0 0,-1 0 0,0 0 1,-1 0-1,0 0 0,-1 0 0,1 0 0,-2-1 0,-7 16 0,7-18-50,0-1 0,0 0 0,0 1-1,-1-2 1,1 1 0,-1 0 0,0-1-1,-1 0 1,1 0 0,-1-1-1,0 0 1,0 1 0,0-2 0,0 1-1,0-1 1,-1 0 0,-7 1 0,-15 1-903,14-9-4135,9-9-983</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="6778.79">4477 740 12662,'0'0'10218,"10"4"-9847,0 1-253,1 0 0,-1 1 0,0 1 0,-1-1 0,0 2 0,0-1 0,0 1 0,-1 0 0,0 1 0,9 13 0,10 17 181,30 56 0,-34-52 0,30 40 0,-52-83-287,-1 0 0,0 0 0,1 0 0,-1 1 0,0-1-1,1 0 1,-1 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0-1,1 0 1,-1 0 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,1 0-1,-1 0 1,0-1 0,1 1 0,-1 0 0,0 0 0,1 0 0,-1-1 0,0 1-1,1 0 1,-1 0 0,0-1 0,0 1 0,1 0 0,-1 0 0,0-1 0,0 1 0,0 0-1,1-1 1,-1 1 0,0 0 0,0-1 0,15-23 86,-11 16 1,345-505 73,-273 419-377,4 5 0,3 2 0,111-87 0,-162 146 17,-23 19 17,-1 1 0,2 0 0,-1 1-1,1-1 1,0 2 0,0 0 0,1 0 0,0 1 0,12-5 0,-23 10 99,1 0 1,-1 1 0,0-1 0,0 0 0,0 0 0,1 0-1,-1 1 1,0-1 0,0 0 0,0 0 0,0 0-1,1 1 1,-1-1 0,0 0 0,0 0 0,0 1 0,0-1-1,0 0 1,0 0 0,0 1 0,0-1 0,0 0-1,0 0 1,0 1 0,0-1 0,0 0 0,0 0 0,0 1-1,0-1 1,0 0 0,0 0 0,0 1 0,0-1 0,-1 0-1,1 0 1,0 1 0,0-1 0,0 0 0,0 0-1,0 0 1,-1 1 0,1-1 0,0 0 0,0 0 0,0 0-1,-1 0 1,1 1 0,0-1 0,-1 0 0,-22 32-4382,-16 14-5530</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7452.04">3565 2190 9332,'0'0'10768,"-2"-11"-9821,2 11-940,-1-3 27,0 1 0,0-1 1,1 0-1,-1 1 0,1-1 1,0 0-1,0 1 1,0-1-1,0 0 0,0 0 1,0 1-1,1-1 1,-1 0-1,1 0 0,0 1 1,0-1-1,0 1 0,0-1 1,0 1-1,1-1 1,-1 1-1,1 0 0,0 0 1,-1-1-1,1 1 1,0 0-1,0 1 0,0-1 1,1 0-1,3-2 0,48-27 65,1 1 0,1 4 0,1 1-1,2 4 1,0 1 0,1 4-1,87-13 1,-123 28-1667,-45 4-14090</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7705.93">3840 1813 1297,'0'0'14414,"17"1"-13915,-3 1-418,1 0 0,-1 0 0,0 1 0,0 1 0,0 0 0,0 1 0,-1 1-1,20 10 1,-13-3 60,1 1 0,-2 1 0,0 1 0,-1 0 0,21 24 0,-32-32-70,0 1-1,-1 0 1,0 0-1,-1 1 0,0 0 1,0 0-1,-1 0 1,0 0-1,-1 0 0,0 1 1,-1 0-1,0-1 1,-1 1-1,1 13 1,-2-18 18,0 1 1,-1-1 0,1 0-1,-1 1 1,-1-1 0,1 0 0,-1 0-1,0 1 1,0-1 0,-1-1-1,0 1 1,0 0 0,0-1 0,-1 1-1,0-1 1,0 0 0,0 0-1,0-1 1,-1 1 0,0-1-1,0 0 1,0 0 0,-10 5 0,0 2-102,6-4-337,0 0 1,-1-1-1,-16 8 1,23-12-3027</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="7705.92">3840 1813 1297,'0'0'14414,"17"1"-13915,-3 1-418,1 0 0,-1 0 0,0 1 0,0 1 0,0 0 0,0 1 0,-1 1-1,20 10 1,-13-3 60,1 1 0,-2 1 0,0 1 0,-1 0 0,21 24 0,-32-32-70,0 1-1,-1 0 1,0 0-1,-1 1 0,0 0 1,0 0-1,-1 0 1,0 0-1,-1 0 0,0 1 1,-1 0-1,0-1 1,-1 1-1,1 13 1,-2-18 18,0 1 1,-1-1 0,1 0-1,-1 1 1,-1-1 0,1 0 0,-1 0-1,0 1 1,0-1 0,-1-1-1,0 1 1,0 0 0,0-1 0,-1 1-1,0-1 1,0 0 0,0 0-1,0-1 1,-1 1 0,0-1-1,0 0 1,0 0 0,-10 5 0,0 2-102,6-4-337,0 0 1,-1-1-1,-16 8 1,23-12-3027</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8071.38">4500 1933 14295,'0'0'7688,"17"16"-7002,-15-14-664,20 19 142,0 1 0,-1 1 1,-1 1-1,30 48 0,-44-62-29,-2 0 0,1 1 0,-1 0 0,-1 0 0,0 0 0,-1 0 0,0 1 0,-1-1 0,0 22 0,-1-32 137,2-7-88,31-67-149,4 1-1,2 2 0,3 2 0,3 2 1,3 1-1,67-68 0,-31 50-481,167-124 0,-144 122-2306,-104 83 1862,3-3-108</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="8873.99">6239 1333 13446,'0'0'9655,"-2"-4"-9233,2 4-416,0 0 0,0-1 0,-1 1 1,1-1-1,0 1 0,0-1 0,0 1 0,0-1 1,0 1-1,0-1 0,0 1 0,0 0 0,0-1 1,0 1-1,0-1 0,0 1 0,1-1 0,-1 1 0,0-1 1,0 1-1,0 0 0,1-1 0,-1 1 0,0-1 1,0 1-1,1 0 0,-1-1 0,0 1 0,1 0 1,-1-1-1,1 1 0,-1 0 0,0 0 0,1-1 1,-1 1-1,1 0 0,-1 0 0,0 0 0,1 0 1,-1-1-1,1 1 0,36-9 242,57 1 81,-74 7-305,154-19 169,-92 9-1623,84 0 0,-162 11 474,9 0-583</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9134.85">6582 1216 8340,'0'0'8924,"0"-1"-8914,0 1-1,0-1 1,0 1 0,0 0-1,0-1 1,0 1 0,0 0 0,0-1-1,0 1 1,0-1 0,0 1-1,0 0 1,1-1 0,-1 1-1,0 0 1,0-1 0,0 1 0,1 0-1,-1-1 1,0 1 0,0 0-1,1-1 1,-1 1 0,0 0-1,1 0 1,-1 0 0,0-1 0,1 1-1,-1 0 1,0 0 0,1 0-1,-1 0 1,0-1 0,1 1-1,-1 0 1,0 0 0,1 0 0,-1 0-1,1 0 1,-1 0 0,0 0-1,1 0 1,0 0 0,4 0 45,1 0 1,-1 0-1,0 1 1,1 0-1,-1 0 0,0 0 1,1 0-1,-1 1 1,0 0-1,5 2 1,53 29 249,-46-24-254,-10-6-7,11 7-5,0 0-1,0 1 1,26 22-1,-39-29 19,-1 0 1,0 0-1,0 1 1,-1-1-1,1 1 1,-1 0-1,0 0 1,-1 0-1,1 0 1,-1 0-1,0 1 0,0-1 1,0 1-1,-1 0 1,0-1-1,0 1 1,0 10-1,-2-11 37,0-1-1,-1 0 1,1 1-1,-1-1 1,0 0 0,0 0-1,0 0 1,-1 0-1,1 0 1,-1 0-1,0-1 1,0 1 0,0-1-1,0 0 1,-1 0-1,0 0 1,1 0 0,-1-1-1,0 0 1,-6 3-1,-13 8 67,0-2-1,-29 10 1,34-15-611,0-1 0,-34 6 0,48-11-1574</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="9134.84">6582 1216 8340,'0'0'8924,"0"-1"-8914,0 1-1,0-1 1,0 1 0,0 0-1,0-1 1,0 1 0,0 0 0,0-1-1,0 1 1,0-1 0,0 1-1,0 0 1,1-1 0,-1 1-1,0 0 1,0-1 0,0 1 0,1 0-1,-1-1 1,0 1 0,0 0-1,1-1 1,-1 1 0,0 0-1,1 0 1,-1 0 0,0-1 0,1 1-1,-1 0 1,0 0 0,1 0-1,-1 0 1,0-1 0,1 1-1,-1 0 1,0 0 0,1 0 0,-1 0-1,1 0 1,-1 0 0,0 0-1,1 0 1,0 0 0,4 0 45,1 0 1,-1 0-1,0 1 1,1 0-1,-1 0 0,0 0 1,1 0-1,-1 1 1,0 0-1,5 2 1,53 29 249,-46-24-254,-10-6-7,11 7-5,0 0-1,0 1 1,26 22-1,-39-29 19,-1 0 1,0 0-1,0 1 1,-1-1-1,1 1 1,-1 0-1,0 0 1,-1 0-1,1 0 1,-1 0-1,0 1 0,0-1 1,0 1-1,-1 0 1,0-1-1,0 1 1,0 10-1,-2-11 37,0-1-1,-1 0 1,1 1-1,-1-1 1,0 0 0,0 0-1,0 0 1,-1 0-1,1 0 1,-1 0-1,0-1 1,0 1 0,0-1-1,0 0 1,-1 0-1,0 0 1,1 0 0,-1-1-1,0 0 1,-6 3-1,-13 8 67,0-2-1,-29 10 1,34-15-611,0-1 0,-34 6 0,48-11-1574</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="10124.22">7332 1154 6787,'0'0'11886,"-8"-4"-7939,8 4-3863,0 0-1,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 1,0 0-1,148 175 346,-41-41 2095,-108-137-2521,1 0-1,0 0 1,0 1 0,0-1-1,0 0 1,0 0 0,1 0-1,-1 0 1,1 1 0,0-1-1,0 0 1,0 1 0,1-4-1,0 3-2,15-33-12,1 1-1,2 1 1,1 1-1,2 1 1,32-34-1,-24 27-13,192-216-290,-172 204 245,2 3 1,103-71-1,-42 45 103,-95 68-44,-10 5-2583</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="12636.96">5598 706 2305,'0'0'3402,"-2"-1"-716,-12 2 13015,12 2-15525,4 13-132,0 0 0,2-1 0,0 1 0,0 0 0,1-1 1,1 0-1,1 0 0,0-1 0,1 0 0,0 0 0,1 0 0,20 22 0,-17-21-84,-12-14 70,0 0 1,0-1 0,1 1-1,-1 0 1,1-1-1,-1 1 1,0-1-1,1 1 1,-1 0 0,1-1-1,0 1 1,-1-1-1,1 1 1,-1-1-1,1 0 1,0 1 0,-1-1-1,1 0 1,0 1-1,-1-1 1,2 0-1,19-19 387,444-511 138,-462 526-624,1 1 1,-1-1 0,1 1-1,0 0 1,0 0-1,8-5 1,-12 8-36,1 0 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 0 0,-1 1 0,1-1 0,0 0 0,0 1 0,0-1 0,-1 1 0,1-1 0,0 1-1,-1 0 1,1-1 0,0 1 0,-1 0 0,1-1 0,-1 1 0,1 0 0,-1-1 0,1 1 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0-1 0,1 1 0,-1 0 0,0 0 0,0 0 0,0 1 0,5 19-4207,-4 2-2116</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="13835.34">6024 1685 4994,'0'0'14143,"-3"-2"-12716,3 2-1392,-1-1 0,1 1 0,-1 0 0,1-1 0,-1 1 0,1 0 0,-1 0 0,0 0 0,1-1 0,-1 1 0,1 0 0,-1 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,0 1 0,-17 20 419,-11 41-148,23-49-134,-17 39 222,-61 152 496,66-158-958,12-32-228,0 1-1,0 0 0,1 0 0,1 1 0,1-1 0,-3 30 1,18-47-6382,0-13 891</inkml:trace>
@@ -20683,7 +20773,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="218.38">150 103 5651,'0'0'9996,"-12"-11"-9409,16 11-573,-1 0-1,0 0 1,0 0-1,1 1 1,-1-1-1,0 1 1,0 0-1,0-1 1,1 2 0,-1-1-1,0 0 1,3 3-1,-2-3 30,-1 2-1,1-1 0,-1 0 0,0 1 1,0-1-1,0 1 0,0 0 1,0 0-1,-1 0 0,1 0 1,-1 0-1,0 1 0,0-1 1,0 1-1,-1-1 0,1 1 1,1 5-1,-3-6 55,1 0-1,-1 1 1,0-1-1,0 0 1,-1 0-1,1 0 1,0 0-1,-1 0 1,0 0 0,0 0-1,0 0 1,0 0-1,0 0 1,0-1-1,-1 1 1,0 0 0,1-1-1,-1 1 1,0-1-1,0 0 1,0 1-1,-5 3 1,0 0-241,-6 8 256,6-9-5704</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="540.09">455 85 12534,'0'0'4906,"-12"0"-3932,-39 3-443,50-3-520,0 0 0,0 0 0,0 0 1,0 0-1,-1 1 0,1-1 1,0 0-1,0 1 0,0-1 0,0 1 1,0-1-1,0 1 0,0-1 0,0 1 1,0 0-1,0 0 0,0-1 1,0 1-1,0 0 0,0 0 0,1 0 1,-1 0-1,0 0 0,1 0 0,-1 0 1,1 0-1,-1 0 0,1 0 0,-1 1 1,1-1-1,0 0 0,0 0 1,-1 0-1,1 1 0,0-1 0,0 0 1,0 0-1,0 0 0,1 1 0,-1-1 1,1 2-1,-1 0-14,1 0 0,0 0-1,0 1 1,0-1 0,1 0 0,-1 0 0,1 0-1,0 0 1,0-1 0,0 1 0,2 2 0,41 23-130,-37-24 125,0 0-1,-1 1 0,0-1 1,0 2-1,13 11 0,-20-17 12,1 0-1,-1 1 0,0-1 0,1 0 0,-1 1 0,0-1 0,0 1 0,1-1 0,-1 0 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0 0,0 1 1,0-1-1,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,0 0 0,-1 1 0,1-1 0,0 1 0,0-1 0,-1 0 0,1 1 1,0-1-1,0 0 0,-1 1 0,1-1 0,0 0 0,-1 1 0,1-1 0,-1 0 0,1 0 0,0 1 0,-1-1 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 1 0,0-1 1,-1 0-1,1 0 0,-2 0 0,-6-3-2413,7-4-1359</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="834.41">580 153 5394,'0'0'6593,"11"-2"-5345,36-9-156,-46 11-983,1-1 1,-1 1 0,1 0 0,-1-1 0,1 1 0,-1-1 0,1 0 0,-1 1 0,0-1 0,1 0 0,-1 0 0,0 0 0,0 0 0,2-2 0,-3 2-71,1 1 0,-1 0 0,0-1 0,0 1 0,0-1 0,0 1 0,0 0 0,0-1 1,0 1-1,0 0 0,0-1 0,0 1 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 1,0 0-1,0-1 0,0 1 0,-1 0 0,1-1 0,0 1 0,0 0 0,0-1 0,-1 1 1,1 0-1,0-1 0,0 1 0,-1 0 0,1 0 0,0-1 0,-1 1 0,1 0 0,-1-1-7,-1 1-1,1-1 0,0 1 0,0-1 1,0 1-1,-1-1 0,1 1 0,0 0 0,0 0 1,-1 0-1,1 0 0,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 0,-1 0 0,1 1 1,0-1-1,0 1 0,-1-1 0,1 1 1,0-1-1,0 1 0,0 0 0,0-1 0,0 1 1,0 0-1,0 0 0,-1 1 0,-2 3 23,1 0-1,0 0 1,0 0 0,1 1-1,-1-1 1,1 1-1,0 0 1,1-1-1,-1 1 1,1 0-1,0 0 1,1 0-1,0 0 1,0 8-1,0-13-134,0 0 0,1 0-1,-1 0 1,1 0 0,-1 0 0,0 0-1,1 0 1,0-1 0,-1 1-1,1 0 1,0 0 0,-1 0-1,1-1 1,0 1 0,0 0-1,-1-1 1,1 1 0,0 0 0,0-1-1,0 1 1,0-1 0,0 0-1,0 1 1,0-1 0,0 0-1,0 1 1,0-1 0,0 0-1,0 0 1,0 0 0,0 0-1,2 0 1,40-1-5092,-40 1 4457,18-3-3840</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1034.87">757 139 6115,'0'0'11701,"-12"6"-11317,6 6 65,6 2-1,0-1-272,0 1-112,0-3 64,0-1-128,15-3 0,-1-3-1089,7-4-1040,3 0-1312,2-7-3666</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1034.85">757 139 6115,'0'0'11701,"-12"6"-11317,6 6 65,6 2-1,0-1-272,0 1-112,0-3 64,0-1-128,15-3 0,-1-3-1089,7-4-1040,3 0-1312,2-7-3666</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1882.54">924 142 11109,'0'0'8524,"-8"7"-8046,-28 21-190,35-28-285,0 1 0,1-1 0,-1 1 0,0 0 1,0-1-1,0 1 0,1 0 0,-1 0 0,0 0 0,1 0 1,-1 0-1,1-1 0,-1 1 0,1 0 0,-1 0 0,1 0 1,0 0-1,-1 1 0,1-1 0,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 1,0 0-1,1 0 0,-1 0 0,0 0 0,1 0 1,-1 0-1,1 0 0,-1 0 0,1 0 0,0 0 0,-1 0 1,1 0-1,0-1 0,-1 1 0,1 0 0,0 0 0,0-1 1,0 1-1,0-1 0,0 1 0,0-1 0,0 1 0,0-1 1,0 1-1,0-1 0,0 0 0,1 1 0,0 0-65,0-1 0,0 1-1,1 0 1,-1-1 0,0 1-1,1-1 1,-1 0 0,0 1-1,1-1 1,-1 0 0,0 0 0,0-1-1,1 1 1,-1-1 0,0 1-1,1-1 1,-1 1 0,0-1-1,0 0 1,0 0 0,0 0-1,0-1 1,3-1 0,-2-2 67,-1 0 0,0 0 1,0-1-1,-1 1 0,1-1 1,-1 1-1,0-1 0,0 0 1,-1 1-1,0-1 0,0-7 1,0 12-8,0 1 1,1-1-1,-1 1 1,1-1-1,-1 1 1,0-1-1,1 1 1,-1 0-1,1-1 1,-1 1-1,1 0 1,0 0-1,-1-1 1,1 1-1,-1 0 1,1 0-1,-1 0 1,1-1-1,0 1 1,-1 0-1,1 0 1,-1 0-1,1 0 1,0 0-1,-1 0 1,1 0-1,-1 1 0,1-1 1,0 0-1,-1 0 1,1 0-1,-1 1 1,1-1-1,-1 0 1,1 0-1,0 1 1,22 9 748,-20-8-681,-1 0 0,0 0 0,1 0 0,0 0 1,-1-1-1,1 1 0,0-1 0,0 0 0,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0-1 0,0 0 0,5 1 0,19 2-387,-6 5-197,-18-6 432,-1-1 0,1 0 0,0 0 0,0 0 0,0 0 1,-1 0-1,1 0 0,0-1 0,5 1 0,37-5-1586,-43 4 1620,0 0-1,0-1 1,0 1 0,0-1 0,0 0 0,-1 1 0,1-1 0,0 0-1,0 0 1,-1 0 0,1 0 0,0 0 0,-1 0 0,1-1-1,-1 1 1,0-1 0,1 1 0,-1-1 0,0 1 0,0-1-1,1-1 1,-2 2 121,0 1 1,-1-1-1,1 1 0,0-1 0,-1 1 1,1-1-1,0 1 0,-1-1 0,1 1 1,-1-1-1,1 1 0,-1 0 0,1-1 0,-1 1 1,1 0-1,-1 0 0,1-1 0,-1 1 1,1 0-1,-1 0 0,1 0 0,-1 0 1,1-1-1,-1 1 0,0 0 0,1 0 1,-1 0-1,1 0 0,-1 0 0,0 1 0,1-1 1,-1 0-1,1 0 0,-1 0 0,1 0 1,-1 1-1,1-1 0,-1 0 0,0 1 1,-1-1-46,0 0 1,0 1-1,0-1 1,0 1-1,0-1 1,0 1 0,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,-1 2 0,-3 11-225,13-13-742,14-18 341,-14 6 631,-1 0 0,-1-1-1,0 0 1,-1 0-1,0-1 1,-1 1-1,0-1 1,-1 1 0,0-1-1,-1 0 1,-1-18-1,0 30 625,0 10-379,-1 41-173,2 62 312,0-101-453,1 1 0,-1 0 1,2-1-1,0 0 0,0 1 0,1-1 0,6 12 0,1-8-2415,-2-7-2100</inkml:trace>
 </inkml:ink>
 </file>
@@ -20713,7 +20803,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">54 198 8900,'0'0'7105,"1"-14"-3005,36 14-4294,-5-1-266,50 6-1,-74 0-2385,-10 2-3774,-4-4 858</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="312.79">1 310 9316,'0'0'4995,"24"3"-2912,55-6-67,0-1-3354,-73 0-3182</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="312.77">1 310 9316,'0'0'4995,"24"3"-2912,55-6-67,0-1-3354,-73 0-3182</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="883.68">123 33 9524,'0'0'8602,"-9"-7"-7351,-26-18-355,147 103 309,72 53-4240,-182-129 3032,-1 0-1,1 0 1,0 0 0,-1 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,0 1 0,0-1-1,-1 0 1,1 1-1,0-1 1,-1 1 0,1-1-1,-1 1 1,0-1 0,0 0-1,0 1 1,0-1 0,-1 1-1,1-1 1,-1 1 0,1-1-1,-1 1 1,0-1 0,0 0-1,-1 4 1,-4 7 32,0-1 0,-1 1 1,-13 17-1,16-25-36,-68 92 56,40-58-101,2 3 0,-26 49 1,52-86-418,-1 1-1170</inkml:trace>
 </inkml:ink>
 </file>
@@ -20838,7 +20928,7 @@
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">80 0 80,'0'0'20129,"0"18"-19347,1-15-763,-1-1-1,1 1 1,0 0 0,-1-1-1,1 0 1,0 1 0,0-1-1,0 1 1,1-1 0,-1 0-1,1 0 1,-1 0 0,1 0-1,0 0 1,-1 0 0,1 0-1,0-1 1,0 1 0,1 0-1,-1-1 1,0 0 0,0 0-1,1 1 1,-1-1 0,1 0-1,-1-1 1,4 2 0,-5-3-7,1 0-1,-1-1 1,0 1 0,0 0 0,1-1-1,-1 1 1,0 0 0,-1-1 0,1 1 0,0-1-1,0 0 1,-1 1 0,1-1 0,0 0-1,-1 1 1,0-1 0,1 0 0,-1 1-1,0-1 1,0 0 0,0 0 0,0-2-1,6-20 151,-4 64-85,-6 43 539,1-42-1293,1-1-3456,2-29-1835</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="358.24">102 283 12198,'0'0'8110,"-9"5"-7737,-29 16-140,37-20-218,0 0 0,0 1 0,0-1 0,0 0 1,0 1-1,0-1 0,0 1 0,0-1 1,1 1-1,-1-1 0,0 1 0,1-1 1,0 1-1,-1 0 0,1-1 0,0 1 0,0 0 1,0 0-1,0-1 0,0 1 0,0 0 1,0-1-1,1 1 0,0 1 0,12 33 93,17-8-53,-27-26-53,0 0 1,0 0-1,0 0 0,0 1 1,-1-1-1,1 1 1,-1-1-1,1 1 1,-1 0-1,0 0 0,0 0 1,-1 0-1,1 0 1,0 0-1,-1 1 1,0-1-1,1 4 1,-9-13-7732,5 3 6024,-6-10-4471</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="496.92">81 330 4706,'0'0'11141,"74"-45"-10965,-65 43-176,-1 2-528,-5 0-1201,-3 10-1504,0 7-5939</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="496.91">81 330 4706,'0'0'11141,"74"-45"-10965,-65 43-176,-1 2-528,-5 0-1201,-3 10-1504,0 7-5939</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="903.53">105 577 13942,'0'0'5504,"-2"4"-5109,-12 49 945,13-51-1319,1-1 1,-1 1 0,1-1-1,0 1 1,-1-1 0,1 0-1,0 1 1,0-1-1,0 1 1,0-1 0,1 1-1,-1-1 1,0 1-1,0-1 1,1 1 0,-1-1-1,1 0 1,0 1 0,-1-1-1,1 0 1,0 0-1,0 1 1,-1-1 0,1 0-1,0 0 1,0 0 0,1 0-1,-1 0 1,0 0-1,0 0 1,0 0 0,1-1-1,-1 1 1,0 0 0,1-1-1,1 1 1,2 0-43,0-1 1,1 0 0,-1-1-1,1 1 1,-1-1-1,0 0 1,1-1 0,-1 1-1,8-4 1,-11 4 13,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0-1 1,0 1-1,0-1 0,0 1 0,-1-1 0,1 1 0,-1-1 0,1 0 0,-1 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,1-1 0,0-3 1,-6 5 100,1 1 1,0-1 0,-1 1 0,1 0 0,0 0 0,-9 1 0,6 1-81,0 0 0,0 1 1,0 0-1,0 0 0,0 0 0,1 1 1,-1 0-1,1 0 0,0 0 0,1 1 1,-1 0-1,-7 9 0,10-11-487,1 0 0,0 0-1,-1 1 1,1-1 0,0 1 0,1 0-1,-1 0 1,-1 7 0,0 2-4628</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1305.55">0 871 12902,'0'0'7310,"11"-5"-6851,-1 1-305,1-1 1,0 1-1,0 1 0,0 0 1,1 1-1,-1 0 1,14 0-1,-24 2-131,0 1 1,-1-1-1,1 1 0,-1-1 1,1 1-1,-1-1 0,1 1 1,-1-1-1,1 1 0,-1 0 1,1-1-1,-1 1 0,0 0 1,0-1-1,1 1 0,-1 0 1,0 0-1,0-1 0,0 1 0,1 0 1,-1 0-1,0-1 0,0 1 1,0 0-1,0 0 0,-1 1 1,0 26 332,1-26-315,-2 14 89,-1-1 1,0 1-1,-1-1 0,-12 27 1,0 2-2070,5 0-4735,8-28-2407</inkml:trace>
 </inkml:ink>
@@ -20992,7 +21082,7 @@
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">136 36 10453,'0'0'7403,"-5"-2"-6792,3 1-506,-1 0 0,1-1-1,-1 1 1,0 1 0,1-1-1,-1 0 1,0 0 0,0 1-1,0 0 1,0 0 0,1 0 0,-1 0-1,0 0 1,-4 1 0,6-1-74,-1 1 1,0 0-1,1 0 0,0 0 1,-1 0-1,1 0 1,0 0-1,-1 0 1,1 0-1,0 0 0,0 1 1,0-1-1,0 1 1,0-1-1,0 0 0,0 1 1,1 0-1,-1-1 1,0 1-1,1-1 1,-1 1-1,1 0 0,0-1 1,0 1-1,-1 0 1,1-1-1,0 1 0,0 0 1,1 2-1,-1-3-34,0 0 0,0 0 0,0 0 0,0-1 0,1 1 0,-1 0 0,0 0 0,0-1 0,0 1 0,1 0-1,-1-1 1,0 1 0,1 0 0,-1 0 0,1-1 0,-1 1 0,1-1 0,-1 1 0,1-1 0,0 1 0,-1-1 0,1 1 0,-1-1-1,1 1 1,0-1 0,1 1 0,24 5-274,-24-6 259,1 0 0,0 1 0,0-1 0,-1 1 0,1-1 0,0 1 0,-1 0-1,1 0 1,-1 0 0,1 0 0,-1 1 0,0-1 0,3 3 0,-46 10 247,7-6-103,-28 3-2976</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="492.39">212 52 6131,'0'0'10984,"-3"9"-8388,-11 30-2018,9-17-385,5-22-194,1 0-1,-1 1 0,0-1 1,0 0-1,0 0 0,0 1 1,0-1-1,0 0 1,0 0-1,0 1 0,1-1 1,-1 0-1,0 0 0,0 1 1,0-1-1,0 0 1,1 0-1,-1 0 0,0 0 1,0 1-1,1-1 0,-1 0 1,0 0-1,0 0 1,1 0-1,-1 0 0,0 0 1,0 0-1,1 1 0,-1-1 1,0 0-1,1 0 0,-1 0 1,0 0-1,1 0 1,1-1-45,0 0 0,0 0 0,0 1 1,0-1-1,0-1 0,0 1 0,0 0 0,-1 0 1,1-1-1,0 1 0,-1-1 0,1 1 1,-1-1-1,2-2 0,1-1-137,0 0-1,-1 0 1,0 0 0,0-1 0,0 1-1,0-1 1,-1 0 0,0 0-1,1-7 1,-3 13 151,0 42 777,0-32-256,0 3 9,0-1-7067</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1108.38">219 13 4370,'0'0'12331,"-1"9"-11451,0-2-779,0-1 92,0 1 1,1-1-1,0 1 0,0-1 1,0 1-1,2 7 1,-2-12-161,1 0 1,-1-1-1,1 1 1,0-1-1,-1 1 0,1 0 1,0-1-1,0 1 1,0-1-1,0 0 1,0 1-1,0-1 1,0 0-1,1 0 1,-1 0-1,0 0 1,1 0-1,-1 0 0,1 0 1,-1 0-1,1 0 1,0-1-1,-1 1 1,1 0-1,0-1 1,-1 0-1,1 1 1,0-1-1,-1 0 1,1 0-1,0 0 0,1 0 1,-1 0-48,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,-1 0 0,1-1 0,0 1-1,0-1 1,0 1 0,-1-1-1,1 1 1,0-1 0,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 0-1,1-1 1,-1 1 0,1 0 0,-1 0-1,0-1 1,0 1 0,0-1-1,0 1 1,0-1 0,0 0 0,0 1-1,-1-1 1,2-2 0,6-12-2386,-8 15 1947,1 1 0,-1-1 0,1 0 1,-1 1-1,1-1 0,-1 1 1,1-1-1,-1 1 0,1-1 1,0 1-1,-1-1 0,1 1 1,0 0-1,0-1 0,-1 1 0,1 0 1,0-1-1,-1 1 0,1 0 1,1 0-1,17 3-72,19 16 9630,-32-15-7741,-5-4-1266,0 1 0,0-1-1,0 1 1,0-1 0,1 0 0,-1 0-1,0 1 1,0-1 0,0 0 0,0 0 0,1 0-1,-1 0 1,0 0 0,0 0 0,0 0-1,1-1 1,-1 1 0,0 0 0,0-1-1,0 1 1,0-1 0,0 1 0,0-1-1,0 1 1,0-1 0,0 0 0,0 0-1,0 1 1,0-1 0,0 0 0,0-1 0,27-39-70,-6 9 137,-21 32-124,1-1 1,-1 1-1,1-1 1,-1 1-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,0 1 0,-1-1-1,1 0 1,-1 1-1,0 0 1,1-1-1,-1 1 1,1 0-1,-1 0 1,0 0-1,2 1 1,20 8-1657</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1108.36">219 13 4370,'0'0'12331,"-1"9"-11451,0-2-779,0-1 92,0 1 1,1-1-1,0 1 0,0-1 1,0 1-1,2 7 1,-2-12-161,1 0 1,-1-1-1,1 1 1,0-1-1,-1 1 0,1 0 1,0-1-1,0 1 1,0-1-1,0 0 1,0 1-1,0-1 1,0 0-1,1 0 1,-1 0-1,0 0 1,1 0-1,-1 0 0,1 0 1,-1 0-1,1 0 1,0-1-1,-1 1 1,1 0-1,0-1 1,-1 0-1,1 1 1,0-1-1,-1 0 1,1 0-1,0 0 0,1 0 1,-1 0-48,0 0-1,0 0 1,0 0 0,0 0-1,0 0 1,-1 0 0,1-1 0,0 1-1,0-1 1,0 1 0,-1-1-1,1 1 1,0-1 0,-1 0 0,1 0-1,-1 0 1,1 0 0,-1 0-1,1-1 1,-1 1 0,1 0 0,-1 0-1,0-1 1,0 1 0,0-1-1,0 1 1,0-1 0,0 0 0,0 1-1,-1-1 1,2-2 0,6-12-2386,-8 15 1947,1 1 0,-1-1 0,1 0 1,-1 1-1,1-1 0,-1 1 1,1-1-1,-1 1 0,1-1 1,0 1-1,-1-1 0,1 1 1,0 0-1,0-1 0,-1 1 0,1 0 1,0-1-1,-1 1 0,1 0 1,1 0-1,17 3-72,19 16 9630,-32-15-7741,-5-4-1266,0 1 0,0-1-1,0 1 1,0-1 0,1 0 0,-1 0-1,0 1 1,0-1 0,0 0 0,0 0 0,1 0-1,-1 0 1,0 0 0,0 0 0,0 0-1,1-1 1,-1 1 0,0 0 0,0-1-1,0 1 1,0-1 0,0 1 0,0-1-1,0 1 1,0-1 0,0 0 0,0 0-1,0 1 1,0-1 0,0 0 0,0-1 0,27-39-70,-6 9 137,-21 32-124,1-1 1,-1 1-1,1-1 1,-1 1-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 0 1,0 1 0,-1-1-1,1 0 1,-1 1-1,0 0 1,1-1-1,-1 1 1,1 0-1,-1 0 1,0 0-1,2 1 1,20 8-1657</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -21023,7 +21113,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0">76 72 3153,'0'0'5771,"0"-2"-5920,-5-13 10468,2 12-9671,2 2-621,-1 1-1,1-1 0,-1 1 0,1 0 1,-1 0-1,1 0 0,-1 0 0,1 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,-1 1 0,1-1 0,-1 1 1,1-1-1,0 1 0,-1 0 0,1-1 1,0 1-1,-1 0 0,1 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 1 0,0-1 1,1 0-1,-1 1 0,0-1 1,1 1-1,-1-1 0,1 0 0,0 1 1,-1-1-1,1 1 0,0-1 0,0 1 1,0-1-1,0 1 0,0-1 0,0 1 1,0-1-1,1 1 0,-1-1 0,1 2 1,1 0-43,0 0 1,0-1 0,0 1 0,0-1 0,1 0 0,-1 0 0,1 1-1,-1-2 1,1 1 0,0 0 0,0-1 0,-1 1 0,1-1-1,0 0 1,1 0 0,-1 0 0,4 1 0,15 7-273,-22-9 289,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,1 1 0,-1-1 0,0 0-1,0 0 1,0 1 0,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1-1,0 0 1,-1 0 0,1 1 0,0-1 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,-1 0-1,1 1 1,0-1 0,0 0 0,0 0 0,-1 0 0,1 0 0,0 1 0,0-1 0,-1 0 0,1 0-1,0 0 1,0 0 0,-1 0 0,1 0 0,0 1 0,0-1 0,-1 0 0,0 0 0,-11 6 115,5-3-152,-2 1-72,0-1-1,-1 0 0,1-1 0,-1 0 1,-15 2-1,33-13-8484,15-5 5609,-16 10 1088,11-8-1967</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="123.34">76 72 2625</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="490.19">76 72 2625,'51'4'3196,"-38"-8"7534,-19 4-6800,-1 8-5237,6-7 1308,0 0 1,1 0-1,-1-1 0,1 1 1,0 0-1,-1 0 0,1 0 1,0 0-1,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,0 0 1,1 2-1,11-5-972,-8 0 816,-1 0 0,0 0 0,0 0 0,-1-1 1,1 0-1,0 1 0,-1-1 0,0 0 0,3-4 1,-5 8 167,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 0 0,1 0 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 0,-1 0 0,1-1 1,0 1-1,0 0 0,0 0 0,0-1 0,0 1 0,-1-1 0,1 1 0,0-1 0,0 1 0,0-1 0,0 1 0,1-1 0,-1 0 0,0 1 0,0-1 0,0 0 0,2 0 0,0 1-73,-1-1-1,1 1 1,0-1-1,-1 0 1,1 0 0,0 0-1,-1 0 1,1 0-1,0 0 1,0-1 0,-1 1-1,1-1 1,-1 0-1,1 0 1,-1 0 0,1 0-1,-1 0 1,5-3-1,-4 0-145,0 1 0,1-1 0,-1 0 0,-1 0-1,1 0 1,-1 0 0,1 0 0,-1-1 0,0 1 0,1-8-1,3-28 2993,-6 58-2092,-1-2-907,5 43 443,-4-56-645,1-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0-1 0,1 0 0,-1 1 0,1-1 0,-1 0 0,4 3 0,-2-3-3741</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="667.84">288 53 8468,'0'0'8564,"15"-49"-8596,0 47-64,2 2-320,-2 0-97,-6 10-799,0 5-1634,-9 6-2576</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="667.83">288 53 8468,'0'0'8564,"15"-49"-8596,0 47-64,2 2-320,-2 0-97,-6 10-799,0 5-1634,-9 6-2576</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -21081,7 +21171,7 @@
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">14 5 9556,'0'0'10274,"-2"-3"-9412,2 3-849,0 0 0,0 1 1,0-1-1,0 0 0,0 0 0,0 1 0,-1-1 0,1 0 1,0 0-1,0 1 0,0-1 0,0 0 0,0 0 0,-1 0 1,1 0-1,0 1 0,0-1 0,0 0 0,-1 0 0,1 0 1,0 0-1,0 0 0,0 1 0,-1-1 0,1 0 0,0 0 1,0 0-1,-1 0 0,1 0 0,0 0 0,0 0 0,-1 0 1,1 0-1,0 0 0,0 0 0,-1 0 0,1 0 0,0 0 1,0 0-1,0 0 0,-1 0 0,1-1 0,0 1 0,0 0 1,-1 0-1,1 0 0,0 0 0,0 0 0,0-1 0,-1 1 0,1 0 1,0 0-1,0 0 0,0 0 0,0-1 0,0 1 0,-1 0 1,1 0-1,0-1 0,0 1 0,0 0 0,0 0 0,0 0 1,0-1-1,0 1 0,0 0 0,0 0 0,0-1 0,0 1 1,0 32 915,1-21-732,1 0-1,0 0 1,1 0 0,0-1-1,6 13 1,-8-20-191,0-1-1,1 1 1,-1-1 0,1 0-1,-1 1 1,1-1 0,0 0 0,0 0-1,0-1 1,0 1 0,0 0-1,0 0 1,1-1 0,-1 0-1,0 1 1,1-1 0,-1 0 0,1 0-1,0 0 1,-1-1 0,1 1-1,0 0 1,-1-1 0,1 0-1,0 0 1,0 0 0,-1 0 0,1 0-1,0 0 1,-1-1 0,1 1-1,0-1 1,-1 0 0,1 0 0,0 0-1,-1 0 1,3-2 0,-1 1-15,0 0 1,-1-1-1,1 0 1,0 0-1,-1 0 1,0 0-1,0-1 1,0 1-1,0-1 0,-1 0 1,1 0-1,-1 0 1,0 0-1,0 0 1,0 0-1,-1 0 1,1-1-1,-1 1 1,0-1-1,0 1 1,0-7-1,-4 202 1717,2-189-1796,1 0 1,0-1 0,0 1 0,1-1 0,-1 1 0,0 0-1,0-1 1,1 1 0,-1-1 0,1 1 0,-1-1 0,1 1-1,0-1 1,0 1 0,0-1 0,-1 1 0,1-1 0,0 0-1,1 0 1,-1 0 0,0 1 0,0-1 0,0 0-1,2 1 1,-1-2-423,0 1-1,0 0 1,-1-1-1,1 0 1,0 1-1,0-1 1,0 0-1,0 0 1,0 0 0,-1 0-1,1 0 1,0 0-1,0-1 1,2 0-1,13-6-8453</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="438.12">284 42 5795,'0'0'16071,"-4"1"-15540,3 0-500,0-1 1,0 0-1,-1 1 0,1-1 1,0 1-1,0-1 0,0 1 0,0 0 1,0-1-1,0 1 0,0 0 1,0 0-1,1 0 0,-1-1 1,0 1-1,0 0 0,1 0 1,-1 0-1,0 0 0,1 1 1,-1-1-1,1 0 0,0 0 0,-1 0 1,1 2-1,-1 0 3,1 0-1,0 0 0,1 0 1,-1-1-1,0 1 1,1 0-1,-1-1 1,1 1-1,0 0 1,0-1-1,2 5 0,-1-3-25,0 0 0,1 0 0,-1-1-1,1 1 1,0 0 0,-1-1 0,2 0 0,-1 0-1,0 0 1,1 0 0,-1 0 0,1-1-1,0 1 1,0-1 0,0 0 0,0 0-1,4 1 1,-6-3-21,1 1 0,-1-1-1,1 1 1,-1-1 0,0 0-1,1 0 1,-1 0 0,1 0 0,-1 0-1,1-1 1,-1 1 0,0-1-1,1 0 1,-1 1 0,0-1 0,0 0-1,1 0 1,-1-1 0,0 1-1,0 0 1,0-1 0,0 1 0,-1-1-1,1 0 1,0 1 0,-1-1-1,3-4 1,-1 1 10,0-1-1,-1 1 1,0-1-1,0 0 1,-1 0-1,0 0 0,0 0 1,0 0-1,0 0 1,-1-9-1,4 71 21,-1-28 19,-2-1 0,-2 54-1,1-75-4,-1-1 0,0 0 0,1 1 0,-2-1 0,1 0 0,-1 0 0,0 0 0,0 0 0,0 0 0,0 0 0,-1 0 0,0-1 0,0 1 0,0-1 0,-1 0 0,0 0 0,1 0 0,-1-1 0,0 1 0,-1-1 0,-4 3 0,8-5-34,0 0-1,0 0 0,0 0 1,0-1-1,0 1 1,-1 0-1,1-1 1,0 1-1,0-1 1,0 0-1,-1 1 0,1-1 1,0 0-1,-1 1 1,1-1-1,0 0 1,-1 0-1,1 0 1,0 0-1,-1-1 0,1 1 1,0 0-1,-1-1 1,1 1-1,0 0 1,0-1-1,-1 1 1,1-1-1,0 0 0,0 1 1,0-1-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 1,0 0-1,0 0 0,1 0 1,-1 0-1,-1-2 1,-4-24-2761,5-3-4410,1 9-3268</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1034.87">593 76 10293,'0'0'10410,"-2"7"-9701,0 0-560,0 1 0,1-1-1,0 1 1,0-1-1,1 1 1,0 0-1,1 7 1,-1-13-134,0 0 1,1 0-1,-1 0 1,1 1-1,-1-1 1,1 0-1,0 0 0,-1 0 1,1 0-1,0 0 1,0-1-1,1 1 1,-1 0-1,0 0 1,1-1-1,-1 1 0,1-1 1,-1 1-1,1-1 1,0 1-1,-1-1 1,1 0-1,0 0 0,0 0 1,0 0-1,0 0 1,0-1-1,0 1 1,0 0-1,0-1 0,1 0 1,-1 1-1,0-1 1,4 0-1,-4 0-23,1-1 1,0 1-1,-1-1 0,1 1 0,-1-1 0,1 0 1,-1 0-1,1 0 0,-1 0 0,1-1 1,-1 1-1,0-1 0,0 1 0,0-1 0,0 0 1,0 0-1,0 0 0,0 0 0,-1 0 0,1 0 1,-1 0-1,1 0 0,-1-1 0,0 1 0,2-6 1,0 0 51,0-1 1,-1 0-1,0 1 1,0-1-1,-1 0 1,1-17 0,-2 25 96,5 40-66,-4-18-18,2 9-10,-4 51-1,1-74 8,-1-1-1,0 1 1,0 0-1,-1 0 0,0-1 1,0 1-1,0-1 1,-1 0-1,0 0 1,0 0-1,-1 0 1,0 0-1,-5 6 1,9-11-65,0-1 0,-1 1 1,1-1-1,0 0 0,0 1 1,0-1-1,-1 0 0,1 0 0,0 1 1,0-1-1,-1 0 0,1 1 1,0-1-1,-1 0 0,1 0 0,0 0 1,-1 1-1,1-1 0,0 0 1,-1 0-1,1 0 0,0 0 0,-1 0 1,1 0-1,0 0 0,-1 1 1,1-1-1,-1 0 0,1 0 0,0 0 1,-1-1-1,1 1 0,0 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,-1-1 0,0-15-1725,9-23-3407,6 6-209</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1034.85">593 76 10293,'0'0'10410,"-2"7"-9701,0 0-560,0 1 0,1-1-1,0 1 1,0-1-1,1 1 1,0 0-1,1 7 1,-1-13-134,0 0 1,1 0-1,-1 0 1,1 1-1,-1-1 1,1 0-1,0 0 0,-1 0 1,1 0-1,0 0 1,0-1-1,1 1 1,-1 0-1,0 0 1,1-1-1,-1 1 0,1-1 1,-1 1-1,1-1 1,0 1-1,-1-1 1,1 0-1,0 0 0,0 0 1,0 0-1,0 0 1,0-1-1,0 1 1,0 0-1,0-1 0,1 0 1,-1 1-1,0-1 1,4 0-1,-4 0-23,1-1 1,0 1-1,-1-1 0,1 1 0,-1-1 0,1 0 1,-1 0-1,1 0 0,-1 0 0,1-1 1,-1 1-1,0-1 0,0 1 0,0-1 0,0 0 1,0 0-1,0 0 0,0 0 0,-1 0 0,1 0 1,-1 0-1,1 0 0,-1-1 0,0 1 0,2-6 1,0 0 51,0-1 1,-1 0-1,0 1 1,0-1-1,-1 0 1,1-17 0,-2 25 96,5 40-66,-4-18-18,2 9-10,-4 51-1,1-74 8,-1-1-1,0 1 1,0 0-1,-1 0 0,0-1 1,0 1-1,0-1 1,-1 0-1,0 0 1,0 0-1,-1 0 1,0 0-1,-5 6 1,9-11-65,0-1 0,-1 1 1,1-1-1,0 0 0,0 1 1,0-1-1,-1 0 0,1 0 0,0 1 1,0-1-1,-1 0 0,1 1 1,0-1-1,-1 0 0,1 0 0,0 0 1,-1 1-1,1-1 0,0 0 1,-1 0-1,1 0 0,0 0 0,-1 0 1,1 0-1,0 0 0,-1 1 1,1-1-1,-1 0 0,1 0 0,0 0 1,-1-1-1,1 1 0,0 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,-1-1 0,0-15-1725,9-23-3407,6 6-209</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1459.42">793 66 5410,'0'0'14540,"2"7"-13536,0 0-835,0-1 1,1 1 0,0-1 0,0 0 0,6 9 0,-8-14-159,-1 0 1,1 0-1,-1 0 1,1 0-1,0 0 0,0 0 1,0 0-1,-1 0 0,1-1 1,0 1-1,0 0 1,0 0-1,0-1 0,0 1 1,0-1-1,1 1 1,-1-1-1,0 1 0,0-1 1,0 0-1,0 1 1,1-1-1,-1 0 0,0 0 1,0 0-1,0 0 0,1 0 1,-1 0-1,0 0 1,0-1-1,0 1 0,1 0 1,-1-1-1,0 1 1,0-1-1,0 1 0,0-1 1,0 1-1,0-1 1,0 0-1,0 0 0,0 1 1,0-1-1,0 0 0,0 0 1,-1 0-1,2-1 1,26-60 540,-27 65-492,1-1 0,-1 0-1,0 1 1,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,-1 0-1,1-1 1,-1 1 0,0 3 0,0-5-19,7 39-3,-2 0 1,-2 1-1,-1-1 1,-6 60-1,-8-56-9,12-43-25,0 0 0,-1 1 1,1-1-1,-1 0 0,1 1 0,-1-1 1,1 0-1,-1 0 0,0 1 1,0-1-1,0 0 0,0 0 1,1 0-1,-1 0 0,0 0 1,-1 0-1,1 0 0,0-1 1,0 1-1,0 0 0,0 0 1,-1-1-1,1 1 0,0-1 1,-1 1-1,1-1 0,-2 0 0,2-4 12,0 0-1,0 0 0,0 0 0,0 0 0,1 0 0,0 0 0,0 0 1,0-1-1,1-4 0,-1 3 15,1-9-18,0 0 0,1 0 0,0 0 0,2 0 0,-1 1-1,2-1 1,7-16 0,7-9-1024,27-42 1,-11 20-3187,-15 23-2165</inkml:trace>
 </inkml:ink>
 </file>
@@ -21111,7 +21201,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">18 46 10165,'0'0'10127,"1"-6"-9516,3-12-295,-2 21 161,-3 36 510,1-11-670,0-11-163,-1 1 0,0 0-1,-1-1 1,-1 1 0,-11 32 0,12-73 412,5-21-561,0 30-16,1 0-1,1 1 1,0-1 0,13-23 0,-17 34 8,1 0 0,0 0 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,1 1 0,0 0 0,-1 0 0,1 0 0,0 0 0,0 0 0,0 1 0,0-1 0,0 1 0,0 0 0,1 0 0,-1 0 0,0 0 1,0 0-1,1 1 0,-1 0 0,1-1 0,-1 1 0,5 1 0,-6 0 1,-1-1 0,1 1 1,0 0-1,-1 0 0,1 0 0,-1 0 1,1 0-1,-1 0 0,0 1 1,0-1-1,1 0 0,-1 1 0,0-1 1,0 0-1,0 1 0,0 0 0,-1-1 1,1 1-1,0-1 0,-1 1 0,1 0 1,-1 0-1,1-1 0,-1 4 1,8 50 53,-8-43-19,3 97 232,-1-125-299,1 0 0,0 0 0,1 0 0,1 0 0,0 1 0,1 0 0,1 0 0,0 0 0,1 1 0,13-18 0,-19 29 28,-1 1 0,1-1 1,0 1-1,0 0 0,0-1 0,0 1 0,0 0 1,1 1-1,-1-1 0,0 0 0,1 1 0,0-1 0,-1 1 1,1 0-1,0 0 0,-1 0 0,1 0 0,4-1 0,-5 3 20,0-1-1,0 1 0,-1 0 0,1-1 0,0 1 1,0 0-1,-1 0 0,1 0 0,-1 0 0,1 0 1,-1 1-1,1-1 0,-1 0 0,0 1 0,0-1 1,0 1-1,0-1 0,0 1 0,0-1 0,0 1 1,0 0-1,0 0 0,-1-1 0,1 1 0,-1 0 1,1 0-1,-1 0 0,0 3 0,6 26 146,-1 1 0,-2 0-1,-2 57 1,-1-66-650</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="576.34">474 86 12950,'0'0'9671,"5"8"-8887,1 5-412,-1 1-1,0 0 1,0 0-1,-2 0 1,0 0-1,0 1 0,-1-1 1,-1 16-1,-1-45-391,1 0 0,0 0 1,1 0-1,1 0 0,0 0 0,1 0 0,0 1 0,1 0 0,1 0 0,1 0 0,-1 1 0,17-24 0,-21 35 15,-1 0 0,0 0 0,1 1 0,0-1 0,-1 0 0,1 1 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,1 0 0,-1 1 0,0-1 0,0 0 0,1 1 0,-1-1 0,0 1 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,1 1 0,-1-1 0,0 1 0,4 1 0,-3 0 5,1 0 0,-1 0 0,0 0-1,-1 1 1,1-1 0,0 1 0,-1 0-1,1 0 1,-1 0 0,0 0-1,0 0 1,0 1 0,0-1 0,-1 1-1,1-1 1,-1 1 0,1 4 0,0-1 8,0 1 0,0-1 0,-1 0 1,0 1-1,-1-1 0,1 1 0,-1-1 0,-1 1 1,1-1-1,-2 1 0,1-1 0,-5 15 0,17-46-1240,14-25-401,-23 47 1454,-1 0 1,1 0-1,0 0 0,-1 0 1,1 0-1,0 1 1,0-1-1,0 1 0,1-1 1,-1 1-1,0 0 1,0 0-1,1 0 0,-1 0 1,1 0-1,-1 1 1,1-1-1,-1 1 0,1-1 1,2 1-1,-4 0 143,-1 1 1,1-1-1,-1 1 1,1-1-1,-1 1 0,1-1 1,-1 1-1,0-1 0,1 1 1,-1-1-1,0 1 1,1 0-1,-1-1 0,0 1 1,0-1-1,1 1 0,-1 0 1,0-1-1,0 1 1,0 0-1,0-1 0,0 1 1,0 0-1,0-1 0,0 2 1,0 25-1940,-1-22 47,1 7-2471</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="576.32">474 86 12950,'0'0'9671,"5"8"-8887,1 5-412,-1 1-1,0 0 1,0 0-1,-2 0 1,0 0-1,0 1 0,-1-1 1,-1 16-1,-1-45-391,1 0 0,0 0 1,1 0-1,1 0 0,0 0 0,1 0 0,0 1 0,1 0 0,1 0 0,1 0 0,-1 1 0,17-24 0,-21 35 15,-1 0 0,0 0 0,1 1 0,0-1 0,-1 0 0,1 1 0,0-1 0,0 1 0,0 0 0,0-1 0,0 1 0,0 0 0,0 0 0,1 0 0,-1 1 0,0-1 0,0 0 0,1 1 0,-1-1 0,0 1 0,1 0 0,-1 0 0,1 0 0,-1 0 0,0 0 0,1 1 0,-1-1 0,0 1 0,4 1 0,-3 0 5,1 0 0,-1 0 0,0 0-1,-1 1 1,1-1 0,0 1 0,-1 0-1,1 0 1,-1 0 0,0 0-1,0 0 1,0 1 0,0-1 0,-1 1-1,1-1 1,-1 1 0,1 4 0,0-1 8,0 1 0,0-1 0,-1 0 1,0 1-1,-1-1 0,1 1 0,-1-1 0,-1 1 1,1-1-1,-2 1 0,1-1 0,-5 15 0,17-46-1240,14-25-401,-23 47 1454,-1 0 1,1 0-1,0 0 0,-1 0 1,1 0-1,0 1 1,0-1-1,0 1 0,1-1 1,-1 1-1,0 0 1,0 0-1,1 0 0,-1 0 1,1 0-1,-1 1 1,1-1-1,-1 1 0,1-1 1,2 1-1,-4 0 143,-1 1 1,1-1-1,-1 1 1,1-1-1,-1 1 0,1-1 1,-1 1-1,0-1 0,1 1 1,-1-1-1,0 1 1,1 0-1,-1-1 0,0 1 1,0-1-1,1 1 0,-1 0 1,0-1-1,0 1 1,0 0-1,0-1 0,0 1 1,0 0-1,0-1 0,0 2 1,0 25-1940,-1-22 47,1 7-2471</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -21140,7 +21230,7 @@
     </inkml:brush>
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">210 302 4018,'0'0'11416,"-5"-6"-10221,4 4-1101,-1 0 0,0 0-1,0 0 1,0 0 0,0 0 0,0 0 0,0 0 0,-1 1 0,1-1-1,0 1 1,-1 0 0,1 0 0,-1 0 0,0 0 0,1 0-1,-1 0 1,0 1 0,1-1 0,-1 1 0,0 0 0,0 0 0,0 0-1,1 0 1,-1 0 0,0 0 0,0 1 0,1 0 0,-1-1 0,0 1-1,1 0 1,-1 0 0,1 0 0,-5 3 0,0 0-27,-1 0-1,0 0 1,1 1 0,0 0 0,0 0 0,1 1-1,-1 0 1,1 0 0,0 1 0,1-1 0,0 1-1,0 0 1,0 1 0,1-1 0,0 1 0,0 0 0,1 0-1,0 0 1,1 1 0,-1-1 0,2 0 0,-2 13-1,3-20-64,1 0-1,-1 0 0,1 0 1,-1 0-1,1 0 0,0 0 0,-1 0 1,1 0-1,0 0 0,0-1 0,-1 1 1,1 0-1,0 0 0,0-1 0,0 1 1,0-1-1,0 1 0,0-1 1,0 1-1,0-1 0,0 0 0,1 1 1,-1-1-1,0 0 0,0 0 0,0 0 1,0 0-1,0 0 0,0 0 0,3 0 1,36-2 22,-32 0-106,-1 0-1,0 0 0,0-1 1,0 0-1,0 0 0,-1-1 0,1 0 1,-1 0-1,0 0 0,0-1 0,0 0 1,-1 0-1,1-1 0,-1 1 1,-1-1-1,1 0 0,-1 0 0,0-1 1,3-7-1,1 0-3,-2-1-1,1 1 1,-2-1 0,0 0 0,-1 0 0,-1-1-1,0 1 1,1-20 0,-3 8 166,1 16 133,-1 0 0,0 0 0,-1 0 1,-1-1-1,1 1 0,-2 0 0,0 0 0,0 0 1,-7-21-1,8 32 64,1 25 73,-2 84 828,5 123 5,-3-231-1260,0 1 0,0-1 1,0 1-1,1-1 0,-1 1 1,0 0-1,1-1 0,0 1 0,-1-1 1,1 0-1,0 1 0,-1-1 1,1 1-1,0-1 0,0 0 1,0 0-1,0 0 0,1 1 1,-1-1-1,0 0 0,0 0 0,1-1 1,-1 1-1,0 0 0,1 0 1,-1-1-1,1 1 0,1 0 1,4 0-1279,-1 0 1,1 0 0,-1-1 0,1 0 0,10-1 0,-12 1 151,21-3-5896</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="549.45">467 282 7796,'0'0'8966,"-12"-3"-7290,-42-10-580,51 12-1018,0 1 0,0 0-1,0 0 1,0 0 0,0 0-1,0 1 1,0-1 0,0 1 0,1 0-1,-1 0 1,0 0 0,0 0-1,1 0 1,-1 0 0,1 1-1,-1-1 1,1 1 0,0 0-1,-1 0 1,1 0 0,0 0 0,0 0-1,0 0 1,1 1 0,-1-1-1,0 1 1,1-1 0,0 1-1,-1-1 1,0 6 0,-1-2-27,0 1 0,1 0 0,0-1 0,0 1 0,1 0 0,0 1 0,0-1 0,1 0 0,-1 0 0,2 10 0,0-15-53,0 0 1,-1-1-1,1 1 0,0-1 1,0 1-1,0-1 1,0 1-1,0-1 1,0 0-1,1 1 1,-1-1-1,0 0 1,1 0-1,-1 0 1,1 0-1,-1 0 0,1 0 1,-1 0-1,1-1 1,0 1-1,-1 0 1,1-1-1,0 0 1,0 1-1,-1-1 1,1 0-1,0 0 0,0 0 1,-1 0-1,1 0 1,0 0-1,2-1 1,2 1-12,-1-1 1,1 0-1,0 0 1,-1 0 0,1-1-1,-1 0 1,1 0-1,8-5 1,-6 2-11,-1-1 0,1 0 0,-1-1 0,0 0 0,-1 0 0,1-1-1,-2 1 1,1-1 0,-1-1 0,0 1 0,-1-1 0,0 1 0,0-1 0,-1 0 0,4-17 0,-1-5 36,-2 0 1,-2-1 0,-1-45-1,-1 61-24,-4-29 97,4 42-28,-1 1-1,1-1 0,-1 1 1,0-1-1,1 1 0,-1 0 1,0-1-1,0 1 0,0 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,-1 0 0,-1-2 1,2 5-43,0-1 1,1 0 0,-1 1-1,0-1 1,1 1 0,-1-1-1,1 1 1,-1-1 0,0 1-1,1 0 1,-1-1 0,1 1-1,0-1 1,-1 1 0,1 0-1,0 0 1,-1-1 0,1 1-1,0 0 1,0 0 0,0-1 0,-1 1-1,1 0 1,0 0 0,0-1-1,0 1 1,0 0 0,1 1-1,-2 1 35,-9 46 121,3 0 1,2 1-1,1 67 0,4-112-159,0 0-1,0 1 1,1-1-1,-1 0 1,1 1-1,0-1 1,1 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,1 0 1,-1 0-1,1-1 1,0 0-1,1 1 1,6 6-1,-5-7-18,0 0-1,0-1 0,1 0 0,0 0 1,-1-1-1,1 1 0,0-1 0,0 0 1,0-1-1,0 1 0,1-1 0,-1-1 1,0 1-1,12-1 0,-6 0-78,1-1 0,0 0 0,-1-1-1,14-4 1,-22 5-154,0 0 1,0 0-1,0-1 0,0 0 1,-1 0-1,1 0 1,5-4-1,-8 5-99,0-1-1,0 1 1,1 0-1,-1 0 1,0-1 0,0 1-1,0-1 1,-1 1 0,1-1-1,0 1 1,0-1 0,-1 0-1,1 1 1,-1-1 0,1 0-1,-1 1 1,0-1-1,0-2 1,-2-5-5119,-10 4-4011</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="549.43">467 282 7796,'0'0'8966,"-12"-3"-7290,-42-10-580,51 12-1018,0 1 0,0 0-1,0 0 1,0 0 0,0 0-1,0 1 1,0-1 0,0 1 0,1 0-1,-1 0 1,0 0 0,0 0-1,1 0 1,-1 0 0,1 1-1,-1-1 1,1 1 0,0 0-1,-1 0 1,1 0 0,0 0 0,0 0-1,0 0 1,1 1 0,-1-1-1,0 1 1,1-1 0,0 1-1,-1-1 1,0 6 0,-1-2-27,0 1 0,1 0 0,0-1 0,0 1 0,1 0 0,0 1 0,0-1 0,1 0 0,-1 0 0,2 10 0,0-15-53,0 0 1,-1-1-1,1 1 0,0-1 1,0 1-1,0-1 1,0 1-1,0-1 1,0 0-1,1 1 1,-1-1-1,0 0 1,1 0-1,-1 0 1,1 0-1,-1 0 0,1 0 1,-1 0-1,1-1 1,0 1-1,-1 0 1,1-1-1,0 0 1,0 1-1,-1-1 1,1 0-1,0 0 0,0 0 1,-1 0-1,1 0 1,0 0-1,2-1 1,2 1-12,-1-1 1,1 0-1,0 0 1,-1 0 0,1-1-1,-1 0 1,1 0-1,8-5 1,-6 2-11,-1-1 0,1 0 0,-1-1 0,0 0 0,-1 0 0,1-1-1,-2 1 1,1-1 0,-1-1 0,0 1 0,-1-1 0,0 1 0,0-1 0,-1 0 0,4-17 0,-1-5 36,-2 0 1,-2-1 0,-1-45-1,-1 61-24,-4-29 97,4 42-28,-1 1-1,1-1 0,-1 1 1,0-1-1,1 1 0,-1 0 1,0-1-1,0 1 0,0 0 1,-1 0-1,1 0 0,-1 0 1,1 0-1,-1 0 0,-1-2 1,2 5-43,0-1 1,1 0 0,-1 1-1,0-1 1,1 1 0,-1-1-1,1 1 1,-1-1 0,0 1-1,1 0 1,-1-1 0,1 1-1,0-1 1,-1 1 0,1 0-1,0 0 1,-1-1 0,1 1-1,0 0 1,0 0 0,0-1 0,-1 1-1,1 0 1,0 0 0,0-1-1,0 1 1,0 0 0,1 1-1,-2 1 35,-9 46 121,3 0 1,2 1-1,1 67 0,4-112-159,0 0-1,0 1 1,1-1-1,-1 0 1,1 1-1,0-1 1,1 0-1,-1 0 1,1 0-1,0 0 1,0 0-1,1 0 1,-1 0-1,1-1 1,0 0-1,1 1 1,6 6-1,-5-7-18,0 0-1,0-1 0,1 0 0,0 0 1,-1-1-1,1 1 0,0-1 0,0 0 1,0-1-1,0 1 0,1-1 0,-1-1 1,0 1-1,12-1 0,-6 0-78,1-1 0,0 0 0,-1-1-1,14-4 1,-22 5-154,0 0 1,0 0-1,0-1 0,0 0 1,-1 0-1,1 0 1,5-4-1,-8 5-99,0-1-1,0 1 1,1 0-1,-1 0 1,0-1 0,0 1-1,0-1 1,-1 1 0,1-1-1,0 1 1,0-1 0,-1 0-1,1 1 1,-1-1 0,1 0-1,-1 1 1,0-1-1,0-2 1,-2-5-5119,-10 4-4011</inkml:trace>
 </inkml:ink>
 </file>
 
@@ -21176,7 +21266,7 @@
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="435.47">164 162 9108,'0'0'5074,"23"24"-4801,-10-12-161,-3-5-112,3 1-176,1-6-785,-1-2-1152,0 0-1296</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="646.6">376 49 3298,'0'0'11429,"0"19"-11093,0 0 496,0 4-239,0 0-193,0-4-208,0 2-128,0-4-32,0-4-32,0-2-144,0-3-1233,0-4-1072</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="850.07">286 150 9973,'0'0'4866,"27"-2"-4690,-4 0-112,4-1-64,-4 3-592,0-2-1057,-3 0-1793,-10 2-2256</inkml:trace>
-  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1180.19">462 129 7363,'0'0'6747,"5"5"-6288,1 2-366,-1 0 0,0 1-1,0-1 1,0 1-1,-1 0 1,5 12-1,-8-18-62,0 1-1,0-1 0,0 1 0,0-1 1,0 1-1,-1 0 0,1-1 1,-1 1-1,0 0 0,0 0 0,0-1 1,0 1-1,0 0 0,0-1 0,-1 1 1,1 0-1,-1-1 0,0 1 0,0 0 1,0-1-1,0 1 0,0-1 1,-1 0-1,1 1 0,-1-1 0,1 0 1,-1 0-1,0 0 0,-2 2 0,3-3 16,0 0-1,1-1 1,-1 1-1,0-1 1,0 1-1,0-1 1,0 1-1,1-1 1,-1 0-1,0 1 1,0-1-1,0 0 1,0 0-1,0 0 1,0 0-1,0 1 1,0-1-1,0 0 1,0-1-1,0 1 1,0 0-1,0 0 1,0 0-1,0-1 1,0 1-1,1 0 1,-1-1-1,0 1 1,0-1-1,0 1 1,0-1-1,1 1 1,-1-1-1,0 0 1,0 1-1,1-1 1,-1 0-1,1 1 1,-1-1-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 1 1,-1-1-1,1 0 1,0 0-1,0 0 1,0 0-1,-1 0 1,1 0-1,0-1 1,0-1-153,-1 0-1,0 1 1,1-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,1 1-1,-1-1 1,1 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,3-3 0,4 0-772,0 1 1,0 0-1,1 0 1,0 0-1,0 1 1,11-3-1,-9 3-898,15-6-2877</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1180.17">462 129 7363,'0'0'6747,"5"5"-6288,1 2-366,-1 0 0,0 1-1,0-1 1,0 1-1,-1 0 1,5 12-1,-8-18-62,0 1-1,0-1 0,0 1 0,0-1 1,0 1-1,-1 0 0,1-1 1,-1 1-1,0 0 0,0 0 0,0-1 1,0 1-1,0 0 0,0-1 0,-1 1 1,1 0-1,-1-1 0,0 1 0,0 0 1,0-1-1,0 1 0,0-1 1,-1 0-1,1 1 0,-1-1 0,1 0 1,-1 0-1,0 0 0,-2 2 0,3-3 16,0 0-1,1-1 1,-1 1-1,0-1 1,0 1-1,0-1 1,0 1-1,1-1 1,-1 0-1,0 1 1,0-1-1,0 0 1,0 0-1,0 0 1,0 0-1,0 1 1,0-1-1,0 0 1,0-1-1,0 1 1,0 0-1,0 0 1,0 0-1,0-1 1,0 1-1,1 0 1,-1-1-1,0 1 1,0-1-1,0 1 1,0-1-1,1 1 1,-1-1-1,0 0 1,0 1-1,1-1 1,-1 0-1,1 1 1,-1-1-1,1 0 1,-1 0-1,1 0 1,-1 0-1,1 1 1,-1-1-1,1 0 1,0 0-1,0 0 1,0 0-1,-1 0 1,1 0-1,0-1 1,0-1-153,-1 0-1,0 1 1,1-1 0,0 1 0,0-1 0,0 0 0,0 1 0,0-1 0,0 0 0,1 1-1,-1-1 1,1 1 0,0-1 0,0 1 0,0-1 0,0 1 0,0-1 0,3-3 0,4 0-772,0 1 1,0 0-1,1 0 1,0 0-1,0 1 1,11-3-1,-9 3-898,15-6-2877</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1908.43">661 122 6531,'0'0'7038,"-12"4"-6200,-36 15-171,45-17-602,1 0 1,-1 0 0,0 1-1,1-1 1,0 1-1,-1-1 1,1 1 0,0 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,1 0 0,0 0-1,0 1 1,0-1 0,0 0-1,0 1 1,1-1 0,0 1-1,-1-1 1,1 1 0,0-1-1,1 1 1,-1-1-1,1 0 1,1 6 0,2-8-177,0 0 0,0-1 0,0 1 0,1-1 0,-1 0 0,0 0 0,1 0 0,-1 0 0,0-1 0,0 0 0,8-2 0,-9 1 61,0 1 0,-1 0 0,1-1-1,-1 0 1,1 0 0,-1 0-1,0 0 1,1 0 0,-1 0-1,0 0 1,-1-1 0,1 1-1,0-1 1,-1 1 0,1-1 0,-1 0-1,0 1 1,0-1 0,0 0-1,1-3 1,1 4 52,0 1 0,1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1 1 0,0 0 0,-1-1 0,1 1 0,4 1 0,4-1-186,10-8-579,-19 6 667,0 1 0,1 0 0,-1-1 0,0 2 0,1-1 0,-1 0 0,1 0 0,3 1-1,-6 0 274,-14 13 610,9-8-663,0-1 1,1 1 0,0 0 0,0 0 0,0 0 0,1 0 0,0 1-1,0-1 1,0 1 0,0-1 0,1 1 0,0 0 0,0-1 0,0 7-1,2-11-128,-1-1-1,1 1 0,-1-1 0,1 1 0,-1-1 0,1 0 0,-1 1 0,1-1 0,-1 0 0,1 1 0,-1-1 0,1 0 0,-1 0 0,1 1 0,0-1 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0 0 1,-1 0-1,1 0 0,0 0 0,-1 0 0,1 0 0,-1 0 0,1 0 0,0-1 0,-1 1 0,1 0 0,0-1 0,25-8-466,-19 4 248,1-1 0,-1 0 0,-1 0 0,1-1 0,-1 0 0,0 0 0,0-1 0,-1 1-1,0-1 1,-1 0 0,1-1 0,-1 1 0,2-10 0,-1 0 512,0 0 0,-2-1 0,0 1-1,-1-1 1,-1-30 1355,-4 73-627,-3 33-854,2 88 1,4-121-294,4 4-1101,8-16-2775,-5-10-1196</inkml:trace>
   <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2127.09">830 148 9716,'0'0'5603,"57"-21"-5219,-27 10-160,6-1-112,4 1-112,-4-4-16,-2 2-144,-8 5-544,-13 0-1585,-6 5-2017</inkml:trace>
 </inkml:ink>
@@ -21971,7 +22061,7 @@
       <c r="D46" s="9" t="s">
         <v>218</v>
       </c>
-      <c r="P46" s="16" t="str" cm="1">
+      <c r="P46" s="13" t="str" cm="1">
         <f t="array" ref="P46:P52">_xlfn.UNIQUE(data[Department])</f>
         <v>Customer Support</v>
       </c>
@@ -22051,7 +22141,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA79FBAC-710E-4D08-8E7D-C38A34576560}">
   <dimension ref="B2:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -22192,10 +22282,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13B71C03-7B12-4842-AAB8-D655859B4B5C}">
-  <dimension ref="B2:J37"/>
+  <dimension ref="B2:N37"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:J4"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -22204,7 +22294,10 @@
     <col min="2" max="2" width="27.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10">
+    <row r="2" spans="2:14">
+      <c r="B2" t="s">
+        <v>903</v>
+      </c>
       <c r="C2" t="s">
         <v>885</v>
       </c>
@@ -22214,202 +22307,345 @@
       <c r="E2" t="s">
         <v>887</v>
       </c>
-      <c r="G2" t="s">
+      <c r="K2" t="s">
         <v>874</v>
       </c>
-      <c r="H2" t="s">
+      <c r="L2" t="s">
         <v>877</v>
       </c>
-      <c r="I2" t="s">
+      <c r="M2" t="s">
         <v>880</v>
       </c>
-      <c r="J2" t="s">
+      <c r="N2" t="s">
         <v>899</v>
       </c>
     </row>
-    <row r="3" spans="2:10">
+    <row r="3" spans="2:14">
       <c r="B3" s="10" t="s">
         <v>345</v>
       </c>
-      <c r="G3" t="s">
+      <c r="C3" t="s">
+        <v>883</v>
+      </c>
+      <c r="D3" t="s">
+        <v>908</v>
+      </c>
+      <c r="E3" t="s">
+        <v>884</v>
+      </c>
+      <c r="G3" t="str">
+        <f>PROPER(LEFT(B3,FIND(".",B3)-1))</f>
+        <v>Siraj</v>
+      </c>
+      <c r="K3" t="s">
         <v>875</v>
       </c>
-      <c r="H3" t="s">
+      <c r="L3" t="s">
         <v>878</v>
       </c>
-      <c r="I3" t="s">
+      <c r="M3" t="s">
         <v>881</v>
       </c>
-      <c r="J3" t="s">
+      <c r="N3" t="s">
         <v>900</v>
       </c>
     </row>
-    <row r="4" spans="2:10">
+    <row r="4" spans="2:14">
       <c r="B4" s="10" t="s">
         <v>346</v>
       </c>
-      <c r="G4" t="s">
+      <c r="C4" t="s">
+        <v>928</v>
+      </c>
+      <c r="D4" t="s">
+        <v>909</v>
+      </c>
+      <c r="E4" t="s">
+        <v>919</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" ref="G4:G13" si="0">PROPER(LEFT(B4,FIND(".",B4)-1))</f>
+        <v>Vishu</v>
+      </c>
+      <c r="K4" t="s">
         <v>876</v>
       </c>
-      <c r="H4" t="s">
+      <c r="L4" t="s">
         <v>879</v>
       </c>
-      <c r="I4" t="s">
+      <c r="M4" t="s">
         <v>882</v>
       </c>
-      <c r="J4" t="s">
+      <c r="N4" t="s">
         <v>901</v>
       </c>
     </row>
-    <row r="5" spans="2:10">
+    <row r="5" spans="2:14">
       <c r="B5" s="10" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="6" spans="2:10">
+      <c r="C5" t="s">
+        <v>904</v>
+      </c>
+      <c r="D5" t="s">
+        <v>910</v>
+      </c>
+      <c r="E5" t="s">
+        <v>920</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="0"/>
+        <v>Srinath</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14">
       <c r="B6" s="10" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="7" spans="2:10">
+      <c r="C6" t="s">
+        <v>905</v>
+      </c>
+      <c r="D6" t="s">
+        <v>911</v>
+      </c>
+      <c r="E6" t="s">
+        <v>921</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="0"/>
+        <v>Bhatia</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14">
       <c r="B7" s="10" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="8" spans="2:10">
+      <c r="C7" t="s">
+        <v>906</v>
+      </c>
+      <c r="D7" t="s">
+        <v>912</v>
+      </c>
+      <c r="E7" t="s">
+        <v>922</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="0"/>
+        <v>Abdul</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14">
       <c r="B8" s="10" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="9" spans="2:10">
+      <c r="C8" t="s">
+        <v>929</v>
+      </c>
+      <c r="D8" t="s">
+        <v>913</v>
+      </c>
+      <c r="E8" t="s">
+        <v>919</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="0"/>
+        <v>Arpit</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14">
       <c r="B9" s="10" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="10" spans="2:10">
+      <c r="C9" t="s">
+        <v>930</v>
+      </c>
+      <c r="D9" t="s">
+        <v>914</v>
+      </c>
+      <c r="E9" t="s">
+        <v>923</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="0"/>
+        <v>Tanya</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14">
       <c r="B10" s="10" t="s">
         <v>352</v>
       </c>
-    </row>
-    <row r="11" spans="2:10">
+      <c r="C10" t="s">
+        <v>917</v>
+      </c>
+      <c r="D10" t="s">
+        <v>915</v>
+      </c>
+      <c r="E10" t="s">
+        <v>924</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="0"/>
+        <v>Kumar</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14">
       <c r="B11" s="10" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="12" spans="2:10">
+      <c r="C11" t="s">
+        <v>907</v>
+      </c>
+      <c r="D11" t="s">
+        <v>916</v>
+      </c>
+      <c r="E11" t="s">
+        <v>925</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="0"/>
+        <v>Priyanshu</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14">
       <c r="B12" s="10" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="13" spans="2:10">
+      <c r="C12" t="s">
+        <v>931</v>
+      </c>
+      <c r="D12" t="s">
+        <v>917</v>
+      </c>
+      <c r="E12" t="s">
+        <v>926</v>
+      </c>
+      <c r="G12" t="str">
+        <f t="shared" si="0"/>
+        <v>Babblu</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14">
       <c r="B13" s="10" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="14" spans="2:10">
+      <c r="C13" t="s">
+        <v>932</v>
+      </c>
+      <c r="D13" t="s">
+        <v>918</v>
+      </c>
+      <c r="E13" t="s">
+        <v>927</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" si="0"/>
+        <v>Arzoo</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14">
       <c r="B14" s="10"/>
     </row>
-    <row r="23" spans="3:9">
+    <row r="23" spans="3:13">
       <c r="C23" t="s">
         <v>884</v>
       </c>
     </row>
-    <row r="24" spans="3:9">
+    <row r="24" spans="3:13">
       <c r="C24" t="s">
         <v>874</v>
       </c>
     </row>
-    <row r="25" spans="3:9">
+    <row r="25" spans="3:13">
       <c r="D25" t="str">
         <f>LEFT(C23,3)</f>
         <v>Acc</v>
       </c>
     </row>
-    <row r="26" spans="3:9">
+    <row r="26" spans="3:13">
       <c r="D26" t="str">
         <f>LEFT(C23,100)</f>
         <v>Acciojob</v>
       </c>
     </row>
-    <row r="27" spans="3:9">
+    <row r="27" spans="3:13">
       <c r="D27" t="str">
         <f>LEFT(C23)</f>
         <v>A</v>
       </c>
     </row>
-    <row r="28" spans="3:9">
+    <row r="28" spans="3:13">
       <c r="D28" t="e">
         <f>LEFT(C23,-3)</f>
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="29" spans="3:9">
+    <row r="29" spans="3:13">
       <c r="C29" t="s">
         <v>875</v>
       </c>
     </row>
-    <row r="30" spans="3:9">
+    <row r="30" spans="3:13">
       <c r="D30" t="str">
         <f>RIGHT(C23,5)</f>
         <v>iojob</v>
       </c>
     </row>
-    <row r="31" spans="3:9">
+    <row r="31" spans="3:13">
       <c r="D31" t="str">
         <f>RIGHT(C23,100)</f>
         <v>Acciojob</v>
       </c>
     </row>
-    <row r="32" spans="3:9">
+    <row r="32" spans="3:13">
       <c r="D32" t="str">
         <f>RIGHT(C23)</f>
         <v>b</v>
       </c>
-      <c r="G32" t="s">
+      <c r="K32" t="s">
         <v>896</v>
       </c>
-      <c r="H32" t="str">
-        <f>LEFT(G32,4)</f>
+      <c r="L32" t="str">
+        <f>LEFT(K32,4)</f>
         <v>5000</v>
       </c>
-      <c r="I32">
-        <f>VALUE(H32)</f>
+      <c r="M32">
+        <f>VALUE(L32)</f>
         <v>5000</v>
       </c>
     </row>
-    <row r="33" spans="3:8">
+    <row r="33" spans="3:12">
       <c r="C33" t="s">
         <v>876</v>
       </c>
-      <c r="G33" t="s">
+      <c r="K33" t="s">
         <v>897</v>
       </c>
     </row>
-    <row r="34" spans="3:8">
+    <row r="34" spans="3:12">
       <c r="D34" t="str">
         <f>MID(C23,4,3)</f>
         <v>ioj</v>
       </c>
-      <c r="H34" t="s">
+      <c r="L34" t="s">
         <v>874</v>
       </c>
     </row>
-    <row r="35" spans="3:8">
+    <row r="35" spans="3:12">
       <c r="D35" t="e">
         <f>MID(C23,4,-3)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="H35" t="s">
+      <c r="L35" t="s">
         <v>880</v>
       </c>
     </row>
-    <row r="36" spans="3:8">
-      <c r="H36" t="s">
+    <row r="36" spans="3:12">
+      <c r="L36" t="s">
         <v>874</v>
       </c>
     </row>
-    <row r="37" spans="3:8">
-      <c r="H37" t="s">
+    <row r="37" spans="3:12">
+      <c r="L37" t="s">
         <v>898</v>
       </c>
     </row>
@@ -53423,88 +53659,88 @@
       <c r="B4" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="18" t="s">
         <v>160</v>
       </c>
-      <c r="E4" s="14"/>
-      <c r="F4" s="15"/>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
     </row>
     <row r="5" spans="1:12">
-      <c r="D5" s="12"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
     </row>
     <row r="6" spans="1:12" ht="14.25" customHeight="1">
       <c r="B6" t="s">
         <v>144</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="19" t="s">
         <v>161</v>
       </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
     </row>
     <row r="7" spans="1:12">
       <c r="C7" t="s">
         <v>145</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
     </row>
     <row r="8" spans="1:12" ht="14.25" customHeight="1">
       <c r="C8" t="s">
         <v>146</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
     </row>
     <row r="9" spans="1:12">
       <c r="C9" t="s">
         <v>147</v>
       </c>
-      <c r="D9" s="13"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
     </row>
     <row r="10" spans="1:12" ht="14.25" customHeight="1">
       <c r="C10" t="s">
@@ -53615,60 +53851,60 @@
       </c>
     </row>
     <row r="5" spans="2:9">
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
     </row>
     <row r="6" spans="2:9">
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
     </row>
     <row r="7" spans="2:9">
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
     </row>
     <row r="8" spans="2:9">
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
     </row>
     <row r="9" spans="2:9">
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
     </row>
     <row r="10" spans="2:9">
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
     </row>
     <row r="13" spans="2:9" s="4" customFormat="1">
       <c r="B13" s="4" t="s">
@@ -53798,7 +54034,7 @@
       <c r="G54" t="s">
         <v>895</v>
       </c>
-      <c r="H54" s="16">
+      <c r="H54" s="13">
         <v>16</v>
       </c>
     </row>
@@ -53812,7 +54048,7 @@
       <c r="G55" t="s">
         <v>172</v>
       </c>
-      <c r="H55" s="17">
+      <c r="H55" s="14">
         <v>17</v>
       </c>
     </row>
@@ -53820,7 +54056,7 @@
       <c r="B56">
         <v>4</v>
       </c>
-      <c r="F56" s="18"/>
+      <c r="F56" s="15"/>
       <c r="G56" t="s">
         <v>173</v>
       </c>
@@ -53841,7 +54077,7 @@
       <c r="G59" t="s">
         <v>895</v>
       </c>
-      <c r="H59" s="16">
+      <c r="H59" s="13">
         <v>2.5</v>
       </c>
     </row>
@@ -53849,59 +54085,59 @@
       <c r="E62" t="s">
         <v>176</v>
       </c>
-      <c r="H62" s="16" t="s">
+      <c r="H62" s="13" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="64" spans="2:18">
-      <c r="D64" s="19" t="s">
+      <c r="D64" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="E64" s="19" t="s">
+      <c r="E64" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="F64" s="19" t="s">
+      <c r="F64" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="G64" s="19" t="s">
+      <c r="G64" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="H64" s="19" t="s">
+      <c r="H64" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="I64" s="19" t="s">
+      <c r="I64" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="J64" s="19" t="s">
+      <c r="J64" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="K64" s="19" t="s">
+      <c r="K64" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="L64" s="19" t="s">
+      <c r="L64" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="M64" s="19" t="s">
+      <c r="M64" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="N64" s="19" t="s">
+      <c r="N64" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="O64" s="19" t="s">
+      <c r="O64" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="P64" s="19" t="s">
+      <c r="P64" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="Q64" s="20" t="s">
+      <c r="Q64" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="R64" s="20" t="s">
+      <c r="R64" s="17" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="65" spans="3:16">
-      <c r="C65" s="16">
+      <c r="C65" s="13">
         <v>21</v>
       </c>
       <c r="D65" t="str" cm="1">

</xml_diff>